<commit_message>
Merged PR 7352: Fixed export template for hiatus days
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\plan-excel-generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6FC5578A-B41F-4914-BB47-089FFB5BC720}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{116C7BE8-72CF-4866-A15D-7825A8F2A260}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="468" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="465" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="91">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -669,6 +669,9 @@
   <si>
     <t>Odd</t>
   </si>
+  <si>
+    <t>Hiatus Days</t>
+  </si>
 </sst>
 </file>
 
@@ -681,7 +684,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -769,8 +772,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFB0C0CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,8 +807,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECF0F3"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F8F8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1088,12 +1112,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB0C0CC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB0C0CC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB0C0CC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB0C0CC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1275,9 +1314,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -1485,6 +1521,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
@@ -1520,48 +1565,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -1692,8 +1711,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF5F8F8"/>
       <color rgb="FF3D5261"/>
-      <color rgb="FFF5F8F8"/>
       <color rgb="FFECF0F3"/>
       <color rgb="FFE5EAED"/>
       <color rgb="FFB0C0CC"/>
@@ -2271,26 +2290,26 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.3984375" style="99" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="6.375" style="98" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3" style="3" customWidth="1"/>
-    <col min="3" max="4" width="24.8984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.8984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.09765625" style="3" customWidth="1"/>
-    <col min="7" max="12" width="24.8984375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="2.3984375" style="3" customWidth="1"/>
-    <col min="14" max="20" width="10.8984375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="24.875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
+    <col min="7" max="12" width="24.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="2.375" style="3" customWidth="1"/>
+    <col min="14" max="20" width="10.875" style="3" customWidth="1"/>
     <col min="21" max="21" width="3" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="10.59765625" style="3"/>
+    <col min="22" max="16384" width="10.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:20" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="str">
         <f>SUBSTITUTE(Proposal!F2, "Broadcast Proposal", "Broadcast Contract")</f>
         <v xml:space="preserve">Broadcast Contract </v>
@@ -2300,8 +2319,8 @@
         <v xml:space="preserve">Created </v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2330,46 +2349,46 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="76">
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="75">
         <f>Proposal!C5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="75">
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="131">
+      <c r="E5" s="133">
         <f>Proposal!H5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="131"/>
-      <c r="G5" s="76">
+      <c r="F5" s="133"/>
+      <c r="G5" s="75">
         <f>Proposal!J5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="76">
+      <c r="H5" s="75">
         <f>Proposal!L5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="76">
+      <c r="I5" s="75">
         <f>Proposal!N5</f>
         <v>0</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="75">
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="76">
+      <c r="K5" s="75">
         <f>Proposal!Q5</f>
         <v>0</v>
       </c>
-      <c r="L5" s="76">
+      <c r="L5" s="75">
         <f>Proposal!T5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
@@ -2384,7 +2403,7 @@
       <c r="S6" s="59"/>
       <c r="T6" s="59"/>
     </row>
-    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="52"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -2400,35 +2419,35 @@
       <c r="S7" s="59"/>
       <c r="T7" s="59"/>
     </row>
-    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99" t="s">
+    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="87" t="s">
+      <c r="D8" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="87" t="s">
+      <c r="E8" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="87" t="s">
+      <c r="F8" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="87" t="s">
+      <c r="G8" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="87" t="s">
+      <c r="H8" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="92" t="s">
+      <c r="J8" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="88" t="s">
+      <c r="K8" s="87" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="59"/>
@@ -2440,293 +2459,293 @@
       <c r="S8" s="59"/>
       <c r="T8" s="59"/>
     </row>
-    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99" t="s">
+    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="95"/>
-    </row>
-    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="94"/>
+    </row>
+    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="38"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="90" t="s">
+      <c r="D10" s="90"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="96" t="s">
+      <c r="G10" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="89"/>
-      <c r="I10" s="90" t="s">
+      <c r="H10" s="88"/>
+      <c r="I10" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="94"/>
-      <c r="K10" s="98"/>
-    </row>
-    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="93"/>
+      <c r="K10" s="97"/>
+    </row>
+    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
         <v>63</v>
       </c>
       <c r="I12" s="59"/>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="100" t="s">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101" t="s">
+      <c r="E13" s="100"/>
+      <c r="F13" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101" t="s">
+      <c r="G13" s="100"/>
+      <c r="H13" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="102"/>
-    </row>
-    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="103"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="106"/>
-    </row>
-    <row r="15" spans="1:20" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="110"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-    </row>
-    <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="113" t="s">
+      <c r="I13" s="101"/>
+    </row>
+    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="102"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="105"/>
+    </row>
+    <row r="15" spans="1:20" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="109"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107"/>
+    </row>
+    <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="114" t="s">
+      <c r="D16" s="108"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="109"/>
-      <c r="I16" s="115"/>
-    </row>
-    <row r="17" spans="3:18" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="110"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-    </row>
-    <row r="18" spans="3:18" s="99" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="108"/>
+      <c r="I16" s="114"/>
+    </row>
+    <row r="17" spans="3:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="109"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+    </row>
+    <row r="18" spans="3:18" s="98" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="133">
+      <c r="D18" s="135">
         <f>Proposal!F17</f>
         <v>0</v>
       </c>
-      <c r="E18" s="133"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="133"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="133"/>
-      <c r="J18" s="133"/>
-      <c r="K18" s="133"/>
-      <c r="L18" s="128"/>
-      <c r="M18" s="128"/>
-      <c r="N18" s="128"/>
-      <c r="O18" s="128"/>
-      <c r="P18" s="128"/>
-      <c r="Q18" s="128"/>
-      <c r="R18" s="128"/>
-    </row>
-    <row r="19" spans="3:18" s="99" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="135"/>
+      <c r="K18" s="135"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="127"/>
+      <c r="O18" s="127"/>
+      <c r="P18" s="127"/>
+      <c r="Q18" s="127"/>
+      <c r="R18" s="127"/>
+    </row>
+    <row r="19" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
-      <c r="G19" s="129"/>
-      <c r="H19" s="129"/>
-      <c r="I19" s="129"/>
-      <c r="J19" s="129"/>
-      <c r="K19" s="129"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="76"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="76"/>
-    </row>
-    <row r="20" spans="3:18" s="117" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="128"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="128"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="75"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75"/>
+    </row>
+    <row r="20" spans="3:18" s="116" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="133">
+      <c r="D20" s="135">
         <f>Proposal!F19</f>
         <v>0</v>
       </c>
-      <c r="E20" s="133"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
-      <c r="K20" s="133"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="128"/>
-      <c r="N20" s="128"/>
-      <c r="O20" s="128"/>
-      <c r="P20" s="128"/>
-      <c r="Q20" s="128"/>
-      <c r="R20" s="128"/>
-    </row>
-    <row r="21" spans="3:18" s="99" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="135"/>
+      <c r="J20" s="135"/>
+      <c r="K20" s="135"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127"/>
+      <c r="N20" s="127"/>
+      <c r="O20" s="127"/>
+      <c r="P20" s="127"/>
+      <c r="Q20" s="127"/>
+      <c r="R20" s="127"/>
+    </row>
+    <row r="21" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="D21" s="130"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="130"/>
-      <c r="I21" s="130"/>
-      <c r="J21" s="130"/>
-      <c r="K21" s="130"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="118"/>
-    </row>
-    <row r="22" spans="3:18" s="99" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
+      <c r="G21" s="129"/>
+      <c r="H21" s="129"/>
+      <c r="I21" s="129"/>
+      <c r="J21" s="129"/>
+      <c r="K21" s="129"/>
+      <c r="L21" s="117"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="117"/>
+      <c r="O21" s="117"/>
+      <c r="P21" s="117"/>
+      <c r="Q21" s="117"/>
+      <c r="R21" s="117"/>
+    </row>
+    <row r="22" spans="3:18" s="98" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="133"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="128"/>
-      <c r="M22" s="128"/>
-      <c r="N22" s="128"/>
-      <c r="O22" s="128"/>
-      <c r="P22" s="128"/>
-      <c r="Q22" s="128"/>
-      <c r="R22" s="128"/>
-    </row>
-    <row r="23" spans="3:18" s="99" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="135"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="135"/>
+      <c r="J22" s="135"/>
+      <c r="K22" s="135"/>
+      <c r="L22" s="127"/>
+      <c r="M22" s="127"/>
+      <c r="N22" s="127"/>
+      <c r="O22" s="127"/>
+      <c r="P22" s="127"/>
+      <c r="Q22" s="127"/>
+      <c r="R22" s="127"/>
+    </row>
+    <row r="23" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="D23" s="130"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="130"/>
-      <c r="I23" s="130"/>
-      <c r="J23" s="130"/>
-      <c r="K23" s="130"/>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="118"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="118"/>
-    </row>
-    <row r="24" spans="3:18" s="117" customFormat="1" ht="48.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
+      <c r="K23" s="129"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="117"/>
+      <c r="O23" s="117"/>
+      <c r="P23" s="117"/>
+      <c r="Q23" s="117"/>
+      <c r="R23" s="117"/>
+    </row>
+    <row r="24" spans="3:18" s="116" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="133">
+      <c r="D24" s="135">
         <f>Proposal!F23</f>
         <v>0</v>
       </c>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="133"/>
-      <c r="I24" s="133"/>
-      <c r="J24" s="133"/>
-      <c r="K24" s="133"/>
-      <c r="L24" s="128"/>
-      <c r="M24" s="128"/>
-      <c r="N24" s="128"/>
-      <c r="O24" s="128"/>
-      <c r="P24" s="128"/>
-      <c r="Q24" s="128"/>
-      <c r="R24" s="128"/>
-    </row>
-    <row r="25" spans="3:18" s="99" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="135"/>
+      <c r="K24" s="135"/>
+      <c r="L24" s="127"/>
+      <c r="M24" s="127"/>
+      <c r="N24" s="127"/>
+      <c r="O24" s="127"/>
+      <c r="P24" s="127"/>
+      <c r="Q24" s="127"/>
+      <c r="R24" s="127"/>
+    </row>
+    <row r="25" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="130"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="130"/>
-      <c r="G25" s="130"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="130"/>
-      <c r="J25" s="130"/>
-      <c r="K25" s="130"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="118"/>
-    </row>
-    <row r="26" spans="3:18" s="99" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="129"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="129"/>
+      <c r="K25" s="129"/>
+      <c r="L25" s="117"/>
+      <c r="M25" s="117"/>
+      <c r="N25" s="117"/>
+      <c r="O25" s="117"/>
+      <c r="P25" s="117"/>
+      <c r="Q25" s="117"/>
+      <c r="R25" s="117"/>
+    </row>
+    <row r="26" spans="3:18" s="98" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="133">
+      <c r="D26" s="135">
         <f>Proposal!F25</f>
         <v>0</v>
       </c>
-      <c r="E26" s="133"/>
-      <c r="F26" s="133"/>
-      <c r="G26" s="133"/>
-      <c r="H26" s="133"/>
-      <c r="I26" s="133"/>
-      <c r="J26" s="133"/>
-      <c r="K26" s="133"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="77"/>
-    </row>
-    <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="132"/>
-      <c r="H27" s="132"/>
-      <c r="I27" s="132"/>
-      <c r="J27" s="132"/>
-      <c r="K27" s="132"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="135"/>
+      <c r="G26" s="135"/>
+      <c r="H26" s="135"/>
+      <c r="I26" s="135"/>
+      <c r="J26" s="135"/>
+      <c r="K26" s="135"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
+      <c r="P26" s="76"/>
+      <c r="Q26" s="76"/>
+      <c r="R26" s="76"/>
+    </row>
+    <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="134"/>
+      <c r="J27" s="134"/>
+      <c r="K27" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2739,27 +2758,27 @@
     <mergeCell ref="D24:K24"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:K1048576">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>$A20="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>$A22="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>$A24="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$A26="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2774,29 +2793,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.09765625" style="3" customWidth="1"/>
-    <col min="3" max="5" width="12.09765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.09765625" style="7" customWidth="1"/>
-    <col min="7" max="9" width="12.09765625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.09765625" style="7" customWidth="1"/>
-    <col min="11" max="13" width="12.09765625" style="3" customWidth="1"/>
-    <col min="14" max="15" width="12.09765625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="11.8984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.125" style="3" customWidth="1"/>
+    <col min="3" max="5" width="12.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="7" customWidth="1"/>
+    <col min="7" max="9" width="12.125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.125" style="7" customWidth="1"/>
+    <col min="11" max="13" width="12.125" style="3" customWidth="1"/>
+    <col min="14" max="15" width="12.125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="11.875" style="3" customWidth="1"/>
     <col min="17" max="17" width="3" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="10.59765625" style="3"/>
+    <col min="18" max="16384" width="10.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="str">
         <f>SUBSTITUTE(Proposal!F2, "Broadcast Proposal", "Flow Chart")</f>
@@ -2809,8 +2828,8 @@
         <v xml:space="preserve">Created </v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2821,56 +2840,56 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="76">
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75">
         <f>Proposal!J5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="75">
         <f>Proposal!N5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="131">
+      <c r="D5" s="133">
         <f>Proposal!F19</f>
         <v>0</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="131"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="131"/>
-    </row>
-    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="133"/>
+    </row>
+    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="59"/>
     </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="59"/>
       <c r="B7" s="52"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="135"/>
-      <c r="I7" s="135"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="134"/>
-      <c r="L7" s="135"/>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
-      <c r="O7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="137"/>
+      <c r="I7" s="137"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="136"/>
+      <c r="L7" s="137"/>
+      <c r="M7" s="137"/>
+      <c r="N7" s="137"/>
+      <c r="O7" s="138"/>
       <c r="P7" s="29"/>
     </row>
-    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59"/>
-      <c r="B8" s="75"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
@@ -2884,113 +2903,132 @@
       <c r="M8" s="55"/>
       <c r="N8" s="55"/>
       <c r="O8" s="55"/>
-      <c r="P8" s="68" t="s">
+      <c r="P8" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="69" t="s">
+      <c r="C9" s="62"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="68" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
       <c r="F10" s="58"/>
-      <c r="G10" s="67"/>
+      <c r="G10" s="66"/>
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
       <c r="J10" s="58"/>
-      <c r="K10" s="67"/>
+      <c r="K10" s="66"/>
       <c r="L10" s="36"/>
       <c r="M10" s="36"/>
       <c r="N10" s="36"/>
       <c r="O10" s="58"/>
       <c r="P10" s="58"/>
     </row>
-    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="66"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
       <c r="F11" s="57"/>
-      <c r="G11" s="66"/>
+      <c r="G11" s="65"/>
       <c r="H11" s="35"/>
       <c r="I11" s="35"/>
       <c r="J11" s="57"/>
-      <c r="K11" s="66"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
       <c r="N11" s="35"/>
       <c r="O11" s="57"/>
       <c r="P11" s="57"/>
     </row>
-    <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="72"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="72"/>
       <c r="L12" s="37"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-    </row>
-    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="61" t="s">
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+    </row>
+    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-    </row>
-    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P15" s="59"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="71"/>
+    </row>
+    <row r="14" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="131" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="145"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="146"/>
+      <c r="F14" s="146"/>
+      <c r="G14" s="145"/>
+      <c r="H14" s="146"/>
+      <c r="I14" s="146"/>
+      <c r="J14" s="147"/>
+      <c r="K14" s="145"/>
+      <c r="L14" s="146"/>
+      <c r="M14" s="146"/>
+      <c r="N14" s="146"/>
+      <c r="O14" s="147"/>
+      <c r="P14" s="132"/>
+    </row>
+    <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3000,20 +3038,23 @@
     <mergeCell ref="K7:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" sqref="C14:O14" xr:uid="{A10332ED-1DF2-4819-9EA2-FAF964C05CC1}"/>
+  </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -3031,23 +3072,23 @@
       <selection activeCell="P4" sqref="P4:T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="3" customWidth="1"/>
-    <col min="2" max="4" width="11.3984375" style="3" customWidth="1"/>
+    <col min="2" max="4" width="11.375" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="0.59765625" style="7" customWidth="1"/>
-    <col min="7" max="11" width="11.3984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="0.625" style="7" customWidth="1"/>
+    <col min="7" max="11" width="11.375" style="3" customWidth="1"/>
     <col min="12" max="12" width="12.5" style="3" customWidth="1"/>
-    <col min="13" max="13" width="0.59765625" style="7" customWidth="1"/>
-    <col min="14" max="19" width="11.3984375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="0.625" style="7" customWidth="1"/>
+    <col min="14" max="19" width="11.375" style="3" customWidth="1"/>
     <col min="20" max="20" width="12.5" style="3" customWidth="1"/>
     <col min="21" max="21" width="3" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="10.59765625" style="3"/>
+    <col min="22" max="16384" width="10.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -3056,8 +3097,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3087,7 +3128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3117,7 +3158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
@@ -3132,7 +3173,7 @@
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
     </row>
-    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
         <v>56</v>
       </c>
@@ -3140,26 +3181,26 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="138" t="s">
+      <c r="G7" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="139"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="141"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="138" t="s">
+      <c r="N7" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="138"/>
-      <c r="S7" s="138"/>
-      <c r="T7" s="139"/>
-    </row>
-    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="140"/>
+      <c r="P7" s="140"/>
+      <c r="Q7" s="140"/>
+      <c r="R7" s="140"/>
+      <c r="S7" s="140"/>
+      <c r="T7" s="141"/>
+    </row>
+    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="38" t="s">
         <v>36</v>
@@ -3215,7 +3256,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="10" t="s">
         <v>32</v>
@@ -3233,7 +3274,7 @@
       <c r="G9" s="47">
         <v>2.2218515429524603</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="77">
         <v>13.331109257714761</v>
       </c>
       <c r="I9" s="14">
@@ -3255,7 +3296,7 @@
       <c r="O9" s="47">
         <v>0.83840543510840237</v>
       </c>
-      <c r="P9" s="78">
+      <c r="P9" s="77">
         <v>5.030432610650414</v>
       </c>
       <c r="Q9" s="14">
@@ -3271,7 +3312,7 @@
         <v>16187.192295867299</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="11" t="s">
         <v>33</v>
@@ -3289,7 +3330,7 @@
       <c r="G10" s="48">
         <v>1.9491242702251876</v>
       </c>
-      <c r="H10" s="79">
+      <c r="H10" s="78">
         <v>9.7456213511259389</v>
       </c>
       <c r="I10" s="16">
@@ -3311,7 +3352,7 @@
       <c r="O10" s="48">
         <v>0.63042261964232194</v>
       </c>
-      <c r="P10" s="79">
+      <c r="P10" s="78">
         <v>3.1521130982116095</v>
       </c>
       <c r="Q10" s="16">
@@ -3327,7 +3368,7 @@
         <v>16188.441978478264</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="38" t="s">
         <v>34</v>
@@ -3347,7 +3388,7 @@
       <c r="G11" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="80">
+      <c r="H11" s="79">
         <f>SUM(H9:H10)</f>
         <v>23.076730608840698</v>
       </c>
@@ -3373,7 +3414,7 @@
       <c r="O11" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="80">
+      <c r="P11" s="79">
         <f>SUM(P9:P10)</f>
         <v>8.1825457088620226</v>
       </c>
@@ -3393,7 +3434,7 @@
         <v>12482.667819304488</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
         <v>57</v>
       </c>
@@ -3401,26 +3442,26 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="134" t="s">
+      <c r="G13" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="135"/>
-      <c r="I13" s="135"/>
-      <c r="J13" s="135"/>
-      <c r="K13" s="135"/>
-      <c r="L13" s="136"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="138"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="134" t="s">
+      <c r="N13" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="135"/>
-      <c r="P13" s="135"/>
-      <c r="Q13" s="135"/>
-      <c r="R13" s="135"/>
-      <c r="S13" s="135"/>
-      <c r="T13" s="136"/>
-    </row>
-    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="137"/>
+      <c r="P13" s="137"/>
+      <c r="Q13" s="137"/>
+      <c r="R13" s="137"/>
+      <c r="S13" s="137"/>
+      <c r="T13" s="138"/>
+    </row>
+    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
         <v>36</v>
       </c>
@@ -3475,7 +3516,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="33" t="s">
         <v>32</v>
       </c>
@@ -3492,7 +3533,7 @@
       <c r="G15" s="47">
         <v>2.2919099249374479</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="77">
         <v>11.45954962468724</v>
       </c>
       <c r="I15" s="14">
@@ -3514,7 +3555,7 @@
       <c r="O15" s="47">
         <v>0.86484164252173046</v>
       </c>
-      <c r="P15" s="78">
+      <c r="P15" s="77">
         <v>4.3242082126086521</v>
       </c>
       <c r="Q15" s="14">
@@ -3530,7 +3571,7 @@
         <v>16187.934659550381</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>33</v>
       </c>
@@ -3547,7 +3588,7 @@
       <c r="G16" s="48">
         <v>2.1401167639699752</v>
       </c>
-      <c r="H16" s="79">
+      <c r="H16" s="78">
         <v>8.5604670558799008</v>
       </c>
       <c r="I16" s="16">
@@ -3569,7 +3610,7 @@
       <c r="O16" s="48">
         <v>0.69219702267958838</v>
       </c>
-      <c r="P16" s="79">
+      <c r="P16" s="78">
         <v>2.7687880907183535</v>
       </c>
       <c r="Q16" s="16">
@@ -3585,7 +3626,7 @@
         <v>16180.364308189717</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>34</v>
       </c>
@@ -3604,7 +3645,7 @@
       <c r="G17" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="80">
+      <c r="H17" s="79">
         <f>SUM(H15:H16)</f>
         <v>20.020016680567139</v>
       </c>
@@ -3630,7 +3671,7 @@
       <c r="O17" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="80">
+      <c r="P17" s="79">
         <f>SUM(P15:P16)</f>
         <v>7.0929963033270056</v>
       </c>
@@ -3650,7 +3691,7 @@
         <v>16184.979533424046</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
         <v>41</v>
       </c>
@@ -3658,26 +3699,26 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="134" t="s">
+      <c r="G19" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="136"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="137"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="137"/>
+      <c r="L19" s="138"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="134" t="s">
+      <c r="N19" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="135"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="135"/>
-      <c r="R19" s="135"/>
-      <c r="S19" s="135"/>
-      <c r="T19" s="136"/>
-    </row>
-    <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O19" s="137"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="137"/>
+      <c r="R19" s="137"/>
+      <c r="S19" s="137"/>
+      <c r="T19" s="138"/>
+    </row>
+    <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
         <v>36</v>
       </c>
@@ -3732,7 +3773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="33" t="s">
         <v>32</v>
       </c>
@@ -3752,7 +3793,7 @@
         <f t="shared" ref="G21:L21" si="0">SUM(G9,G15)</f>
         <v>4.5137614678899087</v>
       </c>
-      <c r="H21" s="78">
+      <c r="H21" s="77">
         <f t="shared" si="0"/>
         <v>24.790658882401999</v>
       </c>
@@ -3781,7 +3822,7 @@
         <f t="shared" si="1"/>
         <v>1.7032470776301327</v>
       </c>
-      <c r="P21" s="78">
+      <c r="P21" s="77">
         <f t="shared" si="1"/>
         <v>9.3546408232590661</v>
       </c>
@@ -3802,7 +3843,7 @@
         <v>32375.12695541768</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
         <v>33</v>
       </c>
@@ -3822,7 +3863,7 @@
         <f t="shared" ref="G22:L22" si="2">SUM(G10,G16)</f>
         <v>4.0892410341951626</v>
       </c>
-      <c r="H22" s="79">
+      <c r="H22" s="78">
         <f t="shared" si="2"/>
         <v>18.306088407005838</v>
       </c>
@@ -3851,7 +3892,7 @@
         <f t="shared" si="3"/>
         <v>1.3226196423219103</v>
       </c>
-      <c r="P22" s="79">
+      <c r="P22" s="78">
         <f t="shared" si="3"/>
         <v>5.920901188929963</v>
       </c>
@@ -3872,7 +3913,7 @@
         <v>32368.806286667983</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="38" t="s">
         <v>34</v>
       </c>
@@ -3892,7 +3933,7 @@
         <f>SUM(G21:G22)</f>
         <v>8.6030025020850722</v>
       </c>
-      <c r="H23" s="80">
+      <c r="H23" s="79">
         <f t="shared" ref="H23:L23" si="4">SUM(H21:H22)</f>
         <v>43.096747289407837</v>
       </c>
@@ -3920,7 +3961,7 @@
         <f t="shared" ref="O23:T23" si="5">SUM(O21:O22)</f>
         <v>3.025866719952043</v>
       </c>
-      <c r="P23" s="80">
+      <c r="P23" s="79">
         <f t="shared" si="5"/>
         <v>15.275542012189028</v>
       </c>
@@ -3941,31 +3982,31 @@
         <v>64743.933242085666</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="140" t="s">
+      <c r="D25" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="140"/>
-      <c r="I25" s="140"/>
-      <c r="J25" s="140"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="140"/>
-      <c r="M25" s="140"/>
-      <c r="N25" s="140"/>
-      <c r="O25" s="140"/>
-      <c r="P25" s="140"/>
-      <c r="Q25" s="140"/>
-      <c r="R25" s="140"/>
-      <c r="S25" s="140"/>
-      <c r="T25" s="140"/>
-    </row>
-    <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="142"/>
+      <c r="F25" s="142"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="142"/>
+      <c r="I25" s="142"/>
+      <c r="J25" s="142"/>
+      <c r="K25" s="142"/>
+      <c r="L25" s="142"/>
+      <c r="M25" s="142"/>
+      <c r="N25" s="142"/>
+      <c r="O25" s="142"/>
+      <c r="P25" s="142"/>
+      <c r="Q25" s="142"/>
+      <c r="R25" s="142"/>
+      <c r="S25" s="142"/>
+      <c r="T25" s="142"/>
+    </row>
+    <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="D26" s="53"/>
       <c r="E26" s="53"/>
@@ -3985,31 +4026,31 @@
       <c r="S26" s="53"/>
       <c r="T26" s="53"/>
     </row>
-    <row r="27" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="140" t="s">
+      <c r="D27" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="140"/>
-      <c r="I27" s="140"/>
-      <c r="J27" s="140"/>
-      <c r="K27" s="140"/>
-      <c r="L27" s="140"/>
-      <c r="M27" s="140"/>
-      <c r="N27" s="140"/>
-      <c r="O27" s="140"/>
-      <c r="P27" s="140"/>
-      <c r="Q27" s="140"/>
-      <c r="R27" s="140"/>
-      <c r="S27" s="140"/>
-      <c r="T27" s="140"/>
-    </row>
-    <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="142"/>
+      <c r="K27" s="142"/>
+      <c r="L27" s="142"/>
+      <c r="M27" s="142"/>
+      <c r="N27" s="142"/>
+      <c r="O27" s="142"/>
+      <c r="P27" s="142"/>
+      <c r="Q27" s="142"/>
+      <c r="R27" s="142"/>
+      <c r="S27" s="142"/>
+      <c r="T27" s="142"/>
+    </row>
+    <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="D28" s="53"/>
       <c r="E28" s="53"/>
@@ -4029,31 +4070,31 @@
       <c r="S28" s="53"/>
       <c r="T28" s="53"/>
     </row>
-    <row r="29" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="140" t="s">
+      <c r="D29" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="140"/>
-      <c r="F29" s="140"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="140"/>
-      <c r="I29" s="140"/>
-      <c r="J29" s="140"/>
-      <c r="K29" s="140"/>
-      <c r="L29" s="140"/>
-      <c r="M29" s="140"/>
-      <c r="N29" s="140"/>
-      <c r="O29" s="140"/>
-      <c r="P29" s="140"/>
-      <c r="Q29" s="140"/>
-      <c r="R29" s="140"/>
-      <c r="S29" s="140"/>
-      <c r="T29" s="140"/>
-    </row>
-    <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="142"/>
+      <c r="F29" s="142"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="142"/>
+      <c r="J29" s="142"/>
+      <c r="K29" s="142"/>
+      <c r="L29" s="142"/>
+      <c r="M29" s="142"/>
+      <c r="N29" s="142"/>
+      <c r="O29" s="142"/>
+      <c r="P29" s="142"/>
+      <c r="Q29" s="142"/>
+      <c r="R29" s="142"/>
+      <c r="S29" s="142"/>
+      <c r="T29" s="142"/>
+    </row>
+    <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="D30" s="53"/>
       <c r="E30" s="53"/>
@@ -4073,31 +4114,31 @@
       <c r="S30" s="53"/>
       <c r="T30" s="53"/>
     </row>
-    <row r="31" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="140" t="s">
+      <c r="D31" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="140"/>
-      <c r="F31" s="140"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="140"/>
-      <c r="I31" s="140"/>
-      <c r="J31" s="140"/>
-      <c r="K31" s="140"/>
-      <c r="L31" s="140"/>
-      <c r="M31" s="140"/>
-      <c r="N31" s="140"/>
-      <c r="O31" s="140"/>
-      <c r="P31" s="140"/>
-      <c r="Q31" s="140"/>
-      <c r="R31" s="140"/>
-      <c r="S31" s="140"/>
-      <c r="T31" s="140"/>
-    </row>
-    <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="142"/>
+      <c r="J31" s="142"/>
+      <c r="K31" s="142"/>
+      <c r="L31" s="142"/>
+      <c r="M31" s="142"/>
+      <c r="N31" s="142"/>
+      <c r="O31" s="142"/>
+      <c r="P31" s="142"/>
+      <c r="Q31" s="142"/>
+      <c r="R31" s="142"/>
+      <c r="S31" s="142"/>
+      <c r="T31" s="142"/>
+    </row>
+    <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="D32" s="53"/>
       <c r="E32" s="53"/>
@@ -4117,31 +4158,31 @@
       <c r="S32" s="53"/>
       <c r="T32" s="53"/>
     </row>
-    <row r="33" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="140" t="s">
+      <c r="D33" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="140"/>
-      <c r="J33" s="140"/>
-      <c r="K33" s="140"/>
-      <c r="L33" s="140"/>
-      <c r="M33" s="140"/>
-      <c r="N33" s="140"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="140"/>
-      <c r="Q33" s="140"/>
-      <c r="R33" s="140"/>
-      <c r="S33" s="140"/>
-      <c r="T33" s="140"/>
-    </row>
-    <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="142"/>
+      <c r="F33" s="142"/>
+      <c r="G33" s="142"/>
+      <c r="H33" s="142"/>
+      <c r="I33" s="142"/>
+      <c r="J33" s="142"/>
+      <c r="K33" s="142"/>
+      <c r="L33" s="142"/>
+      <c r="M33" s="142"/>
+      <c r="N33" s="142"/>
+      <c r="O33" s="142"/>
+      <c r="P33" s="142"/>
+      <c r="Q33" s="142"/>
+      <c r="R33" s="142"/>
+      <c r="S33" s="142"/>
+      <c r="T33" s="142"/>
+    </row>
+    <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="D34" s="53"/>
       <c r="E34" s="53"/>
@@ -4161,29 +4202,29 @@
       <c r="S34" s="53"/>
       <c r="T34" s="53"/>
     </row>
-    <row r="35" spans="2:20" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:20" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="137" t="s">
+      <c r="D35" s="139" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="137"/>
-      <c r="F35" s="137"/>
-      <c r="G35" s="137"/>
-      <c r="H35" s="137"/>
-      <c r="I35" s="137"/>
-      <c r="J35" s="137"/>
-      <c r="K35" s="137"/>
-      <c r="L35" s="137"/>
-      <c r="M35" s="137"/>
-      <c r="N35" s="137"/>
-      <c r="O35" s="137"/>
-      <c r="P35" s="137"/>
-      <c r="Q35" s="137"/>
-      <c r="R35" s="137"/>
-      <c r="S35" s="137"/>
-      <c r="T35" s="137"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="139"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="139"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="139"/>
+      <c r="K35" s="139"/>
+      <c r="L35" s="139"/>
+      <c r="M35" s="139"/>
+      <c r="N35" s="139"/>
+      <c r="O35" s="139"/>
+      <c r="P35" s="139"/>
+      <c r="Q35" s="139"/>
+      <c r="R35" s="139"/>
+      <c r="S35" s="139"/>
+      <c r="T35" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4217,21 +4258,21 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.8984375" style="3" customWidth="1"/>
-    <col min="3" max="5" width="13.3984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="2.59765625" style="7" customWidth="1"/>
-    <col min="7" max="12" width="13.3984375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="2.59765625" style="7" customWidth="1"/>
-    <col min="14" max="20" width="13.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.875" style="3" customWidth="1"/>
+    <col min="3" max="5" width="13.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="2.625" style="7" customWidth="1"/>
+    <col min="7" max="12" width="13.375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="2.625" style="7" customWidth="1"/>
+    <col min="14" max="20" width="13.375" style="3" customWidth="1"/>
     <col min="21" max="21" width="3" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="10.59765625" style="3"/>
+    <col min="22" max="16384" width="10.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -4239,8 +4280,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4271,7 +4312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -4302,7 +4343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
@@ -4317,7 +4358,7 @@
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
     </row>
-    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
         <v>40</v>
       </c>
@@ -4325,26 +4366,26 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="138" t="s">
+      <c r="G7" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="139"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="141"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="138" t="s">
+      <c r="N7" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="138"/>
-      <c r="S7" s="138"/>
-      <c r="T7" s="139"/>
-    </row>
-    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="140"/>
+      <c r="P7" s="140"/>
+      <c r="Q7" s="140"/>
+      <c r="R7" s="140"/>
+      <c r="S7" s="140"/>
+      <c r="T7" s="141"/>
+    </row>
+    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="38" t="s">
         <v>36</v>
@@ -4400,7 +4441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="10" t="s">
         <v>32</v>
@@ -4456,7 +4497,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="11" t="s">
         <v>33</v>
@@ -4512,7 +4553,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="38" t="s">
         <v>34</v>
@@ -4576,7 +4617,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
         <v>39</v>
       </c>
@@ -4584,26 +4625,26 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="134" t="s">
+      <c r="G13" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="135"/>
-      <c r="I13" s="135"/>
-      <c r="J13" s="135"/>
-      <c r="K13" s="135"/>
-      <c r="L13" s="136"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="138"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="134" t="s">
+      <c r="N13" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="135"/>
-      <c r="P13" s="135"/>
-      <c r="Q13" s="135"/>
-      <c r="R13" s="135"/>
-      <c r="S13" s="135"/>
-      <c r="T13" s="136"/>
-    </row>
-    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="137"/>
+      <c r="P13" s="137"/>
+      <c r="Q13" s="137"/>
+      <c r="R13" s="137"/>
+      <c r="S13" s="137"/>
+      <c r="T13" s="138"/>
+    </row>
+    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
         <v>36</v>
       </c>
@@ -4658,7 +4699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="33" t="s">
         <v>32</v>
       </c>
@@ -4713,7 +4754,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>33</v>
       </c>
@@ -4768,7 +4809,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>34</v>
       </c>
@@ -4831,7 +4872,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
         <v>38</v>
       </c>
@@ -4839,26 +4880,26 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="134" t="s">
+      <c r="G19" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="136"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="137"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="137"/>
+      <c r="L19" s="138"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="134" t="s">
+      <c r="N19" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="135"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="135"/>
-      <c r="R19" s="135"/>
-      <c r="S19" s="135"/>
-      <c r="T19" s="136"/>
-    </row>
-    <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O19" s="137"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="137"/>
+      <c r="R19" s="137"/>
+      <c r="S19" s="137"/>
+      <c r="T19" s="138"/>
+    </row>
+    <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
         <v>36</v>
       </c>
@@ -4913,7 +4954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="33" t="s">
         <v>32</v>
       </c>
@@ -4968,7 +5009,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
         <v>33</v>
       </c>
@@ -5023,7 +5064,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="38" t="s">
         <v>34</v>
       </c>
@@ -5086,7 +5127,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="52" t="s">
         <v>41</v>
       </c>
@@ -5094,26 +5135,26 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="134" t="s">
+      <c r="G25" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="135"/>
-      <c r="I25" s="135"/>
-      <c r="J25" s="135"/>
-      <c r="K25" s="135"/>
-      <c r="L25" s="136"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="137"/>
+      <c r="J25" s="137"/>
+      <c r="K25" s="137"/>
+      <c r="L25" s="138"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="134" t="s">
+      <c r="N25" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="135"/>
-      <c r="P25" s="135"/>
-      <c r="Q25" s="135"/>
-      <c r="R25" s="135"/>
-      <c r="S25" s="135"/>
-      <c r="T25" s="136"/>
-    </row>
-    <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O25" s="137"/>
+      <c r="P25" s="137"/>
+      <c r="Q25" s="137"/>
+      <c r="R25" s="137"/>
+      <c r="S25" s="137"/>
+      <c r="T25" s="138"/>
+    </row>
+    <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
         <v>36</v>
       </c>
@@ -5168,7 +5209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="33" t="s">
         <v>32</v>
       </c>
@@ -5225,7 +5266,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="34" t="s">
         <v>33</v>
       </c>
@@ -5282,7 +5323,7 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="38" t="s">
         <v>34</v>
       </c>
@@ -5345,32 +5386,32 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="131"/>
-      <c r="E31" s="131"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="131"/>
-      <c r="H31" s="131"/>
-      <c r="I31" s="131"/>
-      <c r="J31" s="131"/>
-      <c r="K31" s="131"/>
-      <c r="L31" s="131"/>
-      <c r="M31" s="131"/>
-      <c r="N31" s="131"/>
-      <c r="O31" s="131"/>
-      <c r="P31" s="131"/>
-      <c r="Q31" s="131"/>
-      <c r="R31" s="131"/>
-      <c r="S31" s="131"/>
-      <c r="T31" s="131"/>
-    </row>
-    <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="133"/>
+      <c r="H31" s="133"/>
+      <c r="I31" s="133"/>
+      <c r="J31" s="133"/>
+      <c r="K31" s="133"/>
+      <c r="L31" s="133"/>
+      <c r="M31" s="133"/>
+      <c r="N31" s="133"/>
+      <c r="O31" s="133"/>
+      <c r="P31" s="133"/>
+      <c r="Q31" s="133"/>
+      <c r="R31" s="133"/>
+      <c r="S31" s="133"/>
+      <c r="T31" s="133"/>
+    </row>
+    <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="53"/>
       <c r="D32" s="53"/>
@@ -5391,32 +5432,32 @@
       <c r="S32" s="53"/>
       <c r="T32" s="53"/>
     </row>
-    <row r="33" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="131" t="s">
+      <c r="C33" s="133" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="131"/>
-      <c r="H33" s="131"/>
-      <c r="I33" s="131"/>
-      <c r="J33" s="131"/>
-      <c r="K33" s="131"/>
-      <c r="L33" s="131"/>
-      <c r="M33" s="131"/>
-      <c r="N33" s="131"/>
-      <c r="O33" s="131"/>
-      <c r="P33" s="131"/>
-      <c r="Q33" s="131"/>
-      <c r="R33" s="131"/>
-      <c r="S33" s="131"/>
-      <c r="T33" s="131"/>
-    </row>
-    <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="133"/>
+      <c r="G33" s="133"/>
+      <c r="H33" s="133"/>
+      <c r="I33" s="133"/>
+      <c r="J33" s="133"/>
+      <c r="K33" s="133"/>
+      <c r="L33" s="133"/>
+      <c r="M33" s="133"/>
+      <c r="N33" s="133"/>
+      <c r="O33" s="133"/>
+      <c r="P33" s="133"/>
+      <c r="Q33" s="133"/>
+      <c r="R33" s="133"/>
+      <c r="S33" s="133"/>
+      <c r="T33" s="133"/>
+    </row>
+    <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="53"/>
       <c r="D34" s="53"/>
@@ -5437,32 +5478,32 @@
       <c r="S34" s="53"/>
       <c r="T34" s="53"/>
     </row>
-    <row r="35" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="131" t="s">
+      <c r="C35" s="133" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
-      <c r="F35" s="131"/>
-      <c r="G35" s="131"/>
-      <c r="H35" s="131"/>
-      <c r="I35" s="131"/>
-      <c r="J35" s="131"/>
-      <c r="K35" s="131"/>
-      <c r="L35" s="131"/>
-      <c r="M35" s="131"/>
-      <c r="N35" s="131"/>
-      <c r="O35" s="131"/>
-      <c r="P35" s="131"/>
-      <c r="Q35" s="131"/>
-      <c r="R35" s="131"/>
-      <c r="S35" s="131"/>
-      <c r="T35" s="131"/>
-    </row>
-    <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="133"/>
+      <c r="G35" s="133"/>
+      <c r="H35" s="133"/>
+      <c r="I35" s="133"/>
+      <c r="J35" s="133"/>
+      <c r="K35" s="133"/>
+      <c r="L35" s="133"/>
+      <c r="M35" s="133"/>
+      <c r="N35" s="133"/>
+      <c r="O35" s="133"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="133"/>
+      <c r="R35" s="133"/>
+      <c r="S35" s="133"/>
+      <c r="T35" s="133"/>
+    </row>
+    <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="53"/>
       <c r="D36" s="53"/>
@@ -5483,32 +5524,32 @@
       <c r="S36" s="53"/>
       <c r="T36" s="53"/>
     </row>
-    <row r="37" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="131" t="s">
+      <c r="C37" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="131"/>
-      <c r="H37" s="131"/>
-      <c r="I37" s="131"/>
-      <c r="J37" s="131"/>
-      <c r="K37" s="131"/>
-      <c r="L37" s="131"/>
-      <c r="M37" s="131"/>
-      <c r="N37" s="131"/>
-      <c r="O37" s="131"/>
-      <c r="P37" s="131"/>
-      <c r="Q37" s="131"/>
-      <c r="R37" s="131"/>
-      <c r="S37" s="131"/>
-      <c r="T37" s="131"/>
-    </row>
-    <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="133"/>
+      <c r="E37" s="133"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="133"/>
+      <c r="H37" s="133"/>
+      <c r="I37" s="133"/>
+      <c r="J37" s="133"/>
+      <c r="K37" s="133"/>
+      <c r="L37" s="133"/>
+      <c r="M37" s="133"/>
+      <c r="N37" s="133"/>
+      <c r="O37" s="133"/>
+      <c r="P37" s="133"/>
+      <c r="Q37" s="133"/>
+      <c r="R37" s="133"/>
+      <c r="S37" s="133"/>
+      <c r="T37" s="133"/>
+    </row>
+    <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="53"/>
       <c r="D38" s="53"/>
@@ -5529,32 +5570,32 @@
       <c r="S38" s="53"/>
       <c r="T38" s="53"/>
     </row>
-    <row r="39" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="131" t="s">
+      <c r="C39" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="131"/>
-      <c r="E39" s="131"/>
-      <c r="F39" s="131"/>
-      <c r="G39" s="131"/>
-      <c r="H39" s="131"/>
-      <c r="I39" s="131"/>
-      <c r="J39" s="131"/>
-      <c r="K39" s="131"/>
-      <c r="L39" s="131"/>
-      <c r="M39" s="131"/>
-      <c r="N39" s="131"/>
-      <c r="O39" s="131"/>
-      <c r="P39" s="131"/>
-      <c r="Q39" s="131"/>
-      <c r="R39" s="131"/>
-      <c r="S39" s="131"/>
-      <c r="T39" s="131"/>
-    </row>
-    <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="133"/>
+      <c r="E39" s="133"/>
+      <c r="F39" s="133"/>
+      <c r="G39" s="133"/>
+      <c r="H39" s="133"/>
+      <c r="I39" s="133"/>
+      <c r="J39" s="133"/>
+      <c r="K39" s="133"/>
+      <c r="L39" s="133"/>
+      <c r="M39" s="133"/>
+      <c r="N39" s="133"/>
+      <c r="O39" s="133"/>
+      <c r="P39" s="133"/>
+      <c r="Q39" s="133"/>
+      <c r="R39" s="133"/>
+      <c r="S39" s="133"/>
+      <c r="T39" s="133"/>
+    </row>
+    <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="53"/>
       <c r="D40" s="53"/>
@@ -5575,30 +5616,30 @@
       <c r="S40" s="53"/>
       <c r="T40" s="53"/>
     </row>
-    <row r="41" spans="2:20" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:20" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="133" t="s">
+      <c r="C41" s="135" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="133"/>
-      <c r="E41" s="133"/>
-      <c r="F41" s="133"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="133"/>
-      <c r="K41" s="133"/>
-      <c r="L41" s="133"/>
-      <c r="M41" s="133"/>
-      <c r="N41" s="133"/>
-      <c r="O41" s="133"/>
-      <c r="P41" s="133"/>
-      <c r="Q41" s="133"/>
-      <c r="R41" s="133"/>
-      <c r="S41" s="133"/>
-      <c r="T41" s="133"/>
+      <c r="D41" s="135"/>
+      <c r="E41" s="135"/>
+      <c r="F41" s="135"/>
+      <c r="G41" s="135"/>
+      <c r="H41" s="135"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="135"/>
+      <c r="K41" s="135"/>
+      <c r="L41" s="135"/>
+      <c r="M41" s="135"/>
+      <c r="N41" s="135"/>
+      <c r="O41" s="135"/>
+      <c r="P41" s="135"/>
+      <c r="Q41" s="135"/>
+      <c r="R41" s="135"/>
+      <c r="S41" s="135"/>
+      <c r="T41" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5634,114 +5675,114 @@
       <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" style="99" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="3" style="99" customWidth="1"/>
-    <col min="3" max="3" width="24.8984375" style="99" customWidth="1"/>
-    <col min="4" max="4" width="68" style="99" customWidth="1"/>
-    <col min="5" max="5" width="2.3984375" style="99" customWidth="1"/>
-    <col min="6" max="12" width="10.8984375" style="99" customWidth="1"/>
-    <col min="13" max="13" width="3" style="99" customWidth="1"/>
-    <col min="14" max="16384" width="10.59765625" style="99"/>
+    <col min="1" max="1" width="0" style="98" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="98" customWidth="1"/>
+    <col min="3" max="3" width="24.875" style="98" customWidth="1"/>
+    <col min="4" max="4" width="68" style="98" customWidth="1"/>
+    <col min="5" max="5" width="2.375" style="98" customWidth="1"/>
+    <col min="6" max="12" width="10.875" style="98" customWidth="1"/>
+    <col min="13" max="13" width="3" style="98" customWidth="1"/>
+    <col min="14" max="16384" width="10.625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:4" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:4" s="116" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="141" t="s">
+    <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:4" s="115" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="141"/>
-    </row>
-    <row r="5" spans="3:4" s="116" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="141" t="s">
+      <c r="D4" s="143"/>
+    </row>
+    <row r="5" spans="3:4" s="115" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="141"/>
-    </row>
-    <row r="6" spans="3:4" s="116" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="141" t="s">
+      <c r="D5" s="143"/>
+    </row>
+    <row r="6" spans="3:4" s="115" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="141"/>
-    </row>
-    <row r="7" spans="3:4" s="116" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="141" t="s">
+      <c r="D6" s="143"/>
+    </row>
+    <row r="7" spans="3:4" s="115" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="141"/>
-    </row>
-    <row r="8" spans="3:4" s="116" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="141" t="s">
+      <c r="D7" s="143"/>
+    </row>
+    <row r="8" spans="3:4" s="115" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="143" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="141"/>
-    </row>
-    <row r="9" spans="3:4" s="116" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="141" t="s">
+      <c r="D8" s="143"/>
+    </row>
+    <row r="9" spans="3:4" s="115" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="143" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="141"/>
-    </row>
-    <row r="10" spans="3:4" s="116" customFormat="1" ht="147.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="141" t="s">
+      <c r="D9" s="143"/>
+    </row>
+    <row r="10" spans="3:4" s="115" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="143" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="141"/>
-    </row>
-    <row r="11" spans="3:4" s="116" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="141" t="s">
+      <c r="D10" s="143"/>
+    </row>
+    <row r="11" spans="3:4" s="115" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="143" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="141"/>
-    </row>
-    <row r="12" spans="3:4" s="116" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="141" t="s">
+      <c r="D11" s="143"/>
+    </row>
+    <row r="12" spans="3:4" s="115" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="143" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="141"/>
-    </row>
-    <row r="13" spans="3:4" s="116" customFormat="1" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="141" t="s">
+      <c r="D12" s="143"/>
+    </row>
+    <row r="13" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="141"/>
-    </row>
-    <row r="14" spans="3:4" s="116" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="141" t="s">
+      <c r="D13" s="143"/>
+    </row>
+    <row r="14" spans="3:4" s="115" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="141"/>
-    </row>
-    <row r="15" spans="3:4" s="116" customFormat="1" ht="51.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="141" t="s">
+      <c r="D14" s="143"/>
+    </row>
+    <row r="15" spans="3:4" s="115" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="141"/>
-    </row>
-    <row r="16" spans="3:4" s="116" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="141" t="s">
+      <c r="D15" s="143"/>
+    </row>
+    <row r="16" spans="3:4" s="115" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="141"/>
-    </row>
-    <row r="17" spans="3:4" s="116" customFormat="1" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="141" t="s">
+      <c r="D16" s="143"/>
+    </row>
+    <row r="17" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="141"/>
-    </row>
-    <row r="18" spans="3:4" s="116" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="141" t="s">
+      <c r="D17" s="143"/>
+    </row>
+    <row r="18" spans="3:4" s="115" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="143" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="141"/>
+      <c r="D18" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5778,25 +5819,25 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="99" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="3" style="99" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" style="99" customWidth="1"/>
-    <col min="4" max="4" width="9" style="99" customWidth="1"/>
-    <col min="5" max="5" width="7.8984375" style="99" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" style="99" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="99" customWidth="1"/>
-    <col min="8" max="12" width="11.3984375" style="99" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="99" customWidth="1"/>
-    <col min="14" max="19" width="11.3984375" style="99" customWidth="1"/>
-    <col min="20" max="20" width="12.5" style="99" customWidth="1"/>
-    <col min="21" max="21" width="3" style="99" customWidth="1"/>
-    <col min="22" max="16384" width="10.59765625" style="99"/>
+    <col min="1" max="1" width="4" style="98" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="98" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="98" customWidth="1"/>
+    <col min="4" max="4" width="9" style="98" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="98" customWidth="1"/>
+    <col min="6" max="6" width="11.375" style="98" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="98" customWidth="1"/>
+    <col min="8" max="12" width="11.375" style="98" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="98" customWidth="1"/>
+    <col min="14" max="19" width="11.375" style="98" customWidth="1"/>
+    <col min="20" max="20" width="12.5" style="98" customWidth="1"/>
+    <col min="21" max="21" width="3" style="98" customWidth="1"/>
+    <col min="22" max="16384" width="10.625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:20" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
         <v>88</v>
@@ -5805,8 +5846,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -5835,26 +5876,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="131"/>
-      <c r="Q5" s="131"/>
-      <c r="R5" s="131"/>
-      <c r="S5" s="131"/>
-    </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="133"/>
+      <c r="Q5" s="133"/>
+      <c r="R5" s="133"/>
+      <c r="S5" s="133"/>
+    </row>
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
@@ -5869,30 +5910,30 @@
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
     </row>
-    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="134" t="s">
+      <c r="H7" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="135"/>
-      <c r="J7" s="135"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="135"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="138"/>
-      <c r="S7" s="138"/>
-      <c r="T7" s="139"/>
-    </row>
-    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99" t="s">
+      <c r="I7" s="137"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="137"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="140"/>
+      <c r="P7" s="140"/>
+      <c r="Q7" s="140"/>
+      <c r="R7" s="140"/>
+      <c r="S7" s="140"/>
+      <c r="T7" s="141"/>
+    </row>
+    <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="98" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="24"/>
@@ -5951,32 +5992,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99" t="str">
+    <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="98" t="str">
         <f>IF(OR($A8="Start",$A8="Even"),"Odd","Even")</f>
         <v>Odd</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="121"/>
-      <c r="N9" s="127"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="123"/>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="121"/>
-    </row>
-    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="118"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="123"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="126"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="122"/>
+      <c r="Q9" s="118"/>
+      <c r="R9" s="118"/>
+      <c r="S9" s="123"/>
+      <c r="T9" s="120"/>
+    </row>
+    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="24"/>
       <c r="C10" s="38"/>
       <c r="D10" s="39" t="s">
@@ -5990,7 +6031,7 @@
       <c r="H10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="80"/>
+      <c r="I10" s="79"/>
       <c r="J10" s="50" t="s">
         <v>35</v>
       </c>
@@ -6003,7 +6044,7 @@
       <c r="O10" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="80"/>
+      <c r="P10" s="79"/>
       <c r="Q10" s="50" t="s">
         <v>35</v>
       </c>
@@ -6011,7 +6052,7 @@
       <c r="S10" s="46"/>
       <c r="T10" s="42"/>
     </row>
-    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
         <v>41</v>
       </c>
@@ -6019,24 +6060,24 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="134" t="s">
+      <c r="H12" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="135"/>
-      <c r="J12" s="135"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="135"/>
-      <c r="M12" s="136"/>
-      <c r="N12" s="134"/>
-      <c r="O12" s="135"/>
-      <c r="P12" s="135"/>
-      <c r="Q12" s="135"/>
-      <c r="R12" s="135"/>
-      <c r="S12" s="135"/>
-      <c r="T12" s="136"/>
-    </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99" t="s">
+      <c r="I12" s="137"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="138"/>
+      <c r="N12" s="136"/>
+      <c r="O12" s="137"/>
+      <c r="P12" s="137"/>
+      <c r="Q12" s="137"/>
+      <c r="R12" s="137"/>
+      <c r="S12" s="137"/>
+      <c r="T12" s="138"/>
+    </row>
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="98" t="s">
         <v>69</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -6092,31 +6133,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="99" t="str">
+    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="98" t="str">
         <f>IF(OR($A13="Start",$A13="Even"),"Odd","Even")</f>
         <v>Odd</v>
       </c>
-      <c r="C14" s="125"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="121"/>
-      <c r="H14" s="122"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="127"/>
-      <c r="O14" s="122"/>
-      <c r="P14" s="123"/>
-      <c r="Q14" s="119"/>
-      <c r="R14" s="119"/>
-      <c r="S14" s="124"/>
-      <c r="T14" s="121"/>
-    </row>
-    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="124"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="118"/>
+      <c r="L14" s="123"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="126"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="122"/>
+      <c r="Q14" s="118"/>
+      <c r="R14" s="118"/>
+      <c r="S14" s="123"/>
+      <c r="T14" s="120"/>
+    </row>
+    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="38"/>
       <c r="D15" s="39" t="s">
         <v>68</v>
@@ -6129,7 +6170,7 @@
       <c r="H15" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="80"/>
+      <c r="I15" s="79"/>
       <c r="J15" s="50" t="s">
         <v>35</v>
       </c>
@@ -6142,7 +6183,7 @@
       <c r="O15" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="80"/>
+      <c r="P15" s="79"/>
       <c r="Q15" s="50" t="s">
         <v>35</v>
       </c>
@@ -6150,188 +6191,188 @@
       <c r="S15" s="46"/>
       <c r="T15" s="42"/>
     </row>
-    <row r="17" spans="3:20" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="54" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="54"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
-      <c r="H17" s="142"/>
-      <c r="I17" s="142"/>
-      <c r="J17" s="142"/>
-      <c r="K17" s="142"/>
-      <c r="L17" s="142"/>
-      <c r="M17" s="142"/>
-      <c r="N17" s="142"/>
-      <c r="O17" s="142"/>
-      <c r="P17" s="142"/>
-      <c r="Q17" s="142"/>
-      <c r="R17" s="142"/>
-      <c r="S17" s="142"/>
-      <c r="T17" s="142"/>
-    </row>
-    <row r="18" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="116"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="144"/>
+      <c r="I17" s="144"/>
+      <c r="J17" s="144"/>
+      <c r="K17" s="144"/>
+      <c r="L17" s="144"/>
+      <c r="M17" s="144"/>
+      <c r="N17" s="144"/>
+      <c r="O17" s="144"/>
+      <c r="P17" s="144"/>
+      <c r="Q17" s="144"/>
+      <c r="R17" s="144"/>
+      <c r="S17" s="144"/>
+      <c r="T17" s="144"/>
+    </row>
+    <row r="18" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="76"/>
-      <c r="R18" s="76"/>
-      <c r="S18" s="76"/>
-      <c r="T18" s="76"/>
-    </row>
-    <row r="19" spans="3:20" s="117" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="75"/>
+      <c r="T18" s="75"/>
+    </row>
+    <row r="19" spans="3:20" s="116" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="54" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="54"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="142"/>
-      <c r="H19" s="142"/>
-      <c r="I19" s="142"/>
-      <c r="J19" s="142"/>
-      <c r="K19" s="142"/>
-      <c r="L19" s="142"/>
-      <c r="M19" s="142"/>
-      <c r="N19" s="142"/>
-      <c r="O19" s="142"/>
-      <c r="P19" s="142"/>
-      <c r="Q19" s="142"/>
-      <c r="R19" s="142"/>
-      <c r="S19" s="142"/>
-      <c r="T19" s="142"/>
-    </row>
-    <row r="20" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="144"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="144"/>
+      <c r="K19" s="144"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="144"/>
+      <c r="N19" s="144"/>
+      <c r="O19" s="144"/>
+      <c r="P19" s="144"/>
+      <c r="Q19" s="144"/>
+      <c r="R19" s="144"/>
+      <c r="S19" s="144"/>
+      <c r="T19" s="144"/>
+    </row>
+    <row r="20" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="118"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118"/>
-      <c r="O20" s="118"/>
-      <c r="P20" s="118"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="118"/>
-      <c r="S20" s="118"/>
-      <c r="T20" s="118"/>
-    </row>
-    <row r="21" spans="3:20" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="117"/>
+      <c r="K20" s="117"/>
+      <c r="L20" s="117"/>
+      <c r="M20" s="117"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="117"/>
+      <c r="P20" s="117"/>
+      <c r="Q20" s="117"/>
+      <c r="R20" s="117"/>
+      <c r="S20" s="117"/>
+      <c r="T20" s="117"/>
+    </row>
+    <row r="21" spans="3:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="54"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="142"/>
-      <c r="H21" s="142"/>
-      <c r="I21" s="142"/>
-      <c r="J21" s="142"/>
-      <c r="K21" s="142"/>
-      <c r="L21" s="142"/>
-      <c r="M21" s="142"/>
-      <c r="N21" s="142"/>
-      <c r="O21" s="142"/>
-      <c r="P21" s="142"/>
-      <c r="Q21" s="142"/>
-      <c r="R21" s="142"/>
-      <c r="S21" s="142"/>
-      <c r="T21" s="142"/>
-    </row>
-    <row r="22" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="116"/>
+      <c r="F21" s="144"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="144"/>
+      <c r="I21" s="144"/>
+      <c r="J21" s="144"/>
+      <c r="K21" s="144"/>
+      <c r="L21" s="144"/>
+      <c r="M21" s="144"/>
+      <c r="N21" s="144"/>
+      <c r="O21" s="144"/>
+      <c r="P21" s="144"/>
+      <c r="Q21" s="144"/>
+      <c r="R21" s="144"/>
+      <c r="S21" s="144"/>
+      <c r="T21" s="144"/>
+    </row>
+    <row r="22" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
-      <c r="P22" s="118"/>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="118"/>
-      <c r="S22" s="118"/>
-      <c r="T22" s="118"/>
-    </row>
-    <row r="23" spans="3:20" s="117" customFormat="1" ht="48.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="117"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="117"/>
+      <c r="N22" s="117"/>
+      <c r="O22" s="117"/>
+      <c r="P22" s="117"/>
+      <c r="Q22" s="117"/>
+      <c r="R22" s="117"/>
+      <c r="S22" s="117"/>
+      <c r="T22" s="117"/>
+    </row>
+    <row r="23" spans="3:20" s="116" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="54" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="54"/>
-      <c r="F23" s="142"/>
-      <c r="G23" s="142"/>
-      <c r="H23" s="142"/>
-      <c r="I23" s="142"/>
-      <c r="J23" s="142"/>
-      <c r="K23" s="142"/>
-      <c r="L23" s="142"/>
-      <c r="M23" s="142"/>
-      <c r="N23" s="142"/>
-      <c r="O23" s="142"/>
-      <c r="P23" s="142"/>
-      <c r="Q23" s="142"/>
-      <c r="R23" s="142"/>
-      <c r="S23" s="142"/>
-      <c r="T23" s="142"/>
-    </row>
-    <row r="24" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="144"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
+      <c r="J23" s="144"/>
+      <c r="K23" s="144"/>
+      <c r="L23" s="144"/>
+      <c r="M23" s="144"/>
+      <c r="N23" s="144"/>
+      <c r="O23" s="144"/>
+      <c r="P23" s="144"/>
+      <c r="Q23" s="144"/>
+      <c r="R23" s="144"/>
+      <c r="S23" s="144"/>
+      <c r="T23" s="144"/>
+    </row>
+    <row r="24" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="118"/>
-      <c r="P24" s="118"/>
-      <c r="Q24" s="118"/>
-      <c r="R24" s="118"/>
-      <c r="S24" s="118"/>
-      <c r="T24" s="118"/>
-    </row>
-    <row r="25" spans="3:20" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="117"/>
+      <c r="M24" s="117"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="117"/>
+      <c r="P24" s="117"/>
+      <c r="Q24" s="117"/>
+      <c r="R24" s="117"/>
+      <c r="S24" s="117"/>
+      <c r="T24" s="117"/>
+    </row>
+    <row r="25" spans="3:20" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="54" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="54"/>
-      <c r="F25" s="133"/>
-      <c r="G25" s="133"/>
-      <c r="H25" s="133"/>
-      <c r="I25" s="133"/>
-      <c r="J25" s="133"/>
-      <c r="K25" s="133"/>
-      <c r="L25" s="133"/>
-      <c r="M25" s="133"/>
-      <c r="N25" s="133"/>
-      <c r="O25" s="133"/>
-      <c r="P25" s="133"/>
-      <c r="Q25" s="133"/>
-      <c r="R25" s="133"/>
-      <c r="S25" s="133"/>
-      <c r="T25" s="133"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="135"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="135"/>
+      <c r="J25" s="135"/>
+      <c r="K25" s="135"/>
+      <c r="L25" s="135"/>
+      <c r="M25" s="135"/>
+      <c r="N25" s="135"/>
+      <c r="O25" s="135"/>
+      <c r="P25" s="135"/>
+      <c r="Q25" s="135"/>
+      <c r="R25" s="135"/>
+      <c r="S25" s="135"/>
+      <c r="T25" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -6353,52 +6394,52 @@
     <mergeCell ref="F19:T19"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:T3 C5 C4:N4 P4 R4:T4 T5 C6:T1048576">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Merged PR 7326: PRI-19858 Export Campaign to Excel - Proposal tab - Secondary Audiences - Quarterly Delivery
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\plan-excel-generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{116C7BE8-72CF-4866-A15D-7825A8F2A260}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF4FA64D-2E89-41D7-85C2-9CF6A06F27B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="465" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="91">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -1132,7 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1503,12 +1503,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1530,6 +1524,15 @@
     <xf numFmtId="1" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
@@ -1565,15 +1568,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2358,11 +2352,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="133">
+      <c r="E5" s="134">
         <f>Proposal!H5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="133"/>
+      <c r="F5" s="134"/>
       <c r="G5" s="75">
         <f>Proposal!J5</f>
         <v>0</v>
@@ -2557,35 +2551,35 @@
       <c r="C18" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="135">
-        <f>Proposal!F17</f>
+      <c r="D18" s="136">
+        <f>Proposal!F12</f>
         <v>0</v>
       </c>
-      <c r="E18" s="135"/>
-      <c r="F18" s="135"/>
-      <c r="G18" s="135"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
-      <c r="J18" s="135"/>
-      <c r="K18" s="135"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="127"/>
-      <c r="O18" s="127"/>
-      <c r="P18" s="127"/>
-      <c r="Q18" s="127"/>
-      <c r="R18" s="127"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="136"/>
+      <c r="H18" s="136"/>
+      <c r="I18" s="136"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="136"/>
+      <c r="L18" s="125"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
+      <c r="O18" s="125"/>
+      <c r="P18" s="125"/>
+      <c r="Q18" s="125"/>
+      <c r="R18" s="125"/>
     </row>
     <row r="19" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="128"/>
-      <c r="K19" s="128"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="126"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="126"/>
+      <c r="K19" s="126"/>
       <c r="L19" s="75"/>
       <c r="M19" s="75"/>
       <c r="N19" s="75"/>
@@ -2598,35 +2592,35 @@
       <c r="C20" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="135">
-        <f>Proposal!F19</f>
+      <c r="D20" s="136">
+        <f>Proposal!F14</f>
         <v>0</v>
       </c>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
-      <c r="J20" s="135"/>
-      <c r="K20" s="135"/>
-      <c r="L20" s="127"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="127"/>
-      <c r="O20" s="127"/>
-      <c r="P20" s="127"/>
-      <c r="Q20" s="127"/>
-      <c r="R20" s="127"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="136"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="136"/>
+      <c r="L20" s="125"/>
+      <c r="M20" s="125"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="125"/>
+      <c r="Q20" s="125"/>
+      <c r="R20" s="125"/>
     </row>
     <row r="21" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="129"/>
-      <c r="H21" s="129"/>
-      <c r="I21" s="129"/>
-      <c r="J21" s="129"/>
-      <c r="K21" s="129"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="127"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="127"/>
       <c r="L21" s="117"/>
       <c r="M21" s="117"/>
       <c r="N21" s="117"/>
@@ -2639,32 +2633,32 @@
       <c r="C22" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="135"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="135"/>
-      <c r="G22" s="135"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="135"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="135"/>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127"/>
-      <c r="N22" s="127"/>
-      <c r="O22" s="127"/>
-      <c r="P22" s="127"/>
-      <c r="Q22" s="127"/>
-      <c r="R22" s="127"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="136"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="136"/>
+      <c r="K22" s="136"/>
+      <c r="L22" s="125"/>
+      <c r="M22" s="125"/>
+      <c r="N22" s="125"/>
+      <c r="O22" s="125"/>
+      <c r="P22" s="125"/>
+      <c r="Q22" s="125"/>
+      <c r="R22" s="125"/>
     </row>
     <row r="23" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
-      <c r="G23" s="129"/>
-      <c r="H23" s="129"/>
-      <c r="I23" s="129"/>
-      <c r="J23" s="129"/>
-      <c r="K23" s="129"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="127"/>
+      <c r="K23" s="127"/>
       <c r="L23" s="117"/>
       <c r="M23" s="117"/>
       <c r="N23" s="117"/>
@@ -2677,35 +2671,35 @@
       <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="135">
-        <f>Proposal!F23</f>
+      <c r="D24" s="136">
+        <f>Proposal!F18</f>
         <v>0</v>
       </c>
-      <c r="E24" s="135"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="135"/>
-      <c r="H24" s="135"/>
-      <c r="I24" s="135"/>
-      <c r="J24" s="135"/>
-      <c r="K24" s="135"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127"/>
-      <c r="P24" s="127"/>
-      <c r="Q24" s="127"/>
-      <c r="R24" s="127"/>
+      <c r="E24" s="136"/>
+      <c r="F24" s="136"/>
+      <c r="G24" s="136"/>
+      <c r="H24" s="136"/>
+      <c r="I24" s="136"/>
+      <c r="J24" s="136"/>
+      <c r="K24" s="136"/>
+      <c r="L24" s="125"/>
+      <c r="M24" s="125"/>
+      <c r="N24" s="125"/>
+      <c r="O24" s="125"/>
+      <c r="P24" s="125"/>
+      <c r="Q24" s="125"/>
+      <c r="R24" s="125"/>
     </row>
     <row r="25" spans="3:18" s="98" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
-      <c r="G25" s="129"/>
-      <c r="H25" s="129"/>
-      <c r="I25" s="129"/>
-      <c r="J25" s="129"/>
-      <c r="K25" s="129"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="127"/>
+      <c r="I25" s="127"/>
+      <c r="J25" s="127"/>
+      <c r="K25" s="127"/>
       <c r="L25" s="117"/>
       <c r="M25" s="117"/>
       <c r="N25" s="117"/>
@@ -2718,17 +2712,17 @@
       <c r="C26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="135">
-        <f>Proposal!F25</f>
+      <c r="D26" s="136">
+        <f>Proposal!F20</f>
         <v>0</v>
       </c>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
-      <c r="G26" s="135"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
-      <c r="K26" s="135"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136"/>
+      <c r="K26" s="136"/>
       <c r="L26" s="76"/>
       <c r="M26" s="76"/>
       <c r="N26" s="76"/>
@@ -2738,14 +2732,14 @@
       <c r="R26" s="76"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="134"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="134"/>
-      <c r="I27" s="134"/>
-      <c r="J27" s="134"/>
-      <c r="K27" s="134"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="135"/>
+      <c r="G27" s="135"/>
+      <c r="H27" s="135"/>
+      <c r="I27" s="135"/>
+      <c r="J27" s="135"/>
+      <c r="K27" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2849,22 +2843,22 @@
         <f>Proposal!N5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="133">
-        <f>Proposal!F19</f>
+      <c r="D5" s="134">
+        <f>Proposal!F14</f>
         <v>0</v>
       </c>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133"/>
-      <c r="N5" s="133"/>
-      <c r="O5" s="133"/>
-      <c r="P5" s="133"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
     </row>
     <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="59"/>
@@ -2872,19 +2866,19 @@
     <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="59"/>
       <c r="B7" s="52"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="137"/>
-      <c r="N7" s="137"/>
-      <c r="O7" s="138"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="138"/>
+      <c r="O7" s="139"/>
       <c r="P7" s="29"/>
     </row>
     <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3008,24 +3002,24 @@
       <c r="O13" s="71"/>
       <c r="P13" s="71"/>
     </row>
-    <row r="14" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="131" t="s">
+    <row r="14" spans="1:16" s="128" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="145"/>
-      <c r="D14" s="146"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="146"/>
-      <c r="G14" s="145"/>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="147"/>
-      <c r="K14" s="145"/>
-      <c r="L14" s="146"/>
-      <c r="M14" s="146"/>
-      <c r="N14" s="146"/>
-      <c r="O14" s="147"/>
-      <c r="P14" s="132"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="132"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="131"/>
+      <c r="L14" s="132"/>
+      <c r="M14" s="132"/>
+      <c r="N14" s="132"/>
+      <c r="O14" s="133"/>
+      <c r="P14" s="130"/>
     </row>
     <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P16" s="59"/>
@@ -3181,24 +3175,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="140" t="s">
+      <c r="G7" s="141" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="140"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="142"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="140" t="s">
+      <c r="N7" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="140"/>
-      <c r="P7" s="140"/>
-      <c r="Q7" s="140"/>
-      <c r="R7" s="140"/>
-      <c r="S7" s="140"/>
-      <c r="T7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="142"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3442,24 +3436,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="136" t="s">
+      <c r="G13" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
-      <c r="J13" s="137"/>
-      <c r="K13" s="137"/>
-      <c r="L13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="139"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="136" t="s">
+      <c r="N13" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="137"/>
-      <c r="P13" s="137"/>
-      <c r="Q13" s="137"/>
-      <c r="R13" s="137"/>
-      <c r="S13" s="137"/>
-      <c r="T13" s="138"/>
+      <c r="O13" s="138"/>
+      <c r="P13" s="138"/>
+      <c r="Q13" s="138"/>
+      <c r="R13" s="138"/>
+      <c r="S13" s="138"/>
+      <c r="T13" s="139"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -3699,24 +3693,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="136" t="s">
+      <c r="G19" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="137"/>
-      <c r="I19" s="137"/>
-      <c r="J19" s="137"/>
-      <c r="K19" s="137"/>
-      <c r="L19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="139"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="136" t="s">
+      <c r="N19" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="137"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="137"/>
-      <c r="R19" s="137"/>
-      <c r="S19" s="137"/>
-      <c r="T19" s="138"/>
+      <c r="O19" s="138"/>
+      <c r="P19" s="138"/>
+      <c r="Q19" s="138"/>
+      <c r="R19" s="138"/>
+      <c r="S19" s="138"/>
+      <c r="T19" s="139"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -3986,25 +3980,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="142" t="s">
+      <c r="D25" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="142"/>
-      <c r="F25" s="142"/>
-      <c r="G25" s="142"/>
-      <c r="H25" s="142"/>
-      <c r="I25" s="142"/>
-      <c r="J25" s="142"/>
-      <c r="K25" s="142"/>
-      <c r="L25" s="142"/>
-      <c r="M25" s="142"/>
-      <c r="N25" s="142"/>
-      <c r="O25" s="142"/>
-      <c r="P25" s="142"/>
-      <c r="Q25" s="142"/>
-      <c r="R25" s="142"/>
-      <c r="S25" s="142"/>
-      <c r="T25" s="142"/>
+      <c r="E25" s="143"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="143"/>
+      <c r="I25" s="143"/>
+      <c r="J25" s="143"/>
+      <c r="K25" s="143"/>
+      <c r="L25" s="143"/>
+      <c r="M25" s="143"/>
+      <c r="N25" s="143"/>
+      <c r="O25" s="143"/>
+      <c r="P25" s="143"/>
+      <c r="Q25" s="143"/>
+      <c r="R25" s="143"/>
+      <c r="S25" s="143"/>
+      <c r="T25" s="143"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -4030,25 +4024,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="142" t="s">
+      <c r="D27" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="142"/>
-      <c r="F27" s="142"/>
-      <c r="G27" s="142"/>
-      <c r="H27" s="142"/>
-      <c r="I27" s="142"/>
-      <c r="J27" s="142"/>
-      <c r="K27" s="142"/>
-      <c r="L27" s="142"/>
-      <c r="M27" s="142"/>
-      <c r="N27" s="142"/>
-      <c r="O27" s="142"/>
-      <c r="P27" s="142"/>
-      <c r="Q27" s="142"/>
-      <c r="R27" s="142"/>
-      <c r="S27" s="142"/>
-      <c r="T27" s="142"/>
+      <c r="E27" s="143"/>
+      <c r="F27" s="143"/>
+      <c r="G27" s="143"/>
+      <c r="H27" s="143"/>
+      <c r="I27" s="143"/>
+      <c r="J27" s="143"/>
+      <c r="K27" s="143"/>
+      <c r="L27" s="143"/>
+      <c r="M27" s="143"/>
+      <c r="N27" s="143"/>
+      <c r="O27" s="143"/>
+      <c r="P27" s="143"/>
+      <c r="Q27" s="143"/>
+      <c r="R27" s="143"/>
+      <c r="S27" s="143"/>
+      <c r="T27" s="143"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -4074,25 +4068,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="142" t="s">
+      <c r="D29" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="142"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="142"/>
-      <c r="H29" s="142"/>
-      <c r="I29" s="142"/>
-      <c r="J29" s="142"/>
-      <c r="K29" s="142"/>
-      <c r="L29" s="142"/>
-      <c r="M29" s="142"/>
-      <c r="N29" s="142"/>
-      <c r="O29" s="142"/>
-      <c r="P29" s="142"/>
-      <c r="Q29" s="142"/>
-      <c r="R29" s="142"/>
-      <c r="S29" s="142"/>
-      <c r="T29" s="142"/>
+      <c r="E29" s="143"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="143"/>
+      <c r="H29" s="143"/>
+      <c r="I29" s="143"/>
+      <c r="J29" s="143"/>
+      <c r="K29" s="143"/>
+      <c r="L29" s="143"/>
+      <c r="M29" s="143"/>
+      <c r="N29" s="143"/>
+      <c r="O29" s="143"/>
+      <c r="P29" s="143"/>
+      <c r="Q29" s="143"/>
+      <c r="R29" s="143"/>
+      <c r="S29" s="143"/>
+      <c r="T29" s="143"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -4118,25 +4112,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="142" t="s">
+      <c r="D31" s="143" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="142"/>
-      <c r="F31" s="142"/>
-      <c r="G31" s="142"/>
-      <c r="H31" s="142"/>
-      <c r="I31" s="142"/>
-      <c r="J31" s="142"/>
-      <c r="K31" s="142"/>
-      <c r="L31" s="142"/>
-      <c r="M31" s="142"/>
-      <c r="N31" s="142"/>
-      <c r="O31" s="142"/>
-      <c r="P31" s="142"/>
-      <c r="Q31" s="142"/>
-      <c r="R31" s="142"/>
-      <c r="S31" s="142"/>
-      <c r="T31" s="142"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="143"/>
+      <c r="G31" s="143"/>
+      <c r="H31" s="143"/>
+      <c r="I31" s="143"/>
+      <c r="J31" s="143"/>
+      <c r="K31" s="143"/>
+      <c r="L31" s="143"/>
+      <c r="M31" s="143"/>
+      <c r="N31" s="143"/>
+      <c r="O31" s="143"/>
+      <c r="P31" s="143"/>
+      <c r="Q31" s="143"/>
+      <c r="R31" s="143"/>
+      <c r="S31" s="143"/>
+      <c r="T31" s="143"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -4162,25 +4156,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="142" t="s">
+      <c r="D33" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="142"/>
-      <c r="F33" s="142"/>
-      <c r="G33" s="142"/>
-      <c r="H33" s="142"/>
-      <c r="I33" s="142"/>
-      <c r="J33" s="142"/>
-      <c r="K33" s="142"/>
-      <c r="L33" s="142"/>
-      <c r="M33" s="142"/>
-      <c r="N33" s="142"/>
-      <c r="O33" s="142"/>
-      <c r="P33" s="142"/>
-      <c r="Q33" s="142"/>
-      <c r="R33" s="142"/>
-      <c r="S33" s="142"/>
-      <c r="T33" s="142"/>
+      <c r="E33" s="143"/>
+      <c r="F33" s="143"/>
+      <c r="G33" s="143"/>
+      <c r="H33" s="143"/>
+      <c r="I33" s="143"/>
+      <c r="J33" s="143"/>
+      <c r="K33" s="143"/>
+      <c r="L33" s="143"/>
+      <c r="M33" s="143"/>
+      <c r="N33" s="143"/>
+      <c r="O33" s="143"/>
+      <c r="P33" s="143"/>
+      <c r="Q33" s="143"/>
+      <c r="R33" s="143"/>
+      <c r="S33" s="143"/>
+      <c r="T33" s="143"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4206,25 +4200,25 @@
       <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="139" t="s">
+      <c r="D35" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="139"/>
-      <c r="F35" s="139"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="139"/>
-      <c r="I35" s="139"/>
-      <c r="J35" s="139"/>
-      <c r="K35" s="139"/>
-      <c r="L35" s="139"/>
-      <c r="M35" s="139"/>
-      <c r="N35" s="139"/>
-      <c r="O35" s="139"/>
-      <c r="P35" s="139"/>
-      <c r="Q35" s="139"/>
-      <c r="R35" s="139"/>
-      <c r="S35" s="139"/>
-      <c r="T35" s="139"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="140"/>
+      <c r="I35" s="140"/>
+      <c r="J35" s="140"/>
+      <c r="K35" s="140"/>
+      <c r="L35" s="140"/>
+      <c r="M35" s="140"/>
+      <c r="N35" s="140"/>
+      <c r="O35" s="140"/>
+      <c r="P35" s="140"/>
+      <c r="Q35" s="140"/>
+      <c r="R35" s="140"/>
+      <c r="S35" s="140"/>
+      <c r="T35" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4366,24 +4360,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="140" t="s">
+      <c r="G7" s="141" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="140"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="142"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="140" t="s">
+      <c r="N7" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="140"/>
-      <c r="P7" s="140"/>
-      <c r="Q7" s="140"/>
-      <c r="R7" s="140"/>
-      <c r="S7" s="140"/>
-      <c r="T7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="142"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4625,24 +4619,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="136" t="s">
+      <c r="G13" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
-      <c r="J13" s="137"/>
-      <c r="K13" s="137"/>
-      <c r="L13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="139"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="136" t="s">
+      <c r="N13" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="137"/>
-      <c r="P13" s="137"/>
-      <c r="Q13" s="137"/>
-      <c r="R13" s="137"/>
-      <c r="S13" s="137"/>
-      <c r="T13" s="138"/>
+      <c r="O13" s="138"/>
+      <c r="P13" s="138"/>
+      <c r="Q13" s="138"/>
+      <c r="R13" s="138"/>
+      <c r="S13" s="138"/>
+      <c r="T13" s="139"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -4880,24 +4874,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="136" t="s">
+      <c r="G19" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="137"/>
-      <c r="I19" s="137"/>
-      <c r="J19" s="137"/>
-      <c r="K19" s="137"/>
-      <c r="L19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="139"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="136" t="s">
+      <c r="N19" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="137"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="137"/>
-      <c r="R19" s="137"/>
-      <c r="S19" s="137"/>
-      <c r="T19" s="138"/>
+      <c r="O19" s="138"/>
+      <c r="P19" s="138"/>
+      <c r="Q19" s="138"/>
+      <c r="R19" s="138"/>
+      <c r="S19" s="138"/>
+      <c r="T19" s="139"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -5135,24 +5129,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="136" t="s">
+      <c r="G25" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="137"/>
-      <c r="I25" s="137"/>
-      <c r="J25" s="137"/>
-      <c r="K25" s="137"/>
-      <c r="L25" s="138"/>
+      <c r="H25" s="138"/>
+      <c r="I25" s="138"/>
+      <c r="J25" s="138"/>
+      <c r="K25" s="138"/>
+      <c r="L25" s="139"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="136" t="s">
+      <c r="N25" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="137"/>
-      <c r="P25" s="137"/>
-      <c r="Q25" s="137"/>
-      <c r="R25" s="137"/>
-      <c r="S25" s="137"/>
-      <c r="T25" s="138"/>
+      <c r="O25" s="138"/>
+      <c r="P25" s="138"/>
+      <c r="Q25" s="138"/>
+      <c r="R25" s="138"/>
+      <c r="S25" s="138"/>
+      <c r="T25" s="139"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
@@ -5390,26 +5384,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="133" t="s">
+      <c r="C31" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="133"/>
-      <c r="E31" s="133"/>
-      <c r="F31" s="133"/>
-      <c r="G31" s="133"/>
-      <c r="H31" s="133"/>
-      <c r="I31" s="133"/>
-      <c r="J31" s="133"/>
-      <c r="K31" s="133"/>
-      <c r="L31" s="133"/>
-      <c r="M31" s="133"/>
-      <c r="N31" s="133"/>
-      <c r="O31" s="133"/>
-      <c r="P31" s="133"/>
-      <c r="Q31" s="133"/>
-      <c r="R31" s="133"/>
-      <c r="S31" s="133"/>
-      <c r="T31" s="133"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="134"/>
+      <c r="I31" s="134"/>
+      <c r="J31" s="134"/>
+      <c r="K31" s="134"/>
+      <c r="L31" s="134"/>
+      <c r="M31" s="134"/>
+      <c r="N31" s="134"/>
+      <c r="O31" s="134"/>
+      <c r="P31" s="134"/>
+      <c r="Q31" s="134"/>
+      <c r="R31" s="134"/>
+      <c r="S31" s="134"/>
+      <c r="T31" s="134"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5436,26 +5430,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="133" t="s">
+      <c r="C33" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
-      <c r="G33" s="133"/>
-      <c r="H33" s="133"/>
-      <c r="I33" s="133"/>
-      <c r="J33" s="133"/>
-      <c r="K33" s="133"/>
-      <c r="L33" s="133"/>
-      <c r="M33" s="133"/>
-      <c r="N33" s="133"/>
-      <c r="O33" s="133"/>
-      <c r="P33" s="133"/>
-      <c r="Q33" s="133"/>
-      <c r="R33" s="133"/>
-      <c r="S33" s="133"/>
-      <c r="T33" s="133"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="134"/>
+      <c r="I33" s="134"/>
+      <c r="J33" s="134"/>
+      <c r="K33" s="134"/>
+      <c r="L33" s="134"/>
+      <c r="M33" s="134"/>
+      <c r="N33" s="134"/>
+      <c r="O33" s="134"/>
+      <c r="P33" s="134"/>
+      <c r="Q33" s="134"/>
+      <c r="R33" s="134"/>
+      <c r="S33" s="134"/>
+      <c r="T33" s="134"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5482,26 +5476,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="133" t="s">
+      <c r="C35" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="133"/>
-      <c r="E35" s="133"/>
-      <c r="F35" s="133"/>
-      <c r="G35" s="133"/>
-      <c r="H35" s="133"/>
-      <c r="I35" s="133"/>
-      <c r="J35" s="133"/>
-      <c r="K35" s="133"/>
-      <c r="L35" s="133"/>
-      <c r="M35" s="133"/>
-      <c r="N35" s="133"/>
-      <c r="O35" s="133"/>
-      <c r="P35" s="133"/>
-      <c r="Q35" s="133"/>
-      <c r="R35" s="133"/>
-      <c r="S35" s="133"/>
-      <c r="T35" s="133"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="134"/>
+      <c r="F35" s="134"/>
+      <c r="G35" s="134"/>
+      <c r="H35" s="134"/>
+      <c r="I35" s="134"/>
+      <c r="J35" s="134"/>
+      <c r="K35" s="134"/>
+      <c r="L35" s="134"/>
+      <c r="M35" s="134"/>
+      <c r="N35" s="134"/>
+      <c r="O35" s="134"/>
+      <c r="P35" s="134"/>
+      <c r="Q35" s="134"/>
+      <c r="R35" s="134"/>
+      <c r="S35" s="134"/>
+      <c r="T35" s="134"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5528,26 +5522,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="133" t="s">
+      <c r="C37" s="134" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="133"/>
-      <c r="E37" s="133"/>
-      <c r="F37" s="133"/>
-      <c r="G37" s="133"/>
-      <c r="H37" s="133"/>
-      <c r="I37" s="133"/>
-      <c r="J37" s="133"/>
-      <c r="K37" s="133"/>
-      <c r="L37" s="133"/>
-      <c r="M37" s="133"/>
-      <c r="N37" s="133"/>
-      <c r="O37" s="133"/>
-      <c r="P37" s="133"/>
-      <c r="Q37" s="133"/>
-      <c r="R37" s="133"/>
-      <c r="S37" s="133"/>
-      <c r="T37" s="133"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="134"/>
+      <c r="F37" s="134"/>
+      <c r="G37" s="134"/>
+      <c r="H37" s="134"/>
+      <c r="I37" s="134"/>
+      <c r="J37" s="134"/>
+      <c r="K37" s="134"/>
+      <c r="L37" s="134"/>
+      <c r="M37" s="134"/>
+      <c r="N37" s="134"/>
+      <c r="O37" s="134"/>
+      <c r="P37" s="134"/>
+      <c r="Q37" s="134"/>
+      <c r="R37" s="134"/>
+      <c r="S37" s="134"/>
+      <c r="T37" s="134"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5574,26 +5568,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="133" t="s">
+      <c r="C39" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="133"/>
-      <c r="E39" s="133"/>
-      <c r="F39" s="133"/>
-      <c r="G39" s="133"/>
-      <c r="H39" s="133"/>
-      <c r="I39" s="133"/>
-      <c r="J39" s="133"/>
-      <c r="K39" s="133"/>
-      <c r="L39" s="133"/>
-      <c r="M39" s="133"/>
-      <c r="N39" s="133"/>
-      <c r="O39" s="133"/>
-      <c r="P39" s="133"/>
-      <c r="Q39" s="133"/>
-      <c r="R39" s="133"/>
-      <c r="S39" s="133"/>
-      <c r="T39" s="133"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="134"/>
+      <c r="G39" s="134"/>
+      <c r="H39" s="134"/>
+      <c r="I39" s="134"/>
+      <c r="J39" s="134"/>
+      <c r="K39" s="134"/>
+      <c r="L39" s="134"/>
+      <c r="M39" s="134"/>
+      <c r="N39" s="134"/>
+      <c r="O39" s="134"/>
+      <c r="P39" s="134"/>
+      <c r="Q39" s="134"/>
+      <c r="R39" s="134"/>
+      <c r="S39" s="134"/>
+      <c r="T39" s="134"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5620,34 +5614,29 @@
       <c r="B41" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="135" t="s">
+      <c r="C41" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="135"/>
-      <c r="E41" s="135"/>
-      <c r="F41" s="135"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
-      <c r="J41" s="135"/>
-      <c r="K41" s="135"/>
-      <c r="L41" s="135"/>
-      <c r="M41" s="135"/>
-      <c r="N41" s="135"/>
-      <c r="O41" s="135"/>
-      <c r="P41" s="135"/>
-      <c r="Q41" s="135"/>
-      <c r="R41" s="135"/>
-      <c r="S41" s="135"/>
-      <c r="T41" s="135"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
+      <c r="F41" s="136"/>
+      <c r="G41" s="136"/>
+      <c r="H41" s="136"/>
+      <c r="I41" s="136"/>
+      <c r="J41" s="136"/>
+      <c r="K41" s="136"/>
+      <c r="L41" s="136"/>
+      <c r="M41" s="136"/>
+      <c r="N41" s="136"/>
+      <c r="O41" s="136"/>
+      <c r="P41" s="136"/>
+      <c r="Q41" s="136"/>
+      <c r="R41" s="136"/>
+      <c r="S41" s="136"/>
+      <c r="T41" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5657,6 +5646,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5695,94 +5689,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="115" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="143"/>
+      <c r="D4" s="144"/>
     </row>
     <row r="5" spans="3:4" s="115" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="143" t="s">
+      <c r="C5" s="144" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="143"/>
+      <c r="D5" s="144"/>
     </row>
     <row r="6" spans="3:4" s="115" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="143" t="s">
+      <c r="C6" s="144" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="143"/>
+      <c r="D6" s="144"/>
     </row>
     <row r="7" spans="3:4" s="115" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="144" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="143"/>
+      <c r="D7" s="144"/>
     </row>
     <row r="8" spans="3:4" s="115" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="143"/>
+      <c r="D8" s="144"/>
     </row>
     <row r="9" spans="3:4" s="115" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="143" t="s">
+      <c r="C9" s="144" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="143"/>
+      <c r="D9" s="144"/>
     </row>
     <row r="10" spans="3:4" s="115" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="143"/>
+      <c r="D10" s="144"/>
     </row>
     <row r="11" spans="3:4" s="115" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="143" t="s">
+      <c r="C11" s="144" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="143"/>
+      <c r="D11" s="144"/>
     </row>
     <row r="12" spans="3:4" s="115" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="143" t="s">
+      <c r="C12" s="144" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="143"/>
+      <c r="D12" s="144"/>
     </row>
     <row r="13" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="143"/>
+      <c r="D13" s="144"/>
     </row>
     <row r="14" spans="3:4" s="115" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="143" t="s">
+      <c r="C14" s="144" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="143"/>
+      <c r="D14" s="144"/>
     </row>
     <row r="15" spans="3:4" s="115" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="143" t="s">
+      <c r="C15" s="144" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="143"/>
+      <c r="D15" s="144"/>
     </row>
     <row r="16" spans="3:4" s="115" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="144" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="143"/>
+      <c r="D16" s="144"/>
     </row>
     <row r="17" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="143" t="s">
+      <c r="C17" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="143"/>
+      <c r="D17" s="144"/>
     </row>
     <row r="18" spans="3:4" s="115" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="143" t="s">
+      <c r="C18" s="144" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="143"/>
+      <c r="D18" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5813,15 +5807,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="98" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" style="98" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3" style="98" customWidth="1"/>
     <col min="3" max="3" width="11.375" style="98" customWidth="1"/>
     <col min="4" max="4" width="9" style="98" customWidth="1"/>
@@ -5877,23 +5871,23 @@
       </c>
     </row>
     <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
       <c r="N5" s="75"/>
-      <c r="O5" s="133"/>
-      <c r="P5" s="133"/>
-      <c r="Q5" s="133"/>
-      <c r="R5" s="133"/>
-      <c r="S5" s="133"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
+      <c r="Q5" s="134"/>
+      <c r="R5" s="134"/>
+      <c r="S5" s="134"/>
     </row>
     <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H6" s="29"/>
@@ -5902,13 +5896,13 @@
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
     </row>
     <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="52"/>
@@ -5916,21 +5910,21 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="136" t="s">
+      <c r="H7" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="137"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="140"/>
-      <c r="O7" s="140"/>
-      <c r="P7" s="140"/>
-      <c r="Q7" s="140"/>
-      <c r="R7" s="140"/>
-      <c r="S7" s="140"/>
-      <c r="T7" s="141"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="139"/>
+      <c r="N7" s="137"/>
+      <c r="O7" s="138"/>
+      <c r="P7" s="138"/>
+      <c r="Q7" s="138"/>
+      <c r="R7" s="138"/>
+      <c r="S7" s="138"/>
+      <c r="T7" s="139"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98" t="s">
@@ -5993,10 +5987,6 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98" t="str">
-        <f>IF(OR($A8="Start",$A8="Even"),"Odd","Even")</f>
-        <v>Odd</v>
-      </c>
       <c r="B9" s="24"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -6009,7 +5999,7 @@
       <c r="K9" s="118"/>
       <c r="L9" s="123"/>
       <c r="M9" s="120"/>
-      <c r="N9" s="126"/>
+      <c r="N9" s="124"/>
       <c r="O9" s="121"/>
       <c r="P9" s="122"/>
       <c r="Q9" s="118"/>
@@ -6052,346 +6042,205 @@
       <c r="S10" s="46"/>
       <c r="T10" s="42"/>
     </row>
-    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="136" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="137"/>
-      <c r="J12" s="137"/>
-      <c r="K12" s="137"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="138"/>
-      <c r="N12" s="136"/>
-      <c r="O12" s="137"/>
-      <c r="P12" s="137"/>
-      <c r="Q12" s="137"/>
-      <c r="R12" s="137"/>
-      <c r="S12" s="137"/>
-      <c r="T12" s="138"/>
-    </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="38" t="s">
+    <row r="12" spans="1:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="54"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="145"/>
+      <c r="L12" s="145"/>
+      <c r="M12" s="145"/>
+      <c r="N12" s="145"/>
+      <c r="O12" s="145"/>
+      <c r="P12" s="145"/>
+      <c r="Q12" s="145"/>
+      <c r="R12" s="145"/>
+      <c r="S12" s="145"/>
+      <c r="T12" s="145"/>
+    </row>
+    <row r="13" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+    </row>
+    <row r="14" spans="1:20" s="116" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="R13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="S13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="T13" s="43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="98" t="str">
-        <f>IF(OR($A13="Start",$A13="Even"),"Odd","Even")</f>
-        <v>Odd</v>
-      </c>
-      <c r="C14" s="124"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="121"/>
-      <c r="I14" s="122"/>
-      <c r="J14" s="118"/>
-      <c r="K14" s="118"/>
-      <c r="L14" s="123"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="126"/>
-      <c r="O14" s="121"/>
-      <c r="P14" s="122"/>
-      <c r="Q14" s="118"/>
-      <c r="R14" s="118"/>
-      <c r="S14" s="123"/>
-      <c r="T14" s="120"/>
-    </row>
-    <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="38"/>
-      <c r="D15" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="79"/>
-      <c r="J15" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="50"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="O15" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="R15" s="50"/>
-      <c r="S15" s="46"/>
-      <c r="T15" s="42"/>
-    </row>
-    <row r="17" spans="3:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
-      <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
-      <c r="K17" s="144"/>
-      <c r="L17" s="144"/>
-      <c r="M17" s="144"/>
-      <c r="N17" s="144"/>
-      <c r="O17" s="144"/>
-      <c r="P17" s="144"/>
-      <c r="Q17" s="144"/>
-      <c r="R17" s="144"/>
-      <c r="S17" s="144"/>
-      <c r="T17" s="144"/>
-    </row>
-    <row r="18" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
-      <c r="T18" s="75"/>
-    </row>
-    <row r="19" spans="3:20" s="116" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="54"/>
-      <c r="F19" s="144"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="144"/>
-      <c r="J19" s="144"/>
-      <c r="K19" s="144"/>
-      <c r="L19" s="144"/>
-      <c r="M19" s="144"/>
-      <c r="N19" s="144"/>
-      <c r="O19" s="144"/>
-      <c r="P19" s="144"/>
-      <c r="Q19" s="144"/>
-      <c r="R19" s="144"/>
-      <c r="S19" s="144"/>
-      <c r="T19" s="144"/>
-    </row>
-    <row r="20" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="117"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="117"/>
-      <c r="P20" s="117"/>
-      <c r="Q20" s="117"/>
-      <c r="R20" s="117"/>
-      <c r="S20" s="117"/>
-      <c r="T20" s="117"/>
-    </row>
-    <row r="21" spans="3:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="54" t="s">
+      <c r="D14" s="54"/>
+      <c r="F14" s="145"/>
+      <c r="G14" s="145"/>
+      <c r="H14" s="145"/>
+      <c r="I14" s="145"/>
+      <c r="J14" s="145"/>
+      <c r="K14" s="145"/>
+      <c r="L14" s="145"/>
+      <c r="M14" s="145"/>
+      <c r="N14" s="145"/>
+      <c r="O14" s="145"/>
+      <c r="P14" s="145"/>
+      <c r="Q14" s="145"/>
+      <c r="R14" s="145"/>
+      <c r="S14" s="145"/>
+      <c r="T14" s="145"/>
+    </row>
+    <row r="15" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="117"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="117"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="117"/>
+      <c r="N15" s="117"/>
+      <c r="O15" s="117"/>
+      <c r="P15" s="117"/>
+      <c r="Q15" s="117"/>
+      <c r="R15" s="117"/>
+      <c r="S15" s="117"/>
+      <c r="T15" s="117"/>
+    </row>
+    <row r="16" spans="1:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="144"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="144"/>
-      <c r="K21" s="144"/>
-      <c r="L21" s="144"/>
-      <c r="M21" s="144"/>
-      <c r="N21" s="144"/>
-      <c r="O21" s="144"/>
-      <c r="P21" s="144"/>
-      <c r="Q21" s="144"/>
-      <c r="R21" s="144"/>
-      <c r="S21" s="144"/>
-      <c r="T21" s="144"/>
-    </row>
-    <row r="22" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="117"/>
-      <c r="L22" s="117"/>
-      <c r="M22" s="117"/>
-      <c r="N22" s="117"/>
-      <c r="O22" s="117"/>
-      <c r="P22" s="117"/>
-      <c r="Q22" s="117"/>
-      <c r="R22" s="117"/>
-      <c r="S22" s="117"/>
-      <c r="T22" s="117"/>
-    </row>
-    <row r="23" spans="3:20" s="116" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="54" t="s">
+      <c r="D16" s="54"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="145"/>
+      <c r="G16" s="145"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
+      <c r="K16" s="145"/>
+      <c r="L16" s="145"/>
+      <c r="M16" s="145"/>
+      <c r="N16" s="145"/>
+      <c r="O16" s="145"/>
+      <c r="P16" s="145"/>
+      <c r="Q16" s="145"/>
+      <c r="R16" s="145"/>
+      <c r="S16" s="145"/>
+      <c r="T16" s="145"/>
+    </row>
+    <row r="17" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="117"/>
+      <c r="O17" s="117"/>
+      <c r="P17" s="117"/>
+      <c r="Q17" s="117"/>
+      <c r="R17" s="117"/>
+      <c r="S17" s="117"/>
+      <c r="T17" s="117"/>
+    </row>
+    <row r="18" spans="3:20" s="116" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="144"/>
-      <c r="K23" s="144"/>
-      <c r="L23" s="144"/>
-      <c r="M23" s="144"/>
-      <c r="N23" s="144"/>
-      <c r="O23" s="144"/>
-      <c r="P23" s="144"/>
-      <c r="Q23" s="144"/>
-      <c r="R23" s="144"/>
-      <c r="S23" s="144"/>
-      <c r="T23" s="144"/>
-    </row>
-    <row r="24" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="117"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="117"/>
-      <c r="L24" s="117"/>
-      <c r="M24" s="117"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="117"/>
-      <c r="P24" s="117"/>
-      <c r="Q24" s="117"/>
-      <c r="R24" s="117"/>
-      <c r="S24" s="117"/>
-      <c r="T24" s="117"/>
-    </row>
-    <row r="25" spans="3:20" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="54" t="s">
+      <c r="D18" s="54"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="145"/>
+      <c r="L18" s="145"/>
+      <c r="M18" s="145"/>
+      <c r="N18" s="145"/>
+      <c r="O18" s="145"/>
+      <c r="P18" s="145"/>
+      <c r="Q18" s="145"/>
+      <c r="R18" s="145"/>
+      <c r="S18" s="145"/>
+      <c r="T18" s="145"/>
+    </row>
+    <row r="19" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="117"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="117"/>
+      <c r="O19" s="117"/>
+      <c r="P19" s="117"/>
+      <c r="Q19" s="117"/>
+      <c r="R19" s="117"/>
+      <c r="S19" s="117"/>
+      <c r="T19" s="117"/>
+    </row>
+    <row r="20" spans="3:20" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="54"/>
-      <c r="F25" s="135"/>
-      <c r="G25" s="135"/>
-      <c r="H25" s="135"/>
-      <c r="I25" s="135"/>
-      <c r="J25" s="135"/>
-      <c r="K25" s="135"/>
-      <c r="L25" s="135"/>
-      <c r="M25" s="135"/>
-      <c r="N25" s="135"/>
-      <c r="O25" s="135"/>
-      <c r="P25" s="135"/>
-      <c r="Q25" s="135"/>
-      <c r="R25" s="135"/>
-      <c r="S25" s="135"/>
-      <c r="T25" s="135"/>
+      <c r="D20" s="54"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="136"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="136"/>
+      <c r="L20" s="136"/>
+      <c r="M20" s="136"/>
+      <c r="N20" s="136"/>
+      <c r="O20" s="136"/>
+      <c r="P20" s="136"/>
+      <c r="Q20" s="136"/>
+      <c r="R20" s="136"/>
+      <c r="S20" s="136"/>
+      <c r="T20" s="136"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="F21:T21"/>
-    <mergeCell ref="F23:T23"/>
-    <mergeCell ref="F25:T25"/>
+  <mergeCells count="14">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F14:T14"/>
+    <mergeCell ref="F16:T16"/>
+    <mergeCell ref="F18:T18"/>
+    <mergeCell ref="F20:T20"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="Q5:S5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="N7:T7"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="N12:T12"/>
-    <mergeCell ref="F17:T17"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F19:T19"/>
+    <mergeCell ref="F12:T12"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:T3 C5 C4:N4 P4 R4:T4 T5 C6:T1048576">
     <cfRule type="expression" dxfId="9" priority="15">

</xml_diff>

<commit_message>
Merged PR 12875: BP-2740_(DP and Length) - Flow Chart of Campaign Export Daypart and Length Level
BP-2740_(DP and Length) - Flow Chart of Campaign Export Daypart and Length Level
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E91EEE2-103A-4DE2-B420-4E5455B83C81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4D778A-07C7-4A36-8CD3-E1719B608103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="465" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -21,17 +21,26 @@
     <sheet name="Proposal" sheetId="5" r:id="rId6"/>
     <sheet name="Flow Chart Template Tables" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="91">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -669,6 +678,9 @@
   </si>
   <si>
     <t>Receipt Acknowledged:</t>
+  </si>
+  <si>
+    <t>Total Monthly Cost</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1516,18 +1528,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1542,6 +1542,12 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
@@ -1579,8 +1585,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2234,7 +2273,7 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2302,11 +2341,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="138">
+      <c r="E5" s="136">
         <f>Proposal!H5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="138"/>
+      <c r="F5" s="136"/>
       <c r="G5" s="75">
         <f>Proposal!J5</f>
         <v>0</v>
@@ -2501,14 +2540,14 @@
       <c r="C18" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="140"/>
-      <c r="I18" s="140"/>
-      <c r="J18" s="140"/>
-      <c r="K18" s="140"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
       <c r="L18" s="125"/>
       <c r="M18" s="125"/>
       <c r="N18" s="125"/>
@@ -2539,14 +2578,14 @@
       <c r="C20" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="140"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="140"/>
-      <c r="J20" s="140"/>
-      <c r="K20" s="140"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="138"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="138"/>
       <c r="L20" s="125"/>
       <c r="M20" s="125"/>
       <c r="N20" s="125"/>
@@ -2577,14 +2616,14 @@
       <c r="C22" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140"/>
-      <c r="H22" s="140"/>
-      <c r="I22" s="140"/>
-      <c r="J22" s="140"/>
-      <c r="K22" s="140"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="138"/>
       <c r="L22" s="125"/>
       <c r="M22" s="125"/>
       <c r="N22" s="125"/>
@@ -2615,14 +2654,14 @@
       <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140"/>
-      <c r="H24" s="140"/>
-      <c r="I24" s="140"/>
-      <c r="J24" s="140"/>
-      <c r="K24" s="140"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="138"/>
+      <c r="K24" s="138"/>
       <c r="L24" s="125"/>
       <c r="M24" s="125"/>
       <c r="N24" s="125"/>
@@ -2653,14 +2692,14 @@
       <c r="C26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="140"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="138"/>
+      <c r="K26" s="138"/>
       <c r="L26" s="76"/>
       <c r="M26" s="76"/>
       <c r="N26" s="76"/>
@@ -2670,14 +2709,14 @@
       <c r="R26" s="76"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="139"/>
-      <c r="E27" s="139"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="139"/>
-      <c r="H27" s="139"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="139"/>
-      <c r="K27" s="139"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2780,19 +2819,19 @@
         <f>Proposal!N5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="138"/>
-      <c r="L5" s="138"/>
-      <c r="M5" s="138"/>
-      <c r="N5" s="138"/>
-      <c r="O5" s="138"/>
-      <c r="P5" s="138"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="136"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="59"/>
@@ -2945,24 +2984,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="145" t="s">
+      <c r="G7" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
-      <c r="K7" s="145"/>
-      <c r="L7" s="146"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="143"/>
+      <c r="K7" s="143"/>
+      <c r="L7" s="144"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="145" t="s">
+      <c r="N7" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="145"/>
-      <c r="P7" s="145"/>
-      <c r="Q7" s="145"/>
-      <c r="R7" s="145"/>
-      <c r="S7" s="145"/>
-      <c r="T7" s="146"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
+      <c r="T7" s="144"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3206,24 +3245,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="142" t="s">
+      <c r="G13" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="143"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="144"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
+      <c r="J13" s="141"/>
+      <c r="K13" s="141"/>
+      <c r="L13" s="142"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="142" t="s">
+      <c r="N13" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="143"/>
-      <c r="P13" s="143"/>
-      <c r="Q13" s="143"/>
-      <c r="R13" s="143"/>
-      <c r="S13" s="143"/>
-      <c r="T13" s="144"/>
+      <c r="O13" s="141"/>
+      <c r="P13" s="141"/>
+      <c r="Q13" s="141"/>
+      <c r="R13" s="141"/>
+      <c r="S13" s="141"/>
+      <c r="T13" s="142"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -3463,24 +3502,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="142" t="s">
+      <c r="G19" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="144"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
+      <c r="J19" s="141"/>
+      <c r="K19" s="141"/>
+      <c r="L19" s="142"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="142" t="s">
+      <c r="N19" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="143"/>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="143"/>
-      <c r="R19" s="143"/>
-      <c r="S19" s="143"/>
-      <c r="T19" s="144"/>
+      <c r="O19" s="141"/>
+      <c r="P19" s="141"/>
+      <c r="Q19" s="141"/>
+      <c r="R19" s="141"/>
+      <c r="S19" s="141"/>
+      <c r="T19" s="142"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -3750,25 +3789,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="147" t="s">
+      <c r="D25" s="145" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="147"/>
-      <c r="F25" s="147"/>
-      <c r="G25" s="147"/>
-      <c r="H25" s="147"/>
-      <c r="I25" s="147"/>
-      <c r="J25" s="147"/>
-      <c r="K25" s="147"/>
-      <c r="L25" s="147"/>
-      <c r="M25" s="147"/>
-      <c r="N25" s="147"/>
-      <c r="O25" s="147"/>
-      <c r="P25" s="147"/>
-      <c r="Q25" s="147"/>
-      <c r="R25" s="147"/>
-      <c r="S25" s="147"/>
-      <c r="T25" s="147"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="145"/>
+      <c r="L25" s="145"/>
+      <c r="M25" s="145"/>
+      <c r="N25" s="145"/>
+      <c r="O25" s="145"/>
+      <c r="P25" s="145"/>
+      <c r="Q25" s="145"/>
+      <c r="R25" s="145"/>
+      <c r="S25" s="145"/>
+      <c r="T25" s="145"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3794,25 +3833,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="147" t="s">
+      <c r="D27" s="145" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="147"/>
-      <c r="J27" s="147"/>
-      <c r="K27" s="147"/>
-      <c r="L27" s="147"/>
-      <c r="M27" s="147"/>
-      <c r="N27" s="147"/>
-      <c r="O27" s="147"/>
-      <c r="P27" s="147"/>
-      <c r="Q27" s="147"/>
-      <c r="R27" s="147"/>
-      <c r="S27" s="147"/>
-      <c r="T27" s="147"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="145"/>
+      <c r="L27" s="145"/>
+      <c r="M27" s="145"/>
+      <c r="N27" s="145"/>
+      <c r="O27" s="145"/>
+      <c r="P27" s="145"/>
+      <c r="Q27" s="145"/>
+      <c r="R27" s="145"/>
+      <c r="S27" s="145"/>
+      <c r="T27" s="145"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3838,25 +3877,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="147" t="s">
+      <c r="D29" s="145" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="147"/>
-      <c r="J29" s="147"/>
-      <c r="K29" s="147"/>
-      <c r="L29" s="147"/>
-      <c r="M29" s="147"/>
-      <c r="N29" s="147"/>
-      <c r="O29" s="147"/>
-      <c r="P29" s="147"/>
-      <c r="Q29" s="147"/>
-      <c r="R29" s="147"/>
-      <c r="S29" s="147"/>
-      <c r="T29" s="147"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
+      <c r="K29" s="145"/>
+      <c r="L29" s="145"/>
+      <c r="M29" s="145"/>
+      <c r="N29" s="145"/>
+      <c r="O29" s="145"/>
+      <c r="P29" s="145"/>
+      <c r="Q29" s="145"/>
+      <c r="R29" s="145"/>
+      <c r="S29" s="145"/>
+      <c r="T29" s="145"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -3882,25 +3921,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="147" t="s">
+      <c r="D31" s="145" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="147"/>
-      <c r="F31" s="147"/>
-      <c r="G31" s="147"/>
-      <c r="H31" s="147"/>
-      <c r="I31" s="147"/>
-      <c r="J31" s="147"/>
-      <c r="K31" s="147"/>
-      <c r="L31" s="147"/>
-      <c r="M31" s="147"/>
-      <c r="N31" s="147"/>
-      <c r="O31" s="147"/>
-      <c r="P31" s="147"/>
-      <c r="Q31" s="147"/>
-      <c r="R31" s="147"/>
-      <c r="S31" s="147"/>
-      <c r="T31" s="147"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="145"/>
+      <c r="H31" s="145"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="145"/>
+      <c r="K31" s="145"/>
+      <c r="L31" s="145"/>
+      <c r="M31" s="145"/>
+      <c r="N31" s="145"/>
+      <c r="O31" s="145"/>
+      <c r="P31" s="145"/>
+      <c r="Q31" s="145"/>
+      <c r="R31" s="145"/>
+      <c r="S31" s="145"/>
+      <c r="T31" s="145"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -3926,25 +3965,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="147" t="s">
+      <c r="D33" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="147"/>
-      <c r="F33" s="147"/>
-      <c r="G33" s="147"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="147"/>
-      <c r="J33" s="147"/>
-      <c r="K33" s="147"/>
-      <c r="L33" s="147"/>
-      <c r="M33" s="147"/>
-      <c r="N33" s="147"/>
-      <c r="O33" s="147"/>
-      <c r="P33" s="147"/>
-      <c r="Q33" s="147"/>
-      <c r="R33" s="147"/>
-      <c r="S33" s="147"/>
-      <c r="T33" s="147"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="145"/>
+      <c r="I33" s="145"/>
+      <c r="J33" s="145"/>
+      <c r="K33" s="145"/>
+      <c r="L33" s="145"/>
+      <c r="M33" s="145"/>
+      <c r="N33" s="145"/>
+      <c r="O33" s="145"/>
+      <c r="P33" s="145"/>
+      <c r="Q33" s="145"/>
+      <c r="R33" s="145"/>
+      <c r="S33" s="145"/>
+      <c r="T33" s="145"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -3970,25 +4009,25 @@
       <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="141" t="s">
+      <c r="D35" s="139" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="141"/>
-      <c r="F35" s="141"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
-      <c r="J35" s="141"/>
-      <c r="K35" s="141"/>
-      <c r="L35" s="141"/>
-      <c r="M35" s="141"/>
-      <c r="N35" s="141"/>
-      <c r="O35" s="141"/>
-      <c r="P35" s="141"/>
-      <c r="Q35" s="141"/>
-      <c r="R35" s="141"/>
-      <c r="S35" s="141"/>
-      <c r="T35" s="141"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="139"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="139"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="139"/>
+      <c r="K35" s="139"/>
+      <c r="L35" s="139"/>
+      <c r="M35" s="139"/>
+      <c r="N35" s="139"/>
+      <c r="O35" s="139"/>
+      <c r="P35" s="139"/>
+      <c r="Q35" s="139"/>
+      <c r="R35" s="139"/>
+      <c r="S35" s="139"/>
+      <c r="T35" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4130,24 +4169,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="145" t="s">
+      <c r="G7" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
-      <c r="K7" s="145"/>
-      <c r="L7" s="146"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="143"/>
+      <c r="K7" s="143"/>
+      <c r="L7" s="144"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="145" t="s">
+      <c r="N7" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="145"/>
-      <c r="P7" s="145"/>
-      <c r="Q7" s="145"/>
-      <c r="R7" s="145"/>
-      <c r="S7" s="145"/>
-      <c r="T7" s="146"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
+      <c r="T7" s="144"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4389,24 +4428,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="142" t="s">
+      <c r="G13" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="143"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="144"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
+      <c r="J13" s="141"/>
+      <c r="K13" s="141"/>
+      <c r="L13" s="142"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="142" t="s">
+      <c r="N13" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="143"/>
-      <c r="P13" s="143"/>
-      <c r="Q13" s="143"/>
-      <c r="R13" s="143"/>
-      <c r="S13" s="143"/>
-      <c r="T13" s="144"/>
+      <c r="O13" s="141"/>
+      <c r="P13" s="141"/>
+      <c r="Q13" s="141"/>
+      <c r="R13" s="141"/>
+      <c r="S13" s="141"/>
+      <c r="T13" s="142"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -4644,24 +4683,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="142" t="s">
+      <c r="G19" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="144"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
+      <c r="J19" s="141"/>
+      <c r="K19" s="141"/>
+      <c r="L19" s="142"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="142" t="s">
+      <c r="N19" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="143"/>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="143"/>
-      <c r="R19" s="143"/>
-      <c r="S19" s="143"/>
-      <c r="T19" s="144"/>
+      <c r="O19" s="141"/>
+      <c r="P19" s="141"/>
+      <c r="Q19" s="141"/>
+      <c r="R19" s="141"/>
+      <c r="S19" s="141"/>
+      <c r="T19" s="142"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -4899,24 +4938,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="142" t="s">
+      <c r="G25" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="143"/>
-      <c r="I25" s="143"/>
-      <c r="J25" s="143"/>
-      <c r="K25" s="143"/>
-      <c r="L25" s="144"/>
+      <c r="H25" s="141"/>
+      <c r="I25" s="141"/>
+      <c r="J25" s="141"/>
+      <c r="K25" s="141"/>
+      <c r="L25" s="142"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="142" t="s">
+      <c r="N25" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="143"/>
-      <c r="P25" s="143"/>
-      <c r="Q25" s="143"/>
-      <c r="R25" s="143"/>
-      <c r="S25" s="143"/>
-      <c r="T25" s="144"/>
+      <c r="O25" s="141"/>
+      <c r="P25" s="141"/>
+      <c r="Q25" s="141"/>
+      <c r="R25" s="141"/>
+      <c r="S25" s="141"/>
+      <c r="T25" s="142"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
@@ -5154,26 +5193,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="138" t="s">
+      <c r="C31" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="138"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="138"/>
-      <c r="J31" s="138"/>
-      <c r="K31" s="138"/>
-      <c r="L31" s="138"/>
-      <c r="M31" s="138"/>
-      <c r="N31" s="138"/>
-      <c r="O31" s="138"/>
-      <c r="P31" s="138"/>
-      <c r="Q31" s="138"/>
-      <c r="R31" s="138"/>
-      <c r="S31" s="138"/>
-      <c r="T31" s="138"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="136"/>
+      <c r="I31" s="136"/>
+      <c r="J31" s="136"/>
+      <c r="K31" s="136"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="136"/>
+      <c r="N31" s="136"/>
+      <c r="O31" s="136"/>
+      <c r="P31" s="136"/>
+      <c r="Q31" s="136"/>
+      <c r="R31" s="136"/>
+      <c r="S31" s="136"/>
+      <c r="T31" s="136"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5200,26 +5239,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="138" t="s">
+      <c r="C33" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="138"/>
-      <c r="E33" s="138"/>
-      <c r="F33" s="138"/>
-      <c r="G33" s="138"/>
-      <c r="H33" s="138"/>
-      <c r="I33" s="138"/>
-      <c r="J33" s="138"/>
-      <c r="K33" s="138"/>
-      <c r="L33" s="138"/>
-      <c r="M33" s="138"/>
-      <c r="N33" s="138"/>
-      <c r="O33" s="138"/>
-      <c r="P33" s="138"/>
-      <c r="Q33" s="138"/>
-      <c r="R33" s="138"/>
-      <c r="S33" s="138"/>
-      <c r="T33" s="138"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="136"/>
+      <c r="G33" s="136"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="136"/>
+      <c r="J33" s="136"/>
+      <c r="K33" s="136"/>
+      <c r="L33" s="136"/>
+      <c r="M33" s="136"/>
+      <c r="N33" s="136"/>
+      <c r="O33" s="136"/>
+      <c r="P33" s="136"/>
+      <c r="Q33" s="136"/>
+      <c r="R33" s="136"/>
+      <c r="S33" s="136"/>
+      <c r="T33" s="136"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5246,26 +5285,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="138" t="s">
+      <c r="C35" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="138"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="138"/>
-      <c r="I35" s="138"/>
-      <c r="J35" s="138"/>
-      <c r="K35" s="138"/>
-      <c r="L35" s="138"/>
-      <c r="M35" s="138"/>
-      <c r="N35" s="138"/>
-      <c r="O35" s="138"/>
-      <c r="P35" s="138"/>
-      <c r="Q35" s="138"/>
-      <c r="R35" s="138"/>
-      <c r="S35" s="138"/>
-      <c r="T35" s="138"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="136"/>
+      <c r="F35" s="136"/>
+      <c r="G35" s="136"/>
+      <c r="H35" s="136"/>
+      <c r="I35" s="136"/>
+      <c r="J35" s="136"/>
+      <c r="K35" s="136"/>
+      <c r="L35" s="136"/>
+      <c r="M35" s="136"/>
+      <c r="N35" s="136"/>
+      <c r="O35" s="136"/>
+      <c r="P35" s="136"/>
+      <c r="Q35" s="136"/>
+      <c r="R35" s="136"/>
+      <c r="S35" s="136"/>
+      <c r="T35" s="136"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5292,26 +5331,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="138" t="s">
+      <c r="C37" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="138"/>
-      <c r="E37" s="138"/>
-      <c r="F37" s="138"/>
-      <c r="G37" s="138"/>
-      <c r="H37" s="138"/>
-      <c r="I37" s="138"/>
-      <c r="J37" s="138"/>
-      <c r="K37" s="138"/>
-      <c r="L37" s="138"/>
-      <c r="M37" s="138"/>
-      <c r="N37" s="138"/>
-      <c r="O37" s="138"/>
-      <c r="P37" s="138"/>
-      <c r="Q37" s="138"/>
-      <c r="R37" s="138"/>
-      <c r="S37" s="138"/>
-      <c r="T37" s="138"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="136"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="136"/>
+      <c r="H37" s="136"/>
+      <c r="I37" s="136"/>
+      <c r="J37" s="136"/>
+      <c r="K37" s="136"/>
+      <c r="L37" s="136"/>
+      <c r="M37" s="136"/>
+      <c r="N37" s="136"/>
+      <c r="O37" s="136"/>
+      <c r="P37" s="136"/>
+      <c r="Q37" s="136"/>
+      <c r="R37" s="136"/>
+      <c r="S37" s="136"/>
+      <c r="T37" s="136"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5338,26 +5377,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="138" t="s">
+      <c r="C39" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="138"/>
-      <c r="E39" s="138"/>
-      <c r="F39" s="138"/>
-      <c r="G39" s="138"/>
-      <c r="H39" s="138"/>
-      <c r="I39" s="138"/>
-      <c r="J39" s="138"/>
-      <c r="K39" s="138"/>
-      <c r="L39" s="138"/>
-      <c r="M39" s="138"/>
-      <c r="N39" s="138"/>
-      <c r="O39" s="138"/>
-      <c r="P39" s="138"/>
-      <c r="Q39" s="138"/>
-      <c r="R39" s="138"/>
-      <c r="S39" s="138"/>
-      <c r="T39" s="138"/>
+      <c r="D39" s="136"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="136"/>
+      <c r="G39" s="136"/>
+      <c r="H39" s="136"/>
+      <c r="I39" s="136"/>
+      <c r="J39" s="136"/>
+      <c r="K39" s="136"/>
+      <c r="L39" s="136"/>
+      <c r="M39" s="136"/>
+      <c r="N39" s="136"/>
+      <c r="O39" s="136"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="136"/>
+      <c r="R39" s="136"/>
+      <c r="S39" s="136"/>
+      <c r="T39" s="136"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5384,29 +5423,34 @@
       <c r="B41" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="140" t="s">
+      <c r="C41" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="140"/>
-      <c r="E41" s="140"/>
-      <c r="F41" s="140"/>
-      <c r="G41" s="140"/>
-      <c r="H41" s="140"/>
-      <c r="I41" s="140"/>
-      <c r="J41" s="140"/>
-      <c r="K41" s="140"/>
-      <c r="L41" s="140"/>
-      <c r="M41" s="140"/>
-      <c r="N41" s="140"/>
-      <c r="O41" s="140"/>
-      <c r="P41" s="140"/>
-      <c r="Q41" s="140"/>
-      <c r="R41" s="140"/>
-      <c r="S41" s="140"/>
-      <c r="T41" s="140"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138"/>
+      <c r="G41" s="138"/>
+      <c r="H41" s="138"/>
+      <c r="I41" s="138"/>
+      <c r="J41" s="138"/>
+      <c r="K41" s="138"/>
+      <c r="L41" s="138"/>
+      <c r="M41" s="138"/>
+      <c r="N41" s="138"/>
+      <c r="O41" s="138"/>
+      <c r="P41" s="138"/>
+      <c r="Q41" s="138"/>
+      <c r="R41" s="138"/>
+      <c r="S41" s="138"/>
+      <c r="T41" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5416,11 +5460,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5459,94 +5498,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="115" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="146" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="148"/>
+      <c r="D4" s="146"/>
     </row>
     <row r="5" spans="3:4" s="115" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="148"/>
+      <c r="D5" s="146"/>
     </row>
     <row r="6" spans="3:4" s="115" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="148"/>
+      <c r="D6" s="146"/>
     </row>
     <row r="7" spans="3:4" s="115" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="146" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="148"/>
+      <c r="D7" s="146"/>
     </row>
     <row r="8" spans="3:4" s="115" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="148" t="s">
+      <c r="C8" s="146" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="148"/>
+      <c r="D8" s="146"/>
     </row>
     <row r="9" spans="3:4" s="115" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="148" t="s">
+      <c r="C9" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="148"/>
+      <c r="D9" s="146"/>
     </row>
     <row r="10" spans="3:4" s="115" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="148" t="s">
+      <c r="C10" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="148"/>
+      <c r="D10" s="146"/>
     </row>
     <row r="11" spans="3:4" s="115" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="148" t="s">
+      <c r="C11" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="148"/>
+      <c r="D11" s="146"/>
     </row>
     <row r="12" spans="3:4" s="115" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="148" t="s">
+      <c r="C12" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="148"/>
+      <c r="D12" s="146"/>
     </row>
     <row r="13" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="148" t="s">
+      <c r="C13" s="146" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="148"/>
+      <c r="D13" s="146"/>
     </row>
     <row r="14" spans="3:4" s="115" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="148" t="s">
+      <c r="C14" s="146" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="148"/>
+      <c r="D14" s="146"/>
     </row>
     <row r="15" spans="3:4" s="115" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="148" t="s">
+      <c r="C15" s="146" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="148"/>
+      <c r="D15" s="146"/>
     </row>
     <row r="16" spans="3:4" s="115" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="148" t="s">
+      <c r="C16" s="146" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="148"/>
+      <c r="D16" s="146"/>
     </row>
     <row r="17" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="148" t="s">
+      <c r="C17" s="146" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="148"/>
+      <c r="D17" s="146"/>
     </row>
     <row r="18" spans="3:4" s="115" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="148" t="s">
+      <c r="C18" s="146" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="148"/>
+      <c r="D18" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5641,23 +5680,23 @@
       </c>
     </row>
     <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="138"/>
-      <c r="L5" s="138"/>
-      <c r="M5" s="138"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="136"/>
       <c r="N5" s="75"/>
-      <c r="O5" s="138"/>
-      <c r="P5" s="138"/>
-      <c r="Q5" s="138"/>
-      <c r="R5" s="138"/>
-      <c r="S5" s="138"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
+      <c r="Q5" s="136"/>
+      <c r="R5" s="136"/>
+      <c r="S5" s="136"/>
     </row>
     <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H6" s="29"/>
@@ -5680,21 +5719,21 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="142" t="s">
+      <c r="H7" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="144"/>
-      <c r="N7" s="142"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
-      <c r="T7" s="144"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="142"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98" t="s">
@@ -5818,21 +5857,21 @@
       </c>
       <c r="D12" s="54"/>
       <c r="E12" s="116"/>
-      <c r="F12" s="149"/>
-      <c r="G12" s="149"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="149"/>
-      <c r="L12" s="149"/>
-      <c r="M12" s="149"/>
-      <c r="N12" s="149"/>
-      <c r="O12" s="149"/>
-      <c r="P12" s="149"/>
-      <c r="Q12" s="149"/>
-      <c r="R12" s="149"/>
-      <c r="S12" s="149"/>
-      <c r="T12" s="149"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="147"/>
+      <c r="K12" s="147"/>
+      <c r="L12" s="147"/>
+      <c r="M12" s="147"/>
+      <c r="N12" s="147"/>
+      <c r="O12" s="147"/>
+      <c r="P12" s="147"/>
+      <c r="Q12" s="147"/>
+      <c r="R12" s="147"/>
+      <c r="S12" s="147"/>
+      <c r="T12" s="147"/>
     </row>
     <row r="13" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
@@ -5858,21 +5897,21 @@
         <v>36</v>
       </c>
       <c r="D14" s="54"/>
-      <c r="F14" s="149"/>
-      <c r="G14" s="149"/>
-      <c r="H14" s="149"/>
-      <c r="I14" s="149"/>
-      <c r="J14" s="149"/>
-      <c r="K14" s="149"/>
-      <c r="L14" s="149"/>
-      <c r="M14" s="149"/>
-      <c r="N14" s="149"/>
-      <c r="O14" s="149"/>
-      <c r="P14" s="149"/>
-      <c r="Q14" s="149"/>
-      <c r="R14" s="149"/>
-      <c r="S14" s="149"/>
-      <c r="T14" s="149"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
+      <c r="H14" s="147"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="147"/>
+      <c r="K14" s="147"/>
+      <c r="L14" s="147"/>
+      <c r="M14" s="147"/>
+      <c r="N14" s="147"/>
+      <c r="O14" s="147"/>
+      <c r="P14" s="147"/>
+      <c r="Q14" s="147"/>
+      <c r="R14" s="147"/>
+      <c r="S14" s="147"/>
+      <c r="T14" s="147"/>
     </row>
     <row r="15" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -5899,21 +5938,21 @@
       </c>
       <c r="D16" s="54"/>
       <c r="E16" s="116"/>
-      <c r="F16" s="149"/>
-      <c r="G16" s="149"/>
-      <c r="H16" s="149"/>
-      <c r="I16" s="149"/>
-      <c r="J16" s="149"/>
-      <c r="K16" s="149"/>
-      <c r="L16" s="149"/>
-      <c r="M16" s="149"/>
-      <c r="N16" s="149"/>
-      <c r="O16" s="149"/>
-      <c r="P16" s="149"/>
-      <c r="Q16" s="149"/>
-      <c r="R16" s="149"/>
-      <c r="S16" s="149"/>
-      <c r="T16" s="149"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="147"/>
+      <c r="H16" s="147"/>
+      <c r="I16" s="147"/>
+      <c r="J16" s="147"/>
+      <c r="K16" s="147"/>
+      <c r="L16" s="147"/>
+      <c r="M16" s="147"/>
+      <c r="N16" s="147"/>
+      <c r="O16" s="147"/>
+      <c r="P16" s="147"/>
+      <c r="Q16" s="147"/>
+      <c r="R16" s="147"/>
+      <c r="S16" s="147"/>
+      <c r="T16" s="147"/>
     </row>
     <row r="17" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -5939,21 +5978,21 @@
         <v>48</v>
       </c>
       <c r="D18" s="54"/>
-      <c r="F18" s="149"/>
-      <c r="G18" s="149"/>
-      <c r="H18" s="149"/>
-      <c r="I18" s="149"/>
-      <c r="J18" s="149"/>
-      <c r="K18" s="149"/>
-      <c r="L18" s="149"/>
-      <c r="M18" s="149"/>
-      <c r="N18" s="149"/>
-      <c r="O18" s="149"/>
-      <c r="P18" s="149"/>
-      <c r="Q18" s="149"/>
-      <c r="R18" s="149"/>
-      <c r="S18" s="149"/>
-      <c r="T18" s="149"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="147"/>
+      <c r="H18" s="147"/>
+      <c r="I18" s="147"/>
+      <c r="J18" s="147"/>
+      <c r="K18" s="147"/>
+      <c r="L18" s="147"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="147"/>
+      <c r="O18" s="147"/>
+      <c r="P18" s="147"/>
+      <c r="Q18" s="147"/>
+      <c r="R18" s="147"/>
+      <c r="S18" s="147"/>
+      <c r="T18" s="147"/>
     </row>
     <row r="19" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
@@ -5979,29 +6018,24 @@
         <v>49</v>
       </c>
       <c r="D20" s="54"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="140"/>
-      <c r="J20" s="140"/>
-      <c r="K20" s="140"/>
-      <c r="L20" s="140"/>
-      <c r="M20" s="140"/>
-      <c r="N20" s="140"/>
-      <c r="O20" s="140"/>
-      <c r="P20" s="140"/>
-      <c r="Q20" s="140"/>
-      <c r="R20" s="140"/>
-      <c r="S20" s="140"/>
-      <c r="T20" s="140"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="138"/>
+      <c r="L20" s="138"/>
+      <c r="M20" s="138"/>
+      <c r="N20" s="138"/>
+      <c r="O20" s="138"/>
+      <c r="P20" s="138"/>
+      <c r="Q20" s="138"/>
+      <c r="R20" s="138"/>
+      <c r="S20" s="138"/>
+      <c r="T20" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F14:T14"/>
     <mergeCell ref="F16:T16"/>
     <mergeCell ref="F18:T18"/>
     <mergeCell ref="F20:T20"/>
@@ -6011,6 +6045,11 @@
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="N7:T7"/>
     <mergeCell ref="F12:T12"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F14:T14"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:T3 C5 C4:N4 P4 R4:T4 T5 C6:T1048576">
     <cfRule type="expression" dxfId="0" priority="15">
@@ -6028,24 +6067,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="133" customWidth="1"/>
-    <col min="2" max="2" width="23.125" style="133" customWidth="1"/>
-    <col min="3" max="5" width="12.125" style="133" customWidth="1"/>
+    <col min="1" max="1" width="3" style="129" customWidth="1"/>
+    <col min="2" max="2" width="23.125" style="129" customWidth="1"/>
+    <col min="3" max="5" width="12.125" style="129" customWidth="1"/>
     <col min="6" max="6" width="12.125" style="7" customWidth="1"/>
-    <col min="7" max="9" width="12.125" style="133" customWidth="1"/>
+    <col min="7" max="9" width="12.125" style="129" customWidth="1"/>
     <col min="10" max="10" width="12.125" style="7" customWidth="1"/>
-    <col min="11" max="13" width="12.125" style="133" customWidth="1"/>
+    <col min="11" max="13" width="12.125" style="129" customWidth="1"/>
     <col min="14" max="15" width="12.125" style="7" customWidth="1"/>
-    <col min="16" max="17" width="11.875" style="133" customWidth="1"/>
-    <col min="18" max="16384" width="10.625" style="133"/>
+    <col min="16" max="17" width="11.875" style="129" customWidth="1"/>
+    <col min="18" max="16384" width="10.625" style="129"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6053,19 +6092,19 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
-      <c r="B2" s="150"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="144"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="142"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6125,7 +6164,7 @@
       <c r="L5" s="36"/>
       <c r="M5" s="36"/>
       <c r="N5" s="36"/>
-      <c r="O5" s="134"/>
+      <c r="O5" s="130"/>
     </row>
     <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
@@ -6144,7 +6183,7 @@
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
-      <c r="O6" s="135"/>
+      <c r="O6" s="131"/>
     </row>
     <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
@@ -6163,7 +6202,7 @@
       <c r="L7" s="37"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
-      <c r="O7" s="136"/>
+      <c r="O7" s="132"/>
     </row>
     <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="60" t="s">
@@ -6181,988 +6220,1144 @@
       <c r="L8" s="70"/>
       <c r="M8" s="70"/>
       <c r="N8" s="70"/>
-      <c r="O8" s="137"/>
-    </row>
-    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="133"/>
+    </row>
+    <row r="9" spans="1:16" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="130"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="131"/>
-      <c r="J9" s="132"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="131"/>
-      <c r="N9" s="131"/>
-      <c r="O9" s="129"/>
-    </row>
-    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="150"/>
-      <c r="C11" s="142"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="143"/>
-      <c r="F11" s="143"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="144"/>
-      <c r="L11" s="142"/>
-      <c r="M11" s="143"/>
-      <c r="N11" s="143"/>
-      <c r="O11" s="144"/>
-      <c r="P11" s="29"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="133"/>
+    </row>
+    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="152"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="153"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="152"/>
+      <c r="H10" s="153"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="152"/>
+      <c r="L10" s="153"/>
+      <c r="M10" s="153"/>
+      <c r="N10" s="154"/>
+      <c r="O10" s="151"/>
     </row>
     <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="74"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="67" t="s">
+      <c r="B12" s="135"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="141"/>
+      <c r="K12" s="142"/>
+      <c r="L12" s="140"/>
+      <c r="M12" s="141"/>
+      <c r="N12" s="141"/>
+      <c r="O12" s="142"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="74"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="61" t="s">
+    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="68" t="s">
+      <c r="C14" s="62"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="68" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
     </row>
     <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
+        <v>19</v>
+      </c>
+      <c r="C15" s="66"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
     </row>
     <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="72"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
+        <v>24</v>
+      </c>
+      <c r="C16" s="65"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
     </row>
     <row r="17" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="72"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+    </row>
+    <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
-    </row>
-    <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="128" t="s">
+      <c r="C18" s="69"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="71"/>
+    </row>
+    <row r="19" spans="2:16" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="130"/>
-      <c r="D18" s="131"/>
-      <c r="E18" s="131"/>
-      <c r="F18" s="131"/>
-      <c r="G18" s="131"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="131"/>
-      <c r="J18" s="131"/>
-      <c r="K18" s="132"/>
-      <c r="L18" s="130"/>
-      <c r="M18" s="131"/>
-      <c r="N18" s="131"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="129"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="71"/>
+      <c r="P19" s="71"/>
     </row>
     <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="150"/>
-      <c r="C20" s="142"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="144"/>
-      <c r="L20" s="142"/>
-      <c r="M20" s="143"/>
-      <c r="N20" s="143"/>
-      <c r="O20" s="144"/>
-      <c r="P20" s="29"/>
-    </row>
-    <row r="21" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="74"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="67" t="s">
+      <c r="B20" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="157"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="159"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="153"/>
+      <c r="K20" s="154"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="153"/>
+      <c r="O20" s="154"/>
+      <c r="P20" s="155"/>
+    </row>
+    <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="135"/>
+      <c r="C22" s="140"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="142"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="141"/>
+      <c r="I22" s="141"/>
+      <c r="J22" s="141"/>
+      <c r="K22" s="142"/>
+      <c r="L22" s="140"/>
+      <c r="M22" s="141"/>
+      <c r="N22" s="141"/>
+      <c r="O22" s="142"/>
+      <c r="P22" s="29"/>
+    </row>
+    <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="74"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="61" t="s">
+    <row r="24" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="63"/>
-      <c r="N22" s="63"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="68" t="s">
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="68" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="58"/>
-    </row>
-    <row r="24" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
     </row>
     <row r="25" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
+        <v>19</v>
+      </c>
+      <c r="C25" s="66"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
     </row>
     <row r="26" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="65"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+    </row>
+    <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="72"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+    </row>
+    <row r="28" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70"/>
-      <c r="O26" s="71"/>
-      <c r="P26" s="71"/>
-    </row>
-    <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="128" t="s">
+      <c r="C28" s="69"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+    </row>
+    <row r="29" spans="2:16" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="130"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="130"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="131"/>
-      <c r="K27" s="132"/>
-      <c r="L27" s="130"/>
-      <c r="M27" s="131"/>
-      <c r="N27" s="131"/>
-      <c r="O27" s="132"/>
-      <c r="P27" s="129"/>
-    </row>
-    <row r="29" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="150"/>
-      <c r="C29" s="142"/>
-      <c r="D29" s="143"/>
-      <c r="E29" s="143"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="144"/>
-      <c r="K29" s="142"/>
-      <c r="L29" s="143"/>
-      <c r="M29" s="143"/>
-      <c r="N29" s="143"/>
-      <c r="O29" s="144"/>
-      <c r="P29" s="29"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="71"/>
     </row>
     <row r="30" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="74"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="67" t="s">
+      <c r="B30" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="152"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="153"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="153"/>
+      <c r="I30" s="153"/>
+      <c r="J30" s="153"/>
+      <c r="K30" s="154"/>
+      <c r="L30" s="152"/>
+      <c r="M30" s="153"/>
+      <c r="N30" s="153"/>
+      <c r="O30" s="154"/>
+      <c r="P30" s="155"/>
+    </row>
+    <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="135"/>
+      <c r="C32" s="140"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="141"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="141"/>
+      <c r="H32" s="141"/>
+      <c r="I32" s="141"/>
+      <c r="J32" s="142"/>
+      <c r="K32" s="140"/>
+      <c r="L32" s="141"/>
+      <c r="M32" s="141"/>
+      <c r="N32" s="141"/>
+      <c r="O32" s="142"/>
+      <c r="P32" s="29"/>
+    </row>
+    <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="74"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="61" t="s">
+    <row r="34" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="68" t="s">
+      <c r="C34" s="62"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="68" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-    </row>
-    <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="57"/>
-      <c r="P33" s="57"/>
-    </row>
-    <row r="34" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
     </row>
     <row r="35" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="66"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+    </row>
+    <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="65"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+    </row>
+    <row r="37" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="72"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+    </row>
+    <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="70"/>
-      <c r="N35" s="70"/>
-      <c r="O35" s="71"/>
-      <c r="P35" s="71"/>
-    </row>
-    <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="128" t="s">
+      <c r="C38" s="69"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
+      <c r="N38" s="70"/>
+      <c r="O38" s="71"/>
+      <c r="P38" s="71"/>
+    </row>
+    <row r="39" spans="2:17" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="130"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="131"/>
-      <c r="F36" s="131"/>
-      <c r="G36" s="130"/>
-      <c r="H36" s="131"/>
-      <c r="I36" s="131"/>
-      <c r="J36" s="132"/>
-      <c r="K36" s="130"/>
-      <c r="L36" s="131"/>
-      <c r="M36" s="131"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="132"/>
-      <c r="P36" s="129"/>
-    </row>
-    <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="150"/>
-      <c r="C38" s="142"/>
-      <c r="D38" s="143"/>
-      <c r="E38" s="143"/>
-      <c r="F38" s="143"/>
-      <c r="G38" s="144"/>
-      <c r="H38" s="143"/>
-      <c r="I38" s="143"/>
-      <c r="J38" s="143"/>
-      <c r="K38" s="143"/>
-      <c r="L38" s="144"/>
-      <c r="M38" s="142"/>
-      <c r="N38" s="143"/>
-      <c r="O38" s="143"/>
-      <c r="P38" s="144"/>
-      <c r="Q38" s="29"/>
-    </row>
-    <row r="39" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="74"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="55"/>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="55"/>
-      <c r="Q39" s="67" t="s">
+      <c r="C39" s="69"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="70"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="71"/>
+    </row>
+    <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="152"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="154"/>
+      <c r="G40" s="152"/>
+      <c r="H40" s="153"/>
+      <c r="I40" s="153"/>
+      <c r="J40" s="154"/>
+      <c r="K40" s="152"/>
+      <c r="L40" s="153"/>
+      <c r="M40" s="153"/>
+      <c r="N40" s="153"/>
+      <c r="O40" s="154"/>
+      <c r="P40" s="155"/>
+    </row>
+    <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="135"/>
+      <c r="C42" s="140"/>
+      <c r="D42" s="141"/>
+      <c r="E42" s="141"/>
+      <c r="F42" s="141"/>
+      <c r="G42" s="142"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
+      <c r="J42" s="141"/>
+      <c r="K42" s="141"/>
+      <c r="L42" s="142"/>
+      <c r="M42" s="140"/>
+      <c r="N42" s="141"/>
+      <c r="O42" s="141"/>
+      <c r="P42" s="142"/>
+      <c r="Q42" s="29"/>
+    </row>
+    <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="74"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="55"/>
+      <c r="O43" s="55"/>
+      <c r="P43" s="55"/>
+      <c r="Q43" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="61" t="s">
+    <row r="44" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="63"/>
-      <c r="K40" s="63"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="63"/>
-      <c r="O40" s="63"/>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="68" t="s">
+      <c r="C44" s="62"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="64"/>
+      <c r="Q44" s="68" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+    <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="66"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="58"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="58"/>
-      <c r="Q41" s="58"/>
-    </row>
-    <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="60" t="s">
+      <c r="C45" s="66"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="66"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="58"/>
+    </row>
+    <row r="46" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="57"/>
-      <c r="M42" s="65"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="35"/>
-      <c r="P42" s="57"/>
-      <c r="Q42" s="57"/>
-    </row>
-    <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="60" t="s">
+      <c r="C46" s="65"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="65"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="57"/>
+    </row>
+    <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="73"/>
-      <c r="M43" s="72"/>
-      <c r="N43" s="37"/>
-      <c r="O43" s="37"/>
-      <c r="P43" s="73"/>
-      <c r="Q43" s="73"/>
-    </row>
-    <row r="44" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="60" t="s">
+      <c r="C47" s="72"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="73"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="73"/>
+      <c r="M47" s="72"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="73"/>
+      <c r="Q47" s="73"/>
+    </row>
+    <row r="48" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="70"/>
-      <c r="J44" s="70"/>
-      <c r="K44" s="70"/>
-      <c r="L44" s="71"/>
-      <c r="M44" s="69"/>
-      <c r="N44" s="70"/>
-      <c r="O44" s="70"/>
-      <c r="P44" s="71"/>
-      <c r="Q44" s="71"/>
-    </row>
-    <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="128" t="s">
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
+      <c r="K48" s="70"/>
+      <c r="L48" s="71"/>
+      <c r="M48" s="69"/>
+      <c r="N48" s="70"/>
+      <c r="O48" s="70"/>
+      <c r="P48" s="71"/>
+      <c r="Q48" s="71"/>
+    </row>
+    <row r="49" spans="2:17" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="130"/>
-      <c r="D45" s="131"/>
-      <c r="E45" s="131"/>
-      <c r="F45" s="131"/>
-      <c r="G45" s="131"/>
-      <c r="H45" s="130"/>
-      <c r="I45" s="131"/>
-      <c r="J45" s="131"/>
-      <c r="K45" s="131"/>
-      <c r="L45" s="132"/>
-      <c r="M45" s="130"/>
-      <c r="N45" s="131"/>
-      <c r="O45" s="131"/>
-      <c r="P45" s="132"/>
-      <c r="Q45" s="129"/>
-    </row>
-    <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="150"/>
-      <c r="C47" s="142"/>
-      <c r="D47" s="143"/>
-      <c r="E47" s="143"/>
-      <c r="F47" s="143"/>
-      <c r="G47" s="144"/>
-      <c r="H47" s="143"/>
-      <c r="I47" s="143"/>
-      <c r="J47" s="143"/>
-      <c r="K47" s="144"/>
-      <c r="L47" s="142"/>
-      <c r="M47" s="143"/>
-      <c r="N47" s="143"/>
-      <c r="O47" s="143"/>
-      <c r="P47" s="144"/>
-      <c r="Q47" s="29"/>
-    </row>
-    <row r="48" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="74"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="55"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="67" t="s">
+      <c r="C49" s="69"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="70"/>
+      <c r="F49" s="70"/>
+      <c r="G49" s="70"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="70"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="70"/>
+      <c r="O49" s="70"/>
+      <c r="P49" s="71"/>
+      <c r="Q49" s="71"/>
+    </row>
+    <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="152"/>
+      <c r="D50" s="153"/>
+      <c r="E50" s="153"/>
+      <c r="F50" s="153"/>
+      <c r="G50" s="154"/>
+      <c r="H50" s="152"/>
+      <c r="I50" s="153"/>
+      <c r="J50" s="153"/>
+      <c r="K50" s="153"/>
+      <c r="L50" s="154"/>
+      <c r="M50" s="152"/>
+      <c r="N50" s="153"/>
+      <c r="O50" s="153"/>
+      <c r="P50" s="154"/>
+      <c r="Q50" s="155"/>
+    </row>
+    <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="135"/>
+      <c r="C52" s="140"/>
+      <c r="D52" s="141"/>
+      <c r="E52" s="141"/>
+      <c r="F52" s="141"/>
+      <c r="G52" s="142"/>
+      <c r="H52" s="141"/>
+      <c r="I52" s="141"/>
+      <c r="J52" s="141"/>
+      <c r="K52" s="142"/>
+      <c r="L52" s="140"/>
+      <c r="M52" s="141"/>
+      <c r="N52" s="141"/>
+      <c r="O52" s="141"/>
+      <c r="P52" s="142"/>
+      <c r="Q52" s="29"/>
+    </row>
+    <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="74"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="55"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55"/>
+      <c r="O53" s="55"/>
+      <c r="P53" s="55"/>
+      <c r="Q53" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="61" t="s">
+    <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="62"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="63"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="62"/>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-      <c r="O49" s="63"/>
-      <c r="P49" s="64"/>
-      <c r="Q49" s="68" t="s">
+      <c r="C54" s="62"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="64"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="64"/>
+      <c r="L54" s="62"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="63"/>
+      <c r="O54" s="63"/>
+      <c r="P54" s="64"/>
+      <c r="Q54" s="68" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="60" t="s">
+    <row r="55" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="66"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="36"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="66"/>
-      <c r="M50" s="36"/>
-      <c r="N50" s="36"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="58"/>
-      <c r="Q50" s="58"/>
-    </row>
-    <row r="51" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="60" t="s">
+      <c r="C55" s="66"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="58"/>
+      <c r="L55" s="66"/>
+      <c r="M55" s="36"/>
+      <c r="N55" s="36"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+    </row>
+    <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C51" s="65"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="65"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="65"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
-      <c r="O51" s="35"/>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="57"/>
-    </row>
-    <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="60" t="s">
+      <c r="C56" s="65"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="57"/>
+      <c r="L56" s="65"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="35"/>
+      <c r="P56" s="57"/>
+      <c r="Q56" s="57"/>
+    </row>
+    <row r="57" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="73"/>
-      <c r="L52" s="72"/>
-      <c r="M52" s="37"/>
-      <c r="N52" s="37"/>
-      <c r="O52" s="37"/>
-      <c r="P52" s="73"/>
-      <c r="Q52" s="73"/>
-    </row>
-    <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="60" t="s">
+      <c r="C57" s="72"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="73"/>
+      <c r="L57" s="72"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="37"/>
+      <c r="O57" s="37"/>
+      <c r="P57" s="73"/>
+      <c r="Q57" s="73"/>
+    </row>
+    <row r="58" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="69"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="71"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="70"/>
-      <c r="J53" s="70"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="69"/>
-      <c r="M53" s="70"/>
-      <c r="N53" s="70"/>
-      <c r="O53" s="70"/>
-      <c r="P53" s="71"/>
-      <c r="Q53" s="71"/>
-    </row>
-    <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="128" t="s">
+      <c r="C58" s="69"/>
+      <c r="D58" s="70"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="71"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="70"/>
+      <c r="K58" s="71"/>
+      <c r="L58" s="69"/>
+      <c r="M58" s="70"/>
+      <c r="N58" s="70"/>
+      <c r="O58" s="70"/>
+      <c r="P58" s="71"/>
+      <c r="Q58" s="71"/>
+    </row>
+    <row r="59" spans="2:17" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="130"/>
-      <c r="D54" s="131"/>
-      <c r="E54" s="131"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="130"/>
-      <c r="I54" s="131"/>
-      <c r="J54" s="131"/>
-      <c r="K54" s="132"/>
-      <c r="L54" s="130"/>
-      <c r="M54" s="131"/>
-      <c r="N54" s="131"/>
-      <c r="O54" s="131"/>
-      <c r="P54" s="132"/>
-      <c r="Q54" s="129"/>
-    </row>
-    <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="150"/>
-      <c r="C56" s="142"/>
-      <c r="D56" s="143"/>
-      <c r="E56" s="143"/>
-      <c r="F56" s="144"/>
-      <c r="G56" s="143"/>
-      <c r="H56" s="143"/>
-      <c r="I56" s="143"/>
-      <c r="J56" s="143"/>
-      <c r="K56" s="144"/>
-      <c r="L56" s="142"/>
-      <c r="M56" s="143"/>
-      <c r="N56" s="143"/>
-      <c r="O56" s="143"/>
-      <c r="P56" s="144"/>
-      <c r="Q56" s="29"/>
-    </row>
-    <row r="57" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="74"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="56"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="55"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="55"/>
-      <c r="P57" s="55"/>
-      <c r="Q57" s="67" t="s">
+      <c r="C59" s="69"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="70"/>
+      <c r="K59" s="71"/>
+      <c r="L59" s="69"/>
+      <c r="M59" s="70"/>
+      <c r="N59" s="70"/>
+      <c r="O59" s="70"/>
+      <c r="P59" s="71"/>
+      <c r="Q59" s="71"/>
+    </row>
+    <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="148"/>
+      <c r="D60" s="149"/>
+      <c r="E60" s="149"/>
+      <c r="F60" s="149"/>
+      <c r="G60" s="150"/>
+      <c r="H60" s="148"/>
+      <c r="I60" s="149"/>
+      <c r="J60" s="149"/>
+      <c r="K60" s="150"/>
+      <c r="L60" s="148"/>
+      <c r="M60" s="149"/>
+      <c r="N60" s="149"/>
+      <c r="O60" s="149"/>
+      <c r="P60" s="150"/>
+      <c r="Q60" s="156"/>
+    </row>
+    <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="135"/>
+      <c r="C62" s="140"/>
+      <c r="D62" s="141"/>
+      <c r="E62" s="141"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="141"/>
+      <c r="H62" s="141"/>
+      <c r="I62" s="141"/>
+      <c r="J62" s="141"/>
+      <c r="K62" s="142"/>
+      <c r="L62" s="140"/>
+      <c r="M62" s="141"/>
+      <c r="N62" s="141"/>
+      <c r="O62" s="141"/>
+      <c r="P62" s="142"/>
+      <c r="Q62" s="29"/>
+    </row>
+    <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="74"/>
+      <c r="C63" s="55"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
+      <c r="I63" s="55"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="56"/>
+      <c r="L63" s="55"/>
+      <c r="M63" s="55"/>
+      <c r="N63" s="55"/>
+      <c r="O63" s="55"/>
+      <c r="P63" s="55"/>
+      <c r="Q63" s="67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="61" t="s">
+    <row r="64" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="62"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="63"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="62"/>
-      <c r="H58" s="63"/>
-      <c r="I58" s="63"/>
-      <c r="J58" s="63"/>
-      <c r="K58" s="64"/>
-      <c r="L58" s="62"/>
-      <c r="M58" s="63"/>
-      <c r="N58" s="63"/>
-      <c r="O58" s="63"/>
-      <c r="P58" s="64"/>
-      <c r="Q58" s="68" t="s">
+      <c r="C64" s="62"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+      <c r="J64" s="63"/>
+      <c r="K64" s="64"/>
+      <c r="L64" s="62"/>
+      <c r="M64" s="63"/>
+      <c r="N64" s="63"/>
+      <c r="O64" s="63"/>
+      <c r="P64" s="64"/>
+      <c r="Q64" s="68" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="60" t="s">
+    <row r="65" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="66"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="66"/>
-      <c r="M59" s="36"/>
-      <c r="N59" s="36"/>
-      <c r="O59" s="36"/>
-      <c r="P59" s="58"/>
-      <c r="Q59" s="58"/>
-    </row>
-    <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="60" t="s">
+      <c r="C65" s="66"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="58"/>
+      <c r="G65" s="66"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="36"/>
+      <c r="J65" s="36"/>
+      <c r="K65" s="58"/>
+      <c r="L65" s="66"/>
+      <c r="M65" s="36"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="36"/>
+      <c r="P65" s="58"/>
+      <c r="Q65" s="58"/>
+    </row>
+    <row r="66" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="65"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="65"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="65"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="57"/>
-    </row>
-    <row r="61" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="60" t="s">
+      <c r="C66" s="65"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="65"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="57"/>
+      <c r="L66" s="65"/>
+      <c r="M66" s="35"/>
+      <c r="N66" s="35"/>
+      <c r="O66" s="35"/>
+      <c r="P66" s="57"/>
+      <c r="Q66" s="57"/>
+    </row>
+    <row r="67" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="73"/>
-      <c r="G61" s="72"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="73"/>
-      <c r="L61" s="72"/>
-      <c r="M61" s="37"/>
-      <c r="N61" s="37"/>
-      <c r="O61" s="37"/>
-      <c r="P61" s="73"/>
-      <c r="Q61" s="73"/>
-    </row>
-    <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="60" t="s">
+      <c r="C67" s="72"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="73"/>
+      <c r="G67" s="72"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="73"/>
+      <c r="L67" s="72"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="73"/>
+      <c r="Q67" s="73"/>
+    </row>
+    <row r="68" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="69"/>
-      <c r="D62" s="70"/>
-      <c r="E62" s="70"/>
-      <c r="F62" s="71"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="70"/>
-      <c r="I62" s="70"/>
-      <c r="J62" s="70"/>
-      <c r="K62" s="71"/>
-      <c r="L62" s="69"/>
-      <c r="M62" s="70"/>
-      <c r="N62" s="70"/>
-      <c r="O62" s="70"/>
-      <c r="P62" s="71"/>
-      <c r="Q62" s="71"/>
-    </row>
-    <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="128" t="s">
+      <c r="C68" s="69"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="70"/>
+      <c r="F68" s="71"/>
+      <c r="G68" s="69"/>
+      <c r="H68" s="70"/>
+      <c r="I68" s="70"/>
+      <c r="J68" s="70"/>
+      <c r="K68" s="71"/>
+      <c r="L68" s="69"/>
+      <c r="M68" s="70"/>
+      <c r="N68" s="70"/>
+      <c r="O68" s="70"/>
+      <c r="P68" s="71"/>
+      <c r="Q68" s="71"/>
+    </row>
+    <row r="69" spans="2:17" s="134" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="130"/>
-      <c r="D63" s="131"/>
-      <c r="E63" s="131"/>
-      <c r="F63" s="131"/>
-      <c r="G63" s="130"/>
-      <c r="H63" s="131"/>
-      <c r="I63" s="131"/>
-      <c r="J63" s="131"/>
-      <c r="K63" s="132"/>
-      <c r="L63" s="130"/>
-      <c r="M63" s="131"/>
-      <c r="N63" s="131"/>
-      <c r="O63" s="131"/>
-      <c r="P63" s="132"/>
-      <c r="Q63" s="129"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="70"/>
+      <c r="F69" s="70"/>
+      <c r="G69" s="69"/>
+      <c r="H69" s="70"/>
+      <c r="I69" s="70"/>
+      <c r="J69" s="70"/>
+      <c r="K69" s="71"/>
+      <c r="L69" s="69"/>
+      <c r="M69" s="70"/>
+      <c r="N69" s="70"/>
+      <c r="O69" s="70"/>
+      <c r="P69" s="71"/>
+      <c r="Q69" s="71"/>
+    </row>
+    <row r="70" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" s="152"/>
+      <c r="D70" s="153"/>
+      <c r="E70" s="153"/>
+      <c r="F70" s="154"/>
+      <c r="G70" s="152"/>
+      <c r="H70" s="153"/>
+      <c r="I70" s="153"/>
+      <c r="J70" s="153"/>
+      <c r="K70" s="154"/>
+      <c r="L70" s="152"/>
+      <c r="M70" s="153"/>
+      <c r="N70" s="153"/>
+      <c r="O70" s="153"/>
+      <c r="P70" s="154"/>
+      <c r="Q70" s="155"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="42">
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="L70:P70"/>
+    <mergeCell ref="L60:P60"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:O40"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
+    <mergeCell ref="C60:G60"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
     <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="G56:K56"/>
-    <mergeCell ref="L56:P56"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="L47:P47"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{1A174315-2F56-4C74-8CF2-D4F4F4F25C91}"/>
+    <dataValidation allowBlank="1" sqref="L20 L30 L70 K10 K40 M50 C20 H20 C10 G10 C30 G30 C40 G40 C50 H50 C60 C70 H60 G70 L60" xr:uid="{1A174315-2F56-4C74-8CF2-D4F4F4F25C91}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Merged PR 15392: BP-4427-Contract Export needs to display fluidity percentage allowed on Contract and proposal tab
Contract Export needs to display fluidity percentage allowed on Contract and proposal tab
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF019884-A1F1-410F-BCDF-FEC85E9DC5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F93F6D2-03E2-4774-B73D-6C1695672F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="92">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>Total Monthly Cost</t>
+  </si>
+  <si>
+    <t>Fluidity</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1552,6 +1555,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1594,18 +1618,6 @@
     <xf numFmtId="164" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1623,12 +1635,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2282,8 +2288,8 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2293,8 +2299,13 @@
     <col min="3" max="4" width="24.875" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.875" style="3" customWidth="1"/>
     <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
-    <col min="7" max="12" width="24.875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="2.375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.25" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16.5" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.25" style="3" customWidth="1"/>
     <col min="14" max="20" width="10.875" style="3" customWidth="1"/>
     <col min="21" max="21" width="3" style="3" customWidth="1"/>
     <col min="22" max="16384" width="10.625" style="3"/>
@@ -2332,12 +2343,15 @@
         <v>68</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2350,11 +2364,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="136">
+      <c r="E5" s="143">
         <f>Proposal!H5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="136"/>
+      <c r="F5" s="143"/>
       <c r="G5" s="75">
         <f>Proposal!J5</f>
         <v>0</v>
@@ -2372,11 +2386,15 @@
         <v>0</v>
       </c>
       <c r="K5" s="75">
+        <f>Proposal!P5</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="75">
         <f>Proposal!Q5</f>
         <v>0</v>
       </c>
-      <c r="L5" s="75">
-        <f>Proposal!T5</f>
+      <c r="M5" s="2">
+        <f>Proposal!S5</f>
         <v>0</v>
       </c>
     </row>
@@ -2549,14 +2567,14 @@
       <c r="C18" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="138"/>
-      <c r="I18" s="138"/>
-      <c r="J18" s="138"/>
-      <c r="K18" s="138"/>
+      <c r="D18" s="145"/>
+      <c r="E18" s="145"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="145"/>
       <c r="L18" s="125"/>
       <c r="M18" s="125"/>
       <c r="N18" s="125"/>
@@ -2587,14 +2605,14 @@
       <c r="C20" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="138"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="138"/>
-      <c r="K20" s="138"/>
+      <c r="D20" s="145"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="145"/>
       <c r="L20" s="125"/>
       <c r="M20" s="125"/>
       <c r="N20" s="125"/>
@@ -2625,14 +2643,14 @@
       <c r="C22" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="138"/>
-      <c r="J22" s="138"/>
-      <c r="K22" s="138"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="145"/>
+      <c r="K22" s="145"/>
       <c r="L22" s="125"/>
       <c r="M22" s="125"/>
       <c r="N22" s="125"/>
@@ -2663,14 +2681,14 @@
       <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
-      <c r="H24" s="138"/>
-      <c r="I24" s="138"/>
-      <c r="J24" s="138"/>
-      <c r="K24" s="138"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="145"/>
+      <c r="K24" s="145"/>
       <c r="L24" s="125"/>
       <c r="M24" s="125"/>
       <c r="N24" s="125"/>
@@ -2701,14 +2719,14 @@
       <c r="C26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="138"/>
-      <c r="J26" s="138"/>
-      <c r="K26" s="138"/>
+      <c r="D26" s="145"/>
+      <c r="E26" s="145"/>
+      <c r="F26" s="145"/>
+      <c r="G26" s="145"/>
+      <c r="H26" s="145"/>
+      <c r="I26" s="145"/>
+      <c r="J26" s="145"/>
+      <c r="K26" s="145"/>
       <c r="L26" s="76"/>
       <c r="M26" s="76"/>
       <c r="N26" s="76"/>
@@ -2718,14 +2736,14 @@
       <c r="R26" s="76"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="137"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="137"/>
-      <c r="G27" s="137"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="137"/>
-      <c r="J27" s="137"/>
-      <c r="K27" s="137"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="144"/>
+      <c r="F27" s="144"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="144"/>
+      <c r="I27" s="144"/>
+      <c r="J27" s="144"/>
+      <c r="K27" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2828,19 +2846,19 @@
         <f>Proposal!N5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="136"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="136"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
+      <c r="N5" s="143"/>
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="59"/>
@@ -2993,24 +3011,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="143" t="s">
+      <c r="G7" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="144"/>
+      <c r="H7" s="150"/>
+      <c r="I7" s="150"/>
+      <c r="J7" s="150"/>
+      <c r="K7" s="150"/>
+      <c r="L7" s="151"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="143" t="s">
+      <c r="N7" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
-      <c r="T7" s="144"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="150"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="150"/>
+      <c r="S7" s="150"/>
+      <c r="T7" s="151"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3254,24 +3272,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="140" t="s">
+      <c r="G13" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="141"/>
-      <c r="K13" s="141"/>
-      <c r="L13" s="142"/>
+      <c r="H13" s="148"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="148"/>
+      <c r="K13" s="148"/>
+      <c r="L13" s="149"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="140" t="s">
+      <c r="N13" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="141"/>
-      <c r="P13" s="141"/>
-      <c r="Q13" s="141"/>
-      <c r="R13" s="141"/>
-      <c r="S13" s="141"/>
-      <c r="T13" s="142"/>
+      <c r="O13" s="148"/>
+      <c r="P13" s="148"/>
+      <c r="Q13" s="148"/>
+      <c r="R13" s="148"/>
+      <c r="S13" s="148"/>
+      <c r="T13" s="149"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -3511,24 +3529,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="140" t="s">
+      <c r="G19" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
-      <c r="L19" s="142"/>
+      <c r="H19" s="148"/>
+      <c r="I19" s="148"/>
+      <c r="J19" s="148"/>
+      <c r="K19" s="148"/>
+      <c r="L19" s="149"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="140" t="s">
+      <c r="N19" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="141"/>
-      <c r="P19" s="141"/>
-      <c r="Q19" s="141"/>
-      <c r="R19" s="141"/>
-      <c r="S19" s="141"/>
-      <c r="T19" s="142"/>
+      <c r="O19" s="148"/>
+      <c r="P19" s="148"/>
+      <c r="Q19" s="148"/>
+      <c r="R19" s="148"/>
+      <c r="S19" s="148"/>
+      <c r="T19" s="149"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -3798,25 +3816,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="145" t="s">
+      <c r="D25" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="145"/>
-      <c r="I25" s="145"/>
-      <c r="J25" s="145"/>
-      <c r="K25" s="145"/>
-      <c r="L25" s="145"/>
-      <c r="M25" s="145"/>
-      <c r="N25" s="145"/>
-      <c r="O25" s="145"/>
-      <c r="P25" s="145"/>
-      <c r="Q25" s="145"/>
-      <c r="R25" s="145"/>
-      <c r="S25" s="145"/>
-      <c r="T25" s="145"/>
+      <c r="E25" s="152"/>
+      <c r="F25" s="152"/>
+      <c r="G25" s="152"/>
+      <c r="H25" s="152"/>
+      <c r="I25" s="152"/>
+      <c r="J25" s="152"/>
+      <c r="K25" s="152"/>
+      <c r="L25" s="152"/>
+      <c r="M25" s="152"/>
+      <c r="N25" s="152"/>
+      <c r="O25" s="152"/>
+      <c r="P25" s="152"/>
+      <c r="Q25" s="152"/>
+      <c r="R25" s="152"/>
+      <c r="S25" s="152"/>
+      <c r="T25" s="152"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3842,25 +3860,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="145" t="s">
+      <c r="D27" s="152" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="145"/>
-      <c r="I27" s="145"/>
-      <c r="J27" s="145"/>
-      <c r="K27" s="145"/>
-      <c r="L27" s="145"/>
-      <c r="M27" s="145"/>
-      <c r="N27" s="145"/>
-      <c r="O27" s="145"/>
-      <c r="P27" s="145"/>
-      <c r="Q27" s="145"/>
-      <c r="R27" s="145"/>
-      <c r="S27" s="145"/>
-      <c r="T27" s="145"/>
+      <c r="E27" s="152"/>
+      <c r="F27" s="152"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="152"/>
+      <c r="K27" s="152"/>
+      <c r="L27" s="152"/>
+      <c r="M27" s="152"/>
+      <c r="N27" s="152"/>
+      <c r="O27" s="152"/>
+      <c r="P27" s="152"/>
+      <c r="Q27" s="152"/>
+      <c r="R27" s="152"/>
+      <c r="S27" s="152"/>
+      <c r="T27" s="152"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3886,25 +3904,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="145" t="s">
+      <c r="D29" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="145"/>
-      <c r="F29" s="145"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="145"/>
-      <c r="I29" s="145"/>
-      <c r="J29" s="145"/>
-      <c r="K29" s="145"/>
-      <c r="L29" s="145"/>
-      <c r="M29" s="145"/>
-      <c r="N29" s="145"/>
-      <c r="O29" s="145"/>
-      <c r="P29" s="145"/>
-      <c r="Q29" s="145"/>
-      <c r="R29" s="145"/>
-      <c r="S29" s="145"/>
-      <c r="T29" s="145"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="152"/>
+      <c r="J29" s="152"/>
+      <c r="K29" s="152"/>
+      <c r="L29" s="152"/>
+      <c r="M29" s="152"/>
+      <c r="N29" s="152"/>
+      <c r="O29" s="152"/>
+      <c r="P29" s="152"/>
+      <c r="Q29" s="152"/>
+      <c r="R29" s="152"/>
+      <c r="S29" s="152"/>
+      <c r="T29" s="152"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -3930,25 +3948,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="145" t="s">
+      <c r="D31" s="152" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="145"/>
-      <c r="F31" s="145"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="145"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="145"/>
-      <c r="K31" s="145"/>
-      <c r="L31" s="145"/>
-      <c r="M31" s="145"/>
-      <c r="N31" s="145"/>
-      <c r="O31" s="145"/>
-      <c r="P31" s="145"/>
-      <c r="Q31" s="145"/>
-      <c r="R31" s="145"/>
-      <c r="S31" s="145"/>
-      <c r="T31" s="145"/>
+      <c r="E31" s="152"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="152"/>
+      <c r="H31" s="152"/>
+      <c r="I31" s="152"/>
+      <c r="J31" s="152"/>
+      <c r="K31" s="152"/>
+      <c r="L31" s="152"/>
+      <c r="M31" s="152"/>
+      <c r="N31" s="152"/>
+      <c r="O31" s="152"/>
+      <c r="P31" s="152"/>
+      <c r="Q31" s="152"/>
+      <c r="R31" s="152"/>
+      <c r="S31" s="152"/>
+      <c r="T31" s="152"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -3974,25 +3992,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="145" t="s">
+      <c r="D33" s="152" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="145"/>
-      <c r="F33" s="145"/>
-      <c r="G33" s="145"/>
-      <c r="H33" s="145"/>
-      <c r="I33" s="145"/>
-      <c r="J33" s="145"/>
-      <c r="K33" s="145"/>
-      <c r="L33" s="145"/>
-      <c r="M33" s="145"/>
-      <c r="N33" s="145"/>
-      <c r="O33" s="145"/>
-      <c r="P33" s="145"/>
-      <c r="Q33" s="145"/>
-      <c r="R33" s="145"/>
-      <c r="S33" s="145"/>
-      <c r="T33" s="145"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
+      <c r="H33" s="152"/>
+      <c r="I33" s="152"/>
+      <c r="J33" s="152"/>
+      <c r="K33" s="152"/>
+      <c r="L33" s="152"/>
+      <c r="M33" s="152"/>
+      <c r="N33" s="152"/>
+      <c r="O33" s="152"/>
+      <c r="P33" s="152"/>
+      <c r="Q33" s="152"/>
+      <c r="R33" s="152"/>
+      <c r="S33" s="152"/>
+      <c r="T33" s="152"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4018,25 +4036,25 @@
       <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="139" t="s">
+      <c r="D35" s="146" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="139"/>
-      <c r="F35" s="139"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="139"/>
-      <c r="I35" s="139"/>
-      <c r="J35" s="139"/>
-      <c r="K35" s="139"/>
-      <c r="L35" s="139"/>
-      <c r="M35" s="139"/>
-      <c r="N35" s="139"/>
-      <c r="O35" s="139"/>
-      <c r="P35" s="139"/>
-      <c r="Q35" s="139"/>
-      <c r="R35" s="139"/>
-      <c r="S35" s="139"/>
-      <c r="T35" s="139"/>
+      <c r="E35" s="146"/>
+      <c r="F35" s="146"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="146"/>
+      <c r="I35" s="146"/>
+      <c r="J35" s="146"/>
+      <c r="K35" s="146"/>
+      <c r="L35" s="146"/>
+      <c r="M35" s="146"/>
+      <c r="N35" s="146"/>
+      <c r="O35" s="146"/>
+      <c r="P35" s="146"/>
+      <c r="Q35" s="146"/>
+      <c r="R35" s="146"/>
+      <c r="S35" s="146"/>
+      <c r="T35" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4178,24 +4196,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="143" t="s">
+      <c r="G7" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="144"/>
+      <c r="H7" s="150"/>
+      <c r="I7" s="150"/>
+      <c r="J7" s="150"/>
+      <c r="K7" s="150"/>
+      <c r="L7" s="151"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="143" t="s">
+      <c r="N7" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
-      <c r="T7" s="144"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="150"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="150"/>
+      <c r="S7" s="150"/>
+      <c r="T7" s="151"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4437,24 +4455,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="140" t="s">
+      <c r="G13" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="141"/>
-      <c r="K13" s="141"/>
-      <c r="L13" s="142"/>
+      <c r="H13" s="148"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="148"/>
+      <c r="K13" s="148"/>
+      <c r="L13" s="149"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="140" t="s">
+      <c r="N13" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="141"/>
-      <c r="P13" s="141"/>
-      <c r="Q13" s="141"/>
-      <c r="R13" s="141"/>
-      <c r="S13" s="141"/>
-      <c r="T13" s="142"/>
+      <c r="O13" s="148"/>
+      <c r="P13" s="148"/>
+      <c r="Q13" s="148"/>
+      <c r="R13" s="148"/>
+      <c r="S13" s="148"/>
+      <c r="T13" s="149"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -4692,24 +4710,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="140" t="s">
+      <c r="G19" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
-      <c r="L19" s="142"/>
+      <c r="H19" s="148"/>
+      <c r="I19" s="148"/>
+      <c r="J19" s="148"/>
+      <c r="K19" s="148"/>
+      <c r="L19" s="149"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="140" t="s">
+      <c r="N19" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="141"/>
-      <c r="P19" s="141"/>
-      <c r="Q19" s="141"/>
-      <c r="R19" s="141"/>
-      <c r="S19" s="141"/>
-      <c r="T19" s="142"/>
+      <c r="O19" s="148"/>
+      <c r="P19" s="148"/>
+      <c r="Q19" s="148"/>
+      <c r="R19" s="148"/>
+      <c r="S19" s="148"/>
+      <c r="T19" s="149"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -4947,24 +4965,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="140" t="s">
+      <c r="G25" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="141"/>
-      <c r="I25" s="141"/>
-      <c r="J25" s="141"/>
-      <c r="K25" s="141"/>
-      <c r="L25" s="142"/>
+      <c r="H25" s="148"/>
+      <c r="I25" s="148"/>
+      <c r="J25" s="148"/>
+      <c r="K25" s="148"/>
+      <c r="L25" s="149"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="140" t="s">
+      <c r="N25" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="141"/>
-      <c r="P25" s="141"/>
-      <c r="Q25" s="141"/>
-      <c r="R25" s="141"/>
-      <c r="S25" s="141"/>
-      <c r="T25" s="142"/>
+      <c r="O25" s="148"/>
+      <c r="P25" s="148"/>
+      <c r="Q25" s="148"/>
+      <c r="R25" s="148"/>
+      <c r="S25" s="148"/>
+      <c r="T25" s="149"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
@@ -5202,26 +5220,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="136" t="s">
+      <c r="C31" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="136"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="136"/>
-      <c r="G31" s="136"/>
-      <c r="H31" s="136"/>
-      <c r="I31" s="136"/>
-      <c r="J31" s="136"/>
-      <c r="K31" s="136"/>
-      <c r="L31" s="136"/>
-      <c r="M31" s="136"/>
-      <c r="N31" s="136"/>
-      <c r="O31" s="136"/>
-      <c r="P31" s="136"/>
-      <c r="Q31" s="136"/>
-      <c r="R31" s="136"/>
-      <c r="S31" s="136"/>
-      <c r="T31" s="136"/>
+      <c r="D31" s="143"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="143"/>
+      <c r="G31" s="143"/>
+      <c r="H31" s="143"/>
+      <c r="I31" s="143"/>
+      <c r="J31" s="143"/>
+      <c r="K31" s="143"/>
+      <c r="L31" s="143"/>
+      <c r="M31" s="143"/>
+      <c r="N31" s="143"/>
+      <c r="O31" s="143"/>
+      <c r="P31" s="143"/>
+      <c r="Q31" s="143"/>
+      <c r="R31" s="143"/>
+      <c r="S31" s="143"/>
+      <c r="T31" s="143"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5248,26 +5266,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="136"/>
-      <c r="H33" s="136"/>
-      <c r="I33" s="136"/>
-      <c r="J33" s="136"/>
-      <c r="K33" s="136"/>
-      <c r="L33" s="136"/>
-      <c r="M33" s="136"/>
-      <c r="N33" s="136"/>
-      <c r="O33" s="136"/>
-      <c r="P33" s="136"/>
-      <c r="Q33" s="136"/>
-      <c r="R33" s="136"/>
-      <c r="S33" s="136"/>
-      <c r="T33" s="136"/>
+      <c r="D33" s="143"/>
+      <c r="E33" s="143"/>
+      <c r="F33" s="143"/>
+      <c r="G33" s="143"/>
+      <c r="H33" s="143"/>
+      <c r="I33" s="143"/>
+      <c r="J33" s="143"/>
+      <c r="K33" s="143"/>
+      <c r="L33" s="143"/>
+      <c r="M33" s="143"/>
+      <c r="N33" s="143"/>
+      <c r="O33" s="143"/>
+      <c r="P33" s="143"/>
+      <c r="Q33" s="143"/>
+      <c r="R33" s="143"/>
+      <c r="S33" s="143"/>
+      <c r="T33" s="143"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5294,26 +5312,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="136" t="s">
+      <c r="C35" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
-      <c r="F35" s="136"/>
-      <c r="G35" s="136"/>
-      <c r="H35" s="136"/>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="136"/>
-      <c r="L35" s="136"/>
-      <c r="M35" s="136"/>
-      <c r="N35" s="136"/>
-      <c r="O35" s="136"/>
-      <c r="P35" s="136"/>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="136"/>
-      <c r="S35" s="136"/>
-      <c r="T35" s="136"/>
+      <c r="D35" s="143"/>
+      <c r="E35" s="143"/>
+      <c r="F35" s="143"/>
+      <c r="G35" s="143"/>
+      <c r="H35" s="143"/>
+      <c r="I35" s="143"/>
+      <c r="J35" s="143"/>
+      <c r="K35" s="143"/>
+      <c r="L35" s="143"/>
+      <c r="M35" s="143"/>
+      <c r="N35" s="143"/>
+      <c r="O35" s="143"/>
+      <c r="P35" s="143"/>
+      <c r="Q35" s="143"/>
+      <c r="R35" s="143"/>
+      <c r="S35" s="143"/>
+      <c r="T35" s="143"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5340,26 +5358,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="136" t="s">
+      <c r="C37" s="143" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="136"/>
-      <c r="F37" s="136"/>
-      <c r="G37" s="136"/>
-      <c r="H37" s="136"/>
-      <c r="I37" s="136"/>
-      <c r="J37" s="136"/>
-      <c r="K37" s="136"/>
-      <c r="L37" s="136"/>
-      <c r="M37" s="136"/>
-      <c r="N37" s="136"/>
-      <c r="O37" s="136"/>
-      <c r="P37" s="136"/>
-      <c r="Q37" s="136"/>
-      <c r="R37" s="136"/>
-      <c r="S37" s="136"/>
-      <c r="T37" s="136"/>
+      <c r="D37" s="143"/>
+      <c r="E37" s="143"/>
+      <c r="F37" s="143"/>
+      <c r="G37" s="143"/>
+      <c r="H37" s="143"/>
+      <c r="I37" s="143"/>
+      <c r="J37" s="143"/>
+      <c r="K37" s="143"/>
+      <c r="L37" s="143"/>
+      <c r="M37" s="143"/>
+      <c r="N37" s="143"/>
+      <c r="O37" s="143"/>
+      <c r="P37" s="143"/>
+      <c r="Q37" s="143"/>
+      <c r="R37" s="143"/>
+      <c r="S37" s="143"/>
+      <c r="T37" s="143"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5386,26 +5404,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="136" t="s">
+      <c r="C39" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="136"/>
-      <c r="E39" s="136"/>
-      <c r="F39" s="136"/>
-      <c r="G39" s="136"/>
-      <c r="H39" s="136"/>
-      <c r="I39" s="136"/>
-      <c r="J39" s="136"/>
-      <c r="K39" s="136"/>
-      <c r="L39" s="136"/>
-      <c r="M39" s="136"/>
-      <c r="N39" s="136"/>
-      <c r="O39" s="136"/>
-      <c r="P39" s="136"/>
-      <c r="Q39" s="136"/>
-      <c r="R39" s="136"/>
-      <c r="S39" s="136"/>
-      <c r="T39" s="136"/>
+      <c r="D39" s="143"/>
+      <c r="E39" s="143"/>
+      <c r="F39" s="143"/>
+      <c r="G39" s="143"/>
+      <c r="H39" s="143"/>
+      <c r="I39" s="143"/>
+      <c r="J39" s="143"/>
+      <c r="K39" s="143"/>
+      <c r="L39" s="143"/>
+      <c r="M39" s="143"/>
+      <c r="N39" s="143"/>
+      <c r="O39" s="143"/>
+      <c r="P39" s="143"/>
+      <c r="Q39" s="143"/>
+      <c r="R39" s="143"/>
+      <c r="S39" s="143"/>
+      <c r="T39" s="143"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5432,29 +5450,34 @@
       <c r="B41" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="138" t="s">
+      <c r="C41" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="138"/>
-      <c r="E41" s="138"/>
-      <c r="F41" s="138"/>
-      <c r="G41" s="138"/>
-      <c r="H41" s="138"/>
-      <c r="I41" s="138"/>
-      <c r="J41" s="138"/>
-      <c r="K41" s="138"/>
-      <c r="L41" s="138"/>
-      <c r="M41" s="138"/>
-      <c r="N41" s="138"/>
-      <c r="O41" s="138"/>
-      <c r="P41" s="138"/>
-      <c r="Q41" s="138"/>
-      <c r="R41" s="138"/>
-      <c r="S41" s="138"/>
-      <c r="T41" s="138"/>
+      <c r="D41" s="145"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
+      <c r="K41" s="145"/>
+      <c r="L41" s="145"/>
+      <c r="M41" s="145"/>
+      <c r="N41" s="145"/>
+      <c r="O41" s="145"/>
+      <c r="P41" s="145"/>
+      <c r="Q41" s="145"/>
+      <c r="R41" s="145"/>
+      <c r="S41" s="145"/>
+      <c r="T41" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5464,11 +5487,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5507,94 +5525,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="115" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="153" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="146"/>
+      <c r="D4" s="153"/>
     </row>
     <row r="5" spans="3:4" s="115" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="146" t="s">
+      <c r="C5" s="153" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="146"/>
+      <c r="D5" s="153"/>
     </row>
     <row r="6" spans="3:4" s="115" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="146" t="s">
+      <c r="C6" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="146"/>
+      <c r="D6" s="153"/>
     </row>
     <row r="7" spans="3:4" s="115" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="146" t="s">
+      <c r="C7" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="146"/>
+      <c r="D7" s="153"/>
     </row>
     <row r="8" spans="3:4" s="115" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="146" t="s">
+      <c r="C8" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="146"/>
+      <c r="D8" s="153"/>
     </row>
     <row r="9" spans="3:4" s="115" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="146" t="s">
+      <c r="C9" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="146"/>
+      <c r="D9" s="153"/>
     </row>
     <row r="10" spans="3:4" s="115" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="146" t="s">
+      <c r="C10" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="146"/>
+      <c r="D10" s="153"/>
     </row>
     <row r="11" spans="3:4" s="115" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="146" t="s">
+      <c r="C11" s="153" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="146"/>
+      <c r="D11" s="153"/>
     </row>
     <row r="12" spans="3:4" s="115" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="146" t="s">
+      <c r="C12" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="146"/>
+      <c r="D12" s="153"/>
     </row>
     <row r="13" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="146" t="s">
+      <c r="C13" s="153" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="146"/>
+      <c r="D13" s="153"/>
     </row>
     <row r="14" spans="3:4" s="115" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="146" t="s">
+      <c r="C14" s="153" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="146"/>
+      <c r="D14" s="153"/>
     </row>
     <row r="15" spans="3:4" s="115" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="146" t="s">
+      <c r="C15" s="153" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="146"/>
+      <c r="D15" s="153"/>
     </row>
     <row r="16" spans="3:4" s="115" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="146" t="s">
+      <c r="C16" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="146"/>
+      <c r="D16" s="153"/>
     </row>
     <row r="17" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="146" t="s">
+      <c r="C17" s="153" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="146"/>
+      <c r="D17" s="153"/>
     </row>
     <row r="18" spans="3:4" s="115" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="146" t="s">
+      <c r="C18" s="153" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="146"/>
+      <c r="D18" s="153"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5627,8 +5645,8 @@
   </sheetPr>
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+    <sheetView showGridLines="0" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5640,10 +5658,17 @@
     <col min="5" max="5" width="7.875" style="98" customWidth="1"/>
     <col min="6" max="6" width="11.375" style="98" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="98" customWidth="1"/>
-    <col min="8" max="12" width="11.375" style="98" customWidth="1"/>
+    <col min="8" max="9" width="11.375" style="98" customWidth="1"/>
+    <col min="10" max="10" width="21" style="98" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.375" style="98" customWidth="1"/>
     <col min="13" max="13" width="12.5" style="98" customWidth="1"/>
-    <col min="14" max="19" width="11.375" style="98" customWidth="1"/>
-    <col min="20" max="20" width="12.5" style="98" customWidth="1"/>
+    <col min="14" max="14" width="18.75" style="98" customWidth="1"/>
+    <col min="15" max="15" width="17" style="98" customWidth="1"/>
+    <col min="16" max="16" width="29.875" style="98" customWidth="1"/>
+    <col min="17" max="17" width="25.125" style="98" customWidth="1"/>
+    <col min="18" max="18" width="16.125" style="98" customWidth="1"/>
+    <col min="19" max="19" width="13.5" style="98" customWidth="1"/>
+    <col min="20" max="20" width="16.75" style="98" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="3" style="98" customWidth="1"/>
     <col min="22" max="16384" width="10.625" style="98"/>
   </cols>
@@ -5679,27 +5704,30 @@
         <v>68</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
       <c r="N5" s="75"/>
       <c r="O5" s="136"/>
       <c r="P5" s="136"/>
@@ -5728,21 +5756,21 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="140" t="s">
+      <c r="H7" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="141"/>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
-      <c r="L7" s="141"/>
-      <c r="M7" s="142"/>
-      <c r="N7" s="140"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="141"/>
-      <c r="R7" s="141"/>
-      <c r="S7" s="141"/>
-      <c r="T7" s="142"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
+      <c r="K7" s="148"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="149"/>
+      <c r="N7" s="147"/>
+      <c r="O7" s="148"/>
+      <c r="P7" s="148"/>
+      <c r="Q7" s="148"/>
+      <c r="R7" s="148"/>
+      <c r="S7" s="148"/>
+      <c r="T7" s="149"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98" t="s">
@@ -5866,21 +5894,21 @@
       </c>
       <c r="D12" s="54"/>
       <c r="E12" s="116"/>
-      <c r="F12" s="147"/>
-      <c r="G12" s="147"/>
-      <c r="H12" s="147"/>
-      <c r="I12" s="147"/>
-      <c r="J12" s="147"/>
-      <c r="K12" s="147"/>
-      <c r="L12" s="147"/>
-      <c r="M12" s="147"/>
-      <c r="N12" s="147"/>
-      <c r="O12" s="147"/>
-      <c r="P12" s="147"/>
-      <c r="Q12" s="147"/>
-      <c r="R12" s="147"/>
-      <c r="S12" s="147"/>
-      <c r="T12" s="147"/>
+      <c r="F12" s="154"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="154"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="154"/>
+      <c r="N12" s="154"/>
+      <c r="O12" s="154"/>
+      <c r="P12" s="154"/>
+      <c r="Q12" s="154"/>
+      <c r="R12" s="154"/>
+      <c r="S12" s="154"/>
+      <c r="T12" s="154"/>
     </row>
     <row r="13" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
@@ -5906,21 +5934,21 @@
         <v>36</v>
       </c>
       <c r="D14" s="54"/>
-      <c r="F14" s="147"/>
-      <c r="G14" s="147"/>
-      <c r="H14" s="147"/>
-      <c r="I14" s="147"/>
-      <c r="J14" s="147"/>
-      <c r="K14" s="147"/>
-      <c r="L14" s="147"/>
-      <c r="M14" s="147"/>
-      <c r="N14" s="147"/>
-      <c r="O14" s="147"/>
-      <c r="P14" s="147"/>
-      <c r="Q14" s="147"/>
-      <c r="R14" s="147"/>
-      <c r="S14" s="147"/>
-      <c r="T14" s="147"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="154"/>
+      <c r="L14" s="154"/>
+      <c r="M14" s="154"/>
+      <c r="N14" s="154"/>
+      <c r="O14" s="154"/>
+      <c r="P14" s="154"/>
+      <c r="Q14" s="154"/>
+      <c r="R14" s="154"/>
+      <c r="S14" s="154"/>
+      <c r="T14" s="154"/>
     </row>
     <row r="15" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -5947,21 +5975,21 @@
       </c>
       <c r="D16" s="54"/>
       <c r="E16" s="116"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="147"/>
-      <c r="H16" s="147"/>
-      <c r="I16" s="147"/>
-      <c r="J16" s="147"/>
-      <c r="K16" s="147"/>
-      <c r="L16" s="147"/>
-      <c r="M16" s="147"/>
-      <c r="N16" s="147"/>
-      <c r="O16" s="147"/>
-      <c r="P16" s="147"/>
-      <c r="Q16" s="147"/>
-      <c r="R16" s="147"/>
-      <c r="S16" s="147"/>
-      <c r="T16" s="147"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
+      <c r="M16" s="154"/>
+      <c r="N16" s="154"/>
+      <c r="O16" s="154"/>
+      <c r="P16" s="154"/>
+      <c r="Q16" s="154"/>
+      <c r="R16" s="154"/>
+      <c r="S16" s="154"/>
+      <c r="T16" s="154"/>
     </row>
     <row r="17" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -5987,21 +6015,21 @@
         <v>48</v>
       </c>
       <c r="D18" s="54"/>
-      <c r="F18" s="147"/>
-      <c r="G18" s="147"/>
-      <c r="H18" s="147"/>
-      <c r="I18" s="147"/>
-      <c r="J18" s="147"/>
-      <c r="K18" s="147"/>
-      <c r="L18" s="147"/>
-      <c r="M18" s="147"/>
-      <c r="N18" s="147"/>
-      <c r="O18" s="147"/>
-      <c r="P18" s="147"/>
-      <c r="Q18" s="147"/>
-      <c r="R18" s="147"/>
-      <c r="S18" s="147"/>
-      <c r="T18" s="147"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
+      <c r="K18" s="154"/>
+      <c r="L18" s="154"/>
+      <c r="M18" s="154"/>
+      <c r="N18" s="154"/>
+      <c r="O18" s="154"/>
+      <c r="P18" s="154"/>
+      <c r="Q18" s="154"/>
+      <c r="R18" s="154"/>
+      <c r="S18" s="154"/>
+      <c r="T18" s="154"/>
     </row>
     <row r="19" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
@@ -6027,40 +6055,38 @@
         <v>49</v>
       </c>
       <c r="D20" s="54"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="138"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="138"/>
-      <c r="K20" s="138"/>
-      <c r="L20" s="138"/>
-      <c r="M20" s="138"/>
-      <c r="N20" s="138"/>
-      <c r="O20" s="138"/>
-      <c r="P20" s="138"/>
-      <c r="Q20" s="138"/>
-      <c r="R20" s="138"/>
-      <c r="S20" s="138"/>
-      <c r="T20" s="138"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="145"/>
+      <c r="L20" s="145"/>
+      <c r="M20" s="145"/>
+      <c r="N20" s="145"/>
+      <c r="O20" s="145"/>
+      <c r="P20" s="145"/>
+      <c r="Q20" s="145"/>
+      <c r="R20" s="145"/>
+      <c r="S20" s="145"/>
+      <c r="T20" s="145"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="12">
+    <mergeCell ref="F16:T16"/>
+    <mergeCell ref="F18:T18"/>
+    <mergeCell ref="F20:T20"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="F12:T12"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="F14:T14"/>
-    <mergeCell ref="F16:T16"/>
-    <mergeCell ref="F18:T18"/>
-    <mergeCell ref="F20:T20"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="F12:T12"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:T3 C5 C4:N4 P4 R4:T4 T5 C6:T1048576">
+  <conditionalFormatting sqref="C1:T3 C5 C4:N4 T5 C6:T1048576 P4:Q4 S4">
     <cfRule type="expression" dxfId="0" priority="15">
       <formula>$A1="Even"</formula>
     </cfRule>
@@ -6078,7 +6104,7 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:O9"/>
     </sheetView>
   </sheetViews>
@@ -6102,18 +6128,18 @@
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="135"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="141"/>
-      <c r="M2" s="141"/>
-      <c r="N2" s="142"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="149"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6235,53 +6261,53 @@
       <c r="B9" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="152"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="152"/>
-      <c r="L9" s="153"/>
-      <c r="M9" s="153"/>
-      <c r="N9" s="153"/>
-      <c r="O9" s="162"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="140"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="139"/>
+      <c r="N9" s="139"/>
+      <c r="O9" s="142"/>
     </row>
     <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="158"/>
-      <c r="D10" s="159"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="160"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="149"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="150"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="149"/>
-      <c r="M10" s="149"/>
-      <c r="N10" s="150"/>
-      <c r="O10" s="161"/>
+      <c r="C10" s="161"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="162"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="155"/>
+      <c r="H10" s="156"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="157"/>
+      <c r="K10" s="155"/>
+      <c r="L10" s="156"/>
+      <c r="M10" s="156"/>
+      <c r="N10" s="157"/>
+      <c r="O10" s="141"/>
     </row>
     <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="135"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
-      <c r="F12" s="141"/>
-      <c r="G12" s="142"/>
-      <c r="H12" s="141"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="141"/>
-      <c r="K12" s="142"/>
-      <c r="L12" s="140"/>
-      <c r="M12" s="141"/>
-      <c r="N12" s="141"/>
-      <c r="O12" s="142"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="148"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="148"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="148"/>
+      <c r="I12" s="148"/>
+      <c r="J12" s="148"/>
+      <c r="K12" s="149"/>
+      <c r="L12" s="147"/>
+      <c r="M12" s="148"/>
+      <c r="N12" s="148"/>
+      <c r="O12" s="149"/>
       <c r="P12" s="29"/>
     </row>
     <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6404,55 +6430,55 @@
       <c r="B19" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="153"/>
-      <c r="H19" s="152"/>
-      <c r="I19" s="153"/>
-      <c r="J19" s="153"/>
-      <c r="K19" s="154"/>
-      <c r="L19" s="152"/>
-      <c r="M19" s="153"/>
-      <c r="N19" s="153"/>
-      <c r="O19" s="154"/>
-      <c r="P19" s="154"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="139"/>
+      <c r="K19" s="140"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="139"/>
+      <c r="N19" s="139"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="140"/>
     </row>
     <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="155"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="156"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="149"/>
-      <c r="J20" s="149"/>
-      <c r="K20" s="150"/>
-      <c r="L20" s="148"/>
-      <c r="M20" s="149"/>
-      <c r="N20" s="149"/>
-      <c r="O20" s="150"/>
-      <c r="P20" s="151"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="155"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
+      <c r="K20" s="157"/>
+      <c r="L20" s="155"/>
+      <c r="M20" s="156"/>
+      <c r="N20" s="156"/>
+      <c r="O20" s="157"/>
+      <c r="P20" s="137"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="135"/>
-      <c r="C22" s="140"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="141"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="141"/>
-      <c r="K22" s="142"/>
-      <c r="L22" s="140"/>
-      <c r="M22" s="141"/>
-      <c r="N22" s="141"/>
-      <c r="O22" s="142"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="148"/>
+      <c r="F22" s="149"/>
+      <c r="G22" s="148"/>
+      <c r="H22" s="148"/>
+      <c r="I22" s="148"/>
+      <c r="J22" s="148"/>
+      <c r="K22" s="149"/>
+      <c r="L22" s="147"/>
+      <c r="M22" s="148"/>
+      <c r="N22" s="148"/>
+      <c r="O22" s="149"/>
       <c r="P22" s="29"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6575,55 +6601,55 @@
       <c r="B29" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="153"/>
-      <c r="F29" s="153"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="153"/>
-      <c r="I29" s="153"/>
-      <c r="J29" s="153"/>
-      <c r="K29" s="154"/>
-      <c r="L29" s="152"/>
-      <c r="M29" s="153"/>
-      <c r="N29" s="153"/>
-      <c r="O29" s="154"/>
-      <c r="P29" s="154"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="139"/>
+      <c r="N29" s="139"/>
+      <c r="O29" s="140"/>
+      <c r="P29" s="140"/>
     </row>
     <row r="30" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="148"/>
-      <c r="D30" s="149"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="148"/>
-      <c r="H30" s="149"/>
-      <c r="I30" s="149"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="150"/>
-      <c r="L30" s="148"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="150"/>
-      <c r="P30" s="151"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="156"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="155"/>
+      <c r="H30" s="156"/>
+      <c r="I30" s="156"/>
+      <c r="J30" s="156"/>
+      <c r="K30" s="157"/>
+      <c r="L30" s="155"/>
+      <c r="M30" s="156"/>
+      <c r="N30" s="156"/>
+      <c r="O30" s="157"/>
+      <c r="P30" s="137"/>
     </row>
     <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="135"/>
-      <c r="C32" s="140"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="141"/>
-      <c r="F32" s="142"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="141"/>
-      <c r="I32" s="141"/>
-      <c r="J32" s="142"/>
-      <c r="K32" s="140"/>
-      <c r="L32" s="141"/>
-      <c r="M32" s="141"/>
-      <c r="N32" s="141"/>
-      <c r="O32" s="142"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="148"/>
+      <c r="F32" s="149"/>
+      <c r="G32" s="148"/>
+      <c r="H32" s="148"/>
+      <c r="I32" s="148"/>
+      <c r="J32" s="149"/>
+      <c r="K32" s="147"/>
+      <c r="L32" s="148"/>
+      <c r="M32" s="148"/>
+      <c r="N32" s="148"/>
+      <c r="O32" s="149"/>
       <c r="P32" s="29"/>
     </row>
     <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6746,56 +6772,56 @@
       <c r="B39" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="152"/>
-      <c r="D39" s="153"/>
-      <c r="E39" s="153"/>
-      <c r="F39" s="153"/>
-      <c r="G39" s="152"/>
-      <c r="H39" s="153"/>
-      <c r="I39" s="153"/>
-      <c r="J39" s="154"/>
-      <c r="K39" s="152"/>
-      <c r="L39" s="153"/>
-      <c r="M39" s="153"/>
-      <c r="N39" s="153"/>
-      <c r="O39" s="154"/>
-      <c r="P39" s="154"/>
+      <c r="C39" s="138"/>
+      <c r="D39" s="139"/>
+      <c r="E39" s="139"/>
+      <c r="F39" s="139"/>
+      <c r="G39" s="138"/>
+      <c r="H39" s="139"/>
+      <c r="I39" s="139"/>
+      <c r="J39" s="140"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="139"/>
+      <c r="M39" s="139"/>
+      <c r="N39" s="139"/>
+      <c r="O39" s="140"/>
+      <c r="P39" s="140"/>
     </row>
     <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="148"/>
-      <c r="D40" s="149"/>
-      <c r="E40" s="149"/>
-      <c r="F40" s="150"/>
-      <c r="G40" s="148"/>
-      <c r="H40" s="149"/>
-      <c r="I40" s="149"/>
-      <c r="J40" s="150"/>
-      <c r="K40" s="148"/>
-      <c r="L40" s="149"/>
-      <c r="M40" s="149"/>
-      <c r="N40" s="149"/>
-      <c r="O40" s="150"/>
-      <c r="P40" s="151"/>
+      <c r="C40" s="155"/>
+      <c r="D40" s="156"/>
+      <c r="E40" s="156"/>
+      <c r="F40" s="157"/>
+      <c r="G40" s="155"/>
+      <c r="H40" s="156"/>
+      <c r="I40" s="156"/>
+      <c r="J40" s="157"/>
+      <c r="K40" s="155"/>
+      <c r="L40" s="156"/>
+      <c r="M40" s="156"/>
+      <c r="N40" s="156"/>
+      <c r="O40" s="157"/>
+      <c r="P40" s="137"/>
     </row>
     <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="135"/>
-      <c r="C42" s="140"/>
-      <c r="D42" s="141"/>
-      <c r="E42" s="141"/>
-      <c r="F42" s="141"/>
-      <c r="G42" s="142"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="141"/>
-      <c r="J42" s="141"/>
-      <c r="K42" s="141"/>
-      <c r="L42" s="142"/>
-      <c r="M42" s="140"/>
-      <c r="N42" s="141"/>
-      <c r="O42" s="141"/>
-      <c r="P42" s="142"/>
+      <c r="C42" s="147"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="148"/>
+      <c r="G42" s="149"/>
+      <c r="H42" s="148"/>
+      <c r="I42" s="148"/>
+      <c r="J42" s="148"/>
+      <c r="K42" s="148"/>
+      <c r="L42" s="149"/>
+      <c r="M42" s="147"/>
+      <c r="N42" s="148"/>
+      <c r="O42" s="148"/>
+      <c r="P42" s="149"/>
       <c r="Q42" s="29"/>
     </row>
     <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6924,58 +6950,58 @@
       <c r="B49" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="152"/>
-      <c r="D49" s="153"/>
-      <c r="E49" s="153"/>
-      <c r="F49" s="153"/>
-      <c r="G49" s="153"/>
-      <c r="H49" s="152"/>
-      <c r="I49" s="153"/>
-      <c r="J49" s="153"/>
-      <c r="K49" s="153"/>
-      <c r="L49" s="154"/>
-      <c r="M49" s="152"/>
-      <c r="N49" s="153"/>
-      <c r="O49" s="153"/>
-      <c r="P49" s="154"/>
-      <c r="Q49" s="154"/>
+      <c r="C49" s="138"/>
+      <c r="D49" s="139"/>
+      <c r="E49" s="139"/>
+      <c r="F49" s="139"/>
+      <c r="G49" s="139"/>
+      <c r="H49" s="138"/>
+      <c r="I49" s="139"/>
+      <c r="J49" s="139"/>
+      <c r="K49" s="139"/>
+      <c r="L49" s="140"/>
+      <c r="M49" s="138"/>
+      <c r="N49" s="139"/>
+      <c r="O49" s="139"/>
+      <c r="P49" s="140"/>
+      <c r="Q49" s="140"/>
     </row>
     <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="148"/>
-      <c r="D50" s="149"/>
-      <c r="E50" s="149"/>
-      <c r="F50" s="149"/>
-      <c r="G50" s="150"/>
-      <c r="H50" s="148"/>
-      <c r="I50" s="149"/>
-      <c r="J50" s="149"/>
-      <c r="K50" s="149"/>
-      <c r="L50" s="150"/>
-      <c r="M50" s="148"/>
-      <c r="N50" s="149"/>
-      <c r="O50" s="149"/>
-      <c r="P50" s="150"/>
-      <c r="Q50" s="151"/>
+      <c r="C50" s="155"/>
+      <c r="D50" s="156"/>
+      <c r="E50" s="156"/>
+      <c r="F50" s="156"/>
+      <c r="G50" s="157"/>
+      <c r="H50" s="155"/>
+      <c r="I50" s="156"/>
+      <c r="J50" s="156"/>
+      <c r="K50" s="156"/>
+      <c r="L50" s="157"/>
+      <c r="M50" s="155"/>
+      <c r="N50" s="156"/>
+      <c r="O50" s="156"/>
+      <c r="P50" s="157"/>
+      <c r="Q50" s="137"/>
     </row>
     <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="135"/>
-      <c r="C52" s="140"/>
-      <c r="D52" s="141"/>
-      <c r="E52" s="141"/>
-      <c r="F52" s="141"/>
-      <c r="G52" s="142"/>
-      <c r="H52" s="141"/>
-      <c r="I52" s="141"/>
-      <c r="J52" s="141"/>
-      <c r="K52" s="142"/>
-      <c r="L52" s="140"/>
-      <c r="M52" s="141"/>
-      <c r="N52" s="141"/>
-      <c r="O52" s="141"/>
-      <c r="P52" s="142"/>
+      <c r="C52" s="147"/>
+      <c r="D52" s="148"/>
+      <c r="E52" s="148"/>
+      <c r="F52" s="148"/>
+      <c r="G52" s="149"/>
+      <c r="H52" s="148"/>
+      <c r="I52" s="148"/>
+      <c r="J52" s="148"/>
+      <c r="K52" s="149"/>
+      <c r="L52" s="147"/>
+      <c r="M52" s="148"/>
+      <c r="N52" s="148"/>
+      <c r="O52" s="148"/>
+      <c r="P52" s="149"/>
       <c r="Q52" s="29"/>
     </row>
     <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7104,58 +7130,58 @@
       <c r="B59" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="152"/>
-      <c r="D59" s="153"/>
-      <c r="E59" s="153"/>
-      <c r="F59" s="153"/>
-      <c r="G59" s="153"/>
-      <c r="H59" s="152"/>
-      <c r="I59" s="153"/>
-      <c r="J59" s="153"/>
-      <c r="K59" s="154"/>
-      <c r="L59" s="152"/>
-      <c r="M59" s="153"/>
-      <c r="N59" s="153"/>
-      <c r="O59" s="153"/>
-      <c r="P59" s="154"/>
-      <c r="Q59" s="154"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="139"/>
+      <c r="E59" s="139"/>
+      <c r="F59" s="139"/>
+      <c r="G59" s="139"/>
+      <c r="H59" s="138"/>
+      <c r="I59" s="139"/>
+      <c r="J59" s="139"/>
+      <c r="K59" s="140"/>
+      <c r="L59" s="138"/>
+      <c r="M59" s="139"/>
+      <c r="N59" s="139"/>
+      <c r="O59" s="139"/>
+      <c r="P59" s="140"/>
+      <c r="Q59" s="140"/>
     </row>
     <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="148"/>
-      <c r="D60" s="149"/>
-      <c r="E60" s="149"/>
-      <c r="F60" s="149"/>
-      <c r="G60" s="150"/>
-      <c r="H60" s="148"/>
-      <c r="I60" s="149"/>
-      <c r="J60" s="149"/>
-      <c r="K60" s="150"/>
-      <c r="L60" s="148"/>
-      <c r="M60" s="149"/>
-      <c r="N60" s="149"/>
-      <c r="O60" s="149"/>
-      <c r="P60" s="150"/>
-      <c r="Q60" s="151"/>
+      <c r="C60" s="155"/>
+      <c r="D60" s="156"/>
+      <c r="E60" s="156"/>
+      <c r="F60" s="156"/>
+      <c r="G60" s="157"/>
+      <c r="H60" s="155"/>
+      <c r="I60" s="156"/>
+      <c r="J60" s="156"/>
+      <c r="K60" s="157"/>
+      <c r="L60" s="155"/>
+      <c r="M60" s="156"/>
+      <c r="N60" s="156"/>
+      <c r="O60" s="156"/>
+      <c r="P60" s="157"/>
+      <c r="Q60" s="137"/>
     </row>
     <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="135"/>
-      <c r="C62" s="140"/>
-      <c r="D62" s="141"/>
-      <c r="E62" s="141"/>
-      <c r="F62" s="142"/>
-      <c r="G62" s="141"/>
-      <c r="H62" s="141"/>
-      <c r="I62" s="141"/>
-      <c r="J62" s="141"/>
-      <c r="K62" s="142"/>
-      <c r="L62" s="140"/>
-      <c r="M62" s="141"/>
-      <c r="N62" s="141"/>
-      <c r="O62" s="141"/>
-      <c r="P62" s="142"/>
+      <c r="C62" s="147"/>
+      <c r="D62" s="148"/>
+      <c r="E62" s="148"/>
+      <c r="F62" s="149"/>
+      <c r="G62" s="148"/>
+      <c r="H62" s="148"/>
+      <c r="I62" s="148"/>
+      <c r="J62" s="148"/>
+      <c r="K62" s="149"/>
+      <c r="L62" s="147"/>
+      <c r="M62" s="148"/>
+      <c r="N62" s="148"/>
+      <c r="O62" s="148"/>
+      <c r="P62" s="149"/>
       <c r="Q62" s="29"/>
     </row>
     <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7284,44 +7310,70 @@
       <c r="B69" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="152"/>
-      <c r="D69" s="153"/>
-      <c r="E69" s="153"/>
-      <c r="F69" s="153"/>
-      <c r="G69" s="152"/>
-      <c r="H69" s="153"/>
-      <c r="I69" s="153"/>
-      <c r="J69" s="153"/>
-      <c r="K69" s="154"/>
-      <c r="L69" s="152"/>
-      <c r="M69" s="153"/>
-      <c r="N69" s="153"/>
-      <c r="O69" s="153"/>
-      <c r="P69" s="154"/>
-      <c r="Q69" s="154"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="139"/>
+      <c r="E69" s="139"/>
+      <c r="F69" s="139"/>
+      <c r="G69" s="138"/>
+      <c r="H69" s="139"/>
+      <c r="I69" s="139"/>
+      <c r="J69" s="139"/>
+      <c r="K69" s="140"/>
+      <c r="L69" s="138"/>
+      <c r="M69" s="139"/>
+      <c r="N69" s="139"/>
+      <c r="O69" s="139"/>
+      <c r="P69" s="140"/>
+      <c r="Q69" s="140"/>
     </row>
     <row r="70" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="148"/>
-      <c r="D70" s="149"/>
-      <c r="E70" s="149"/>
-      <c r="F70" s="150"/>
-      <c r="G70" s="148"/>
-      <c r="H70" s="149"/>
-      <c r="I70" s="149"/>
-      <c r="J70" s="149"/>
-      <c r="K70" s="150"/>
-      <c r="L70" s="148"/>
-      <c r="M70" s="149"/>
-      <c r="N70" s="149"/>
-      <c r="O70" s="149"/>
-      <c r="P70" s="150"/>
-      <c r="Q70" s="151"/>
+      <c r="C70" s="155"/>
+      <c r="D70" s="156"/>
+      <c r="E70" s="156"/>
+      <c r="F70" s="157"/>
+      <c r="G70" s="155"/>
+      <c r="H70" s="156"/>
+      <c r="I70" s="156"/>
+      <c r="J70" s="156"/>
+      <c r="K70" s="157"/>
+      <c r="L70" s="155"/>
+      <c r="M70" s="156"/>
+      <c r="N70" s="156"/>
+      <c r="O70" s="156"/>
+      <c r="P70" s="157"/>
+      <c r="Q70" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="L70:P70"/>
+    <mergeCell ref="L60:P60"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:O40"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="H52:K52"/>
     <mergeCell ref="L52:P52"/>
@@ -7338,32 +7390,6 @@
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="G22:K22"/>
     <mergeCell ref="L22:O22"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="K40:O40"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="H50:L50"/>
-    <mergeCell ref="M50:P50"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C70:F70"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="L70:P70"/>
-    <mergeCell ref="L60:P60"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 L30 L70 K10 K40 M50 C20 H20 C10 G10 C30 G30 C40 G40 C50 H50 C60 C70 H60 G70 L60" xr:uid="{1A174315-2F56-4C74-8CF2-D4F4F4F25C91}"/>

</xml_diff>

<commit_message>
Merged PR 17435: BP-5508_[Stage/QA]User is getting "Call your administrator to check the log messages." error message when user tries to export SCX report when buying is running
BP-5508_[Stage/QA]User is getting "Call your administrator to check the log messages." error message when user tries to export SCX report when buying is running
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F93F6D2-03E2-4774-B73D-6C1695672F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DC8BE1-2C95-4425-809A-065A63A0B2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -1145,7 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1572,6 +1572,9 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
@@ -2288,8 +2291,8 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2364,11 +2367,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="143">
+      <c r="E5" s="144">
         <f>Proposal!H5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="143"/>
+      <c r="F5" s="144"/>
       <c r="G5" s="75">
         <f>Proposal!J5</f>
         <v>0</v>
@@ -2385,14 +2388,8 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="75">
-        <f>Proposal!P5</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="75">
-        <f>Proposal!Q5</f>
-        <v>0</v>
-      </c>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
       <c r="M5" s="2">
         <f>Proposal!S5</f>
         <v>0</v>
@@ -2567,14 +2564,14 @@
       <c r="C18" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="145"/>
-      <c r="J18" s="145"/>
-      <c r="K18" s="145"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="146"/>
       <c r="L18" s="125"/>
       <c r="M18" s="125"/>
       <c r="N18" s="125"/>
@@ -2605,14 +2602,14 @@
       <c r="C20" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="145"/>
-      <c r="E20" s="145"/>
-      <c r="F20" s="145"/>
-      <c r="G20" s="145"/>
-      <c r="H20" s="145"/>
-      <c r="I20" s="145"/>
-      <c r="J20" s="145"/>
-      <c r="K20" s="145"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="146"/>
+      <c r="J20" s="146"/>
+      <c r="K20" s="146"/>
       <c r="L20" s="125"/>
       <c r="M20" s="125"/>
       <c r="N20" s="125"/>
@@ -2643,14 +2640,14 @@
       <c r="C22" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="145"/>
-      <c r="E22" s="145"/>
-      <c r="F22" s="145"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="145"/>
-      <c r="I22" s="145"/>
-      <c r="J22" s="145"/>
-      <c r="K22" s="145"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="146"/>
+      <c r="J22" s="146"/>
+      <c r="K22" s="146"/>
       <c r="L22" s="125"/>
       <c r="M22" s="125"/>
       <c r="N22" s="125"/>
@@ -2681,14 +2678,14 @@
       <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="145"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="145"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="145"/>
-      <c r="I24" s="145"/>
-      <c r="J24" s="145"/>
-      <c r="K24" s="145"/>
+      <c r="D24" s="146"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="146"/>
+      <c r="J24" s="146"/>
+      <c r="K24" s="146"/>
       <c r="L24" s="125"/>
       <c r="M24" s="125"/>
       <c r="N24" s="125"/>
@@ -2719,14 +2716,14 @@
       <c r="C26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="145"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="145"/>
-      <c r="I26" s="145"/>
-      <c r="J26" s="145"/>
-      <c r="K26" s="145"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="146"/>
+      <c r="I26" s="146"/>
+      <c r="J26" s="146"/>
+      <c r="K26" s="146"/>
       <c r="L26" s="76"/>
       <c r="M26" s="76"/>
       <c r="N26" s="76"/>
@@ -2736,14 +2733,14 @@
       <c r="R26" s="76"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="144"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="144"/>
-      <c r="G27" s="144"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="144"/>
-      <c r="J27" s="144"/>
-      <c r="K27" s="144"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2755,7 +2752,7 @@
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D24:K24"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:K1048576">
+  <conditionalFormatting sqref="C1:K4 C6:K1048576 C5:J5">
     <cfRule type="expression" dxfId="8" priority="5">
       <formula>$A1="Even"</formula>
     </cfRule>
@@ -2846,19 +2843,19 @@
         <f>Proposal!N5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="143"/>
-      <c r="E5" s="143"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="143"/>
-      <c r="H5" s="143"/>
-      <c r="I5" s="143"/>
-      <c r="J5" s="143"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="143"/>
-      <c r="M5" s="143"/>
-      <c r="N5" s="143"/>
-      <c r="O5" s="143"/>
-      <c r="P5" s="143"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="144"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="144"/>
+      <c r="L5" s="144"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="144"/>
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="59"/>
@@ -3011,24 +3008,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="150" t="s">
+      <c r="G7" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="150"/>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
+      <c r="L7" s="152"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="150" t="s">
+      <c r="N7" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="150"/>
-      <c r="P7" s="150"/>
-      <c r="Q7" s="150"/>
-      <c r="R7" s="150"/>
-      <c r="S7" s="150"/>
-      <c r="T7" s="151"/>
+      <c r="O7" s="151"/>
+      <c r="P7" s="151"/>
+      <c r="Q7" s="151"/>
+      <c r="R7" s="151"/>
+      <c r="S7" s="151"/>
+      <c r="T7" s="152"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3272,24 +3269,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="147" t="s">
+      <c r="G13" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="148"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="149"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="150"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="147" t="s">
+      <c r="N13" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="148"/>
-      <c r="T13" s="149"/>
+      <c r="O13" s="149"/>
+      <c r="P13" s="149"/>
+      <c r="Q13" s="149"/>
+      <c r="R13" s="149"/>
+      <c r="S13" s="149"/>
+      <c r="T13" s="150"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -3529,24 +3526,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="147" t="s">
+      <c r="G19" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="148"/>
-      <c r="K19" s="148"/>
-      <c r="L19" s="149"/>
+      <c r="H19" s="149"/>
+      <c r="I19" s="149"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="150"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="147" t="s">
+      <c r="N19" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="148"/>
-      <c r="P19" s="148"/>
-      <c r="Q19" s="148"/>
-      <c r="R19" s="148"/>
-      <c r="S19" s="148"/>
-      <c r="T19" s="149"/>
+      <c r="O19" s="149"/>
+      <c r="P19" s="149"/>
+      <c r="Q19" s="149"/>
+      <c r="R19" s="149"/>
+      <c r="S19" s="149"/>
+      <c r="T19" s="150"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -3816,25 +3813,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="152" t="s">
+      <c r="D25" s="153" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="152"/>
-      <c r="F25" s="152"/>
-      <c r="G25" s="152"/>
-      <c r="H25" s="152"/>
-      <c r="I25" s="152"/>
-      <c r="J25" s="152"/>
-      <c r="K25" s="152"/>
-      <c r="L25" s="152"/>
-      <c r="M25" s="152"/>
-      <c r="N25" s="152"/>
-      <c r="O25" s="152"/>
-      <c r="P25" s="152"/>
-      <c r="Q25" s="152"/>
-      <c r="R25" s="152"/>
-      <c r="S25" s="152"/>
-      <c r="T25" s="152"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="153"/>
+      <c r="G25" s="153"/>
+      <c r="H25" s="153"/>
+      <c r="I25" s="153"/>
+      <c r="J25" s="153"/>
+      <c r="K25" s="153"/>
+      <c r="L25" s="153"/>
+      <c r="M25" s="153"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="153"/>
+      <c r="P25" s="153"/>
+      <c r="Q25" s="153"/>
+      <c r="R25" s="153"/>
+      <c r="S25" s="153"/>
+      <c r="T25" s="153"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3860,25 +3857,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="152" t="s">
+      <c r="D27" s="153" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="152"/>
-      <c r="F27" s="152"/>
-      <c r="G27" s="152"/>
-      <c r="H27" s="152"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="152"/>
-      <c r="K27" s="152"/>
-      <c r="L27" s="152"/>
-      <c r="M27" s="152"/>
-      <c r="N27" s="152"/>
-      <c r="O27" s="152"/>
-      <c r="P27" s="152"/>
-      <c r="Q27" s="152"/>
-      <c r="R27" s="152"/>
-      <c r="S27" s="152"/>
-      <c r="T27" s="152"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="153"/>
+      <c r="I27" s="153"/>
+      <c r="J27" s="153"/>
+      <c r="K27" s="153"/>
+      <c r="L27" s="153"/>
+      <c r="M27" s="153"/>
+      <c r="N27" s="153"/>
+      <c r="O27" s="153"/>
+      <c r="P27" s="153"/>
+      <c r="Q27" s="153"/>
+      <c r="R27" s="153"/>
+      <c r="S27" s="153"/>
+      <c r="T27" s="153"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3904,25 +3901,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="152" t="s">
+      <c r="D29" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="152"/>
-      <c r="J29" s="152"/>
-      <c r="K29" s="152"/>
-      <c r="L29" s="152"/>
-      <c r="M29" s="152"/>
-      <c r="N29" s="152"/>
-      <c r="O29" s="152"/>
-      <c r="P29" s="152"/>
-      <c r="Q29" s="152"/>
-      <c r="R29" s="152"/>
-      <c r="S29" s="152"/>
-      <c r="T29" s="152"/>
+      <c r="E29" s="153"/>
+      <c r="F29" s="153"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="153"/>
+      <c r="I29" s="153"/>
+      <c r="J29" s="153"/>
+      <c r="K29" s="153"/>
+      <c r="L29" s="153"/>
+      <c r="M29" s="153"/>
+      <c r="N29" s="153"/>
+      <c r="O29" s="153"/>
+      <c r="P29" s="153"/>
+      <c r="Q29" s="153"/>
+      <c r="R29" s="153"/>
+      <c r="S29" s="153"/>
+      <c r="T29" s="153"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -3948,25 +3945,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="152" t="s">
+      <c r="D31" s="153" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="152"/>
-      <c r="I31" s="152"/>
-      <c r="J31" s="152"/>
-      <c r="K31" s="152"/>
-      <c r="L31" s="152"/>
-      <c r="M31" s="152"/>
-      <c r="N31" s="152"/>
-      <c r="O31" s="152"/>
-      <c r="P31" s="152"/>
-      <c r="Q31" s="152"/>
-      <c r="R31" s="152"/>
-      <c r="S31" s="152"/>
-      <c r="T31" s="152"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
+      <c r="H31" s="153"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="153"/>
+      <c r="K31" s="153"/>
+      <c r="L31" s="153"/>
+      <c r="M31" s="153"/>
+      <c r="N31" s="153"/>
+      <c r="O31" s="153"/>
+      <c r="P31" s="153"/>
+      <c r="Q31" s="153"/>
+      <c r="R31" s="153"/>
+      <c r="S31" s="153"/>
+      <c r="T31" s="153"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -3992,25 +3989,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="152" t="s">
+      <c r="D33" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="152"/>
-      <c r="H33" s="152"/>
-      <c r="I33" s="152"/>
-      <c r="J33" s="152"/>
-      <c r="K33" s="152"/>
-      <c r="L33" s="152"/>
-      <c r="M33" s="152"/>
-      <c r="N33" s="152"/>
-      <c r="O33" s="152"/>
-      <c r="P33" s="152"/>
-      <c r="Q33" s="152"/>
-      <c r="R33" s="152"/>
-      <c r="S33" s="152"/>
-      <c r="T33" s="152"/>
+      <c r="E33" s="153"/>
+      <c r="F33" s="153"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="153"/>
+      <c r="I33" s="153"/>
+      <c r="J33" s="153"/>
+      <c r="K33" s="153"/>
+      <c r="L33" s="153"/>
+      <c r="M33" s="153"/>
+      <c r="N33" s="153"/>
+      <c r="O33" s="153"/>
+      <c r="P33" s="153"/>
+      <c r="Q33" s="153"/>
+      <c r="R33" s="153"/>
+      <c r="S33" s="153"/>
+      <c r="T33" s="153"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4036,25 +4033,25 @@
       <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="146" t="s">
+      <c r="D35" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="146"/>
-      <c r="F35" s="146"/>
-      <c r="G35" s="146"/>
-      <c r="H35" s="146"/>
-      <c r="I35" s="146"/>
-      <c r="J35" s="146"/>
-      <c r="K35" s="146"/>
-      <c r="L35" s="146"/>
-      <c r="M35" s="146"/>
-      <c r="N35" s="146"/>
-      <c r="O35" s="146"/>
-      <c r="P35" s="146"/>
-      <c r="Q35" s="146"/>
-      <c r="R35" s="146"/>
-      <c r="S35" s="146"/>
-      <c r="T35" s="146"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
+      <c r="H35" s="147"/>
+      <c r="I35" s="147"/>
+      <c r="J35" s="147"/>
+      <c r="K35" s="147"/>
+      <c r="L35" s="147"/>
+      <c r="M35" s="147"/>
+      <c r="N35" s="147"/>
+      <c r="O35" s="147"/>
+      <c r="P35" s="147"/>
+      <c r="Q35" s="147"/>
+      <c r="R35" s="147"/>
+      <c r="S35" s="147"/>
+      <c r="T35" s="147"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4196,24 +4193,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="150" t="s">
+      <c r="G7" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="150"/>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
+      <c r="L7" s="152"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="150" t="s">
+      <c r="N7" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="150"/>
-      <c r="P7" s="150"/>
-      <c r="Q7" s="150"/>
-      <c r="R7" s="150"/>
-      <c r="S7" s="150"/>
-      <c r="T7" s="151"/>
+      <c r="O7" s="151"/>
+      <c r="P7" s="151"/>
+      <c r="Q7" s="151"/>
+      <c r="R7" s="151"/>
+      <c r="S7" s="151"/>
+      <c r="T7" s="152"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4455,24 +4452,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="147" t="s">
+      <c r="G13" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="148"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="149"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="150"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="147" t="s">
+      <c r="N13" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="148"/>
-      <c r="T13" s="149"/>
+      <c r="O13" s="149"/>
+      <c r="P13" s="149"/>
+      <c r="Q13" s="149"/>
+      <c r="R13" s="149"/>
+      <c r="S13" s="149"/>
+      <c r="T13" s="150"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
@@ -4710,24 +4707,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="147" t="s">
+      <c r="G19" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="148"/>
-      <c r="K19" s="148"/>
-      <c r="L19" s="149"/>
+      <c r="H19" s="149"/>
+      <c r="I19" s="149"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="150"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="147" t="s">
+      <c r="N19" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="148"/>
-      <c r="P19" s="148"/>
-      <c r="Q19" s="148"/>
-      <c r="R19" s="148"/>
-      <c r="S19" s="148"/>
-      <c r="T19" s="149"/>
+      <c r="O19" s="149"/>
+      <c r="P19" s="149"/>
+      <c r="Q19" s="149"/>
+      <c r="R19" s="149"/>
+      <c r="S19" s="149"/>
+      <c r="T19" s="150"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
@@ -4965,24 +4962,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="147" t="s">
+      <c r="G25" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="148"/>
-      <c r="I25" s="148"/>
-      <c r="J25" s="148"/>
-      <c r="K25" s="148"/>
-      <c r="L25" s="149"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="149"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="149"/>
+      <c r="L25" s="150"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="147" t="s">
+      <c r="N25" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="148"/>
-      <c r="P25" s="148"/>
-      <c r="Q25" s="148"/>
-      <c r="R25" s="148"/>
-      <c r="S25" s="148"/>
-      <c r="T25" s="149"/>
+      <c r="O25" s="149"/>
+      <c r="P25" s="149"/>
+      <c r="Q25" s="149"/>
+      <c r="R25" s="149"/>
+      <c r="S25" s="149"/>
+      <c r="T25" s="150"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
@@ -5220,26 +5217,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="143" t="s">
+      <c r="C31" s="144" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="143"/>
-      <c r="E31" s="143"/>
-      <c r="F31" s="143"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="143"/>
-      <c r="I31" s="143"/>
-      <c r="J31" s="143"/>
-      <c r="K31" s="143"/>
-      <c r="L31" s="143"/>
-      <c r="M31" s="143"/>
-      <c r="N31" s="143"/>
-      <c r="O31" s="143"/>
-      <c r="P31" s="143"/>
-      <c r="Q31" s="143"/>
-      <c r="R31" s="143"/>
-      <c r="S31" s="143"/>
-      <c r="T31" s="143"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="144"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="144"/>
+      <c r="J31" s="144"/>
+      <c r="K31" s="144"/>
+      <c r="L31" s="144"/>
+      <c r="M31" s="144"/>
+      <c r="N31" s="144"/>
+      <c r="O31" s="144"/>
+      <c r="P31" s="144"/>
+      <c r="Q31" s="144"/>
+      <c r="R31" s="144"/>
+      <c r="S31" s="144"/>
+      <c r="T31" s="144"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5266,26 +5263,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="143" t="s">
+      <c r="C33" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="143"/>
-      <c r="E33" s="143"/>
-      <c r="F33" s="143"/>
-      <c r="G33" s="143"/>
-      <c r="H33" s="143"/>
-      <c r="I33" s="143"/>
-      <c r="J33" s="143"/>
-      <c r="K33" s="143"/>
-      <c r="L33" s="143"/>
-      <c r="M33" s="143"/>
-      <c r="N33" s="143"/>
-      <c r="O33" s="143"/>
-      <c r="P33" s="143"/>
-      <c r="Q33" s="143"/>
-      <c r="R33" s="143"/>
-      <c r="S33" s="143"/>
-      <c r="T33" s="143"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="144"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
+      <c r="J33" s="144"/>
+      <c r="K33" s="144"/>
+      <c r="L33" s="144"/>
+      <c r="M33" s="144"/>
+      <c r="N33" s="144"/>
+      <c r="O33" s="144"/>
+      <c r="P33" s="144"/>
+      <c r="Q33" s="144"/>
+      <c r="R33" s="144"/>
+      <c r="S33" s="144"/>
+      <c r="T33" s="144"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5312,26 +5309,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="143" t="s">
+      <c r="C35" s="144" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="143"/>
-      <c r="E35" s="143"/>
-      <c r="F35" s="143"/>
-      <c r="G35" s="143"/>
-      <c r="H35" s="143"/>
-      <c r="I35" s="143"/>
-      <c r="J35" s="143"/>
-      <c r="K35" s="143"/>
-      <c r="L35" s="143"/>
-      <c r="M35" s="143"/>
-      <c r="N35" s="143"/>
-      <c r="O35" s="143"/>
-      <c r="P35" s="143"/>
-      <c r="Q35" s="143"/>
-      <c r="R35" s="143"/>
-      <c r="S35" s="143"/>
-      <c r="T35" s="143"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="144"/>
+      <c r="J35" s="144"/>
+      <c r="K35" s="144"/>
+      <c r="L35" s="144"/>
+      <c r="M35" s="144"/>
+      <c r="N35" s="144"/>
+      <c r="O35" s="144"/>
+      <c r="P35" s="144"/>
+      <c r="Q35" s="144"/>
+      <c r="R35" s="144"/>
+      <c r="S35" s="144"/>
+      <c r="T35" s="144"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5358,26 +5355,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="143" t="s">
+      <c r="C37" s="144" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="143"/>
-      <c r="E37" s="143"/>
-      <c r="F37" s="143"/>
-      <c r="G37" s="143"/>
-      <c r="H37" s="143"/>
-      <c r="I37" s="143"/>
-      <c r="J37" s="143"/>
-      <c r="K37" s="143"/>
-      <c r="L37" s="143"/>
-      <c r="M37" s="143"/>
-      <c r="N37" s="143"/>
-      <c r="O37" s="143"/>
-      <c r="P37" s="143"/>
-      <c r="Q37" s="143"/>
-      <c r="R37" s="143"/>
-      <c r="S37" s="143"/>
-      <c r="T37" s="143"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
+      <c r="I37" s="144"/>
+      <c r="J37" s="144"/>
+      <c r="K37" s="144"/>
+      <c r="L37" s="144"/>
+      <c r="M37" s="144"/>
+      <c r="N37" s="144"/>
+      <c r="O37" s="144"/>
+      <c r="P37" s="144"/>
+      <c r="Q37" s="144"/>
+      <c r="R37" s="144"/>
+      <c r="S37" s="144"/>
+      <c r="T37" s="144"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5404,26 +5401,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="143" t="s">
+      <c r="C39" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="143"/>
-      <c r="E39" s="143"/>
-      <c r="F39" s="143"/>
-      <c r="G39" s="143"/>
-      <c r="H39" s="143"/>
-      <c r="I39" s="143"/>
-      <c r="J39" s="143"/>
-      <c r="K39" s="143"/>
-      <c r="L39" s="143"/>
-      <c r="M39" s="143"/>
-      <c r="N39" s="143"/>
-      <c r="O39" s="143"/>
-      <c r="P39" s="143"/>
-      <c r="Q39" s="143"/>
-      <c r="R39" s="143"/>
-      <c r="S39" s="143"/>
-      <c r="T39" s="143"/>
+      <c r="D39" s="144"/>
+      <c r="E39" s="144"/>
+      <c r="F39" s="144"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="144"/>
+      <c r="I39" s="144"/>
+      <c r="J39" s="144"/>
+      <c r="K39" s="144"/>
+      <c r="L39" s="144"/>
+      <c r="M39" s="144"/>
+      <c r="N39" s="144"/>
+      <c r="O39" s="144"/>
+      <c r="P39" s="144"/>
+      <c r="Q39" s="144"/>
+      <c r="R39" s="144"/>
+      <c r="S39" s="144"/>
+      <c r="T39" s="144"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5450,34 +5447,29 @@
       <c r="B41" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="145" t="s">
+      <c r="C41" s="146" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="145"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="145"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="145"/>
-      <c r="I41" s="145"/>
-      <c r="J41" s="145"/>
-      <c r="K41" s="145"/>
-      <c r="L41" s="145"/>
-      <c r="M41" s="145"/>
-      <c r="N41" s="145"/>
-      <c r="O41" s="145"/>
-      <c r="P41" s="145"/>
-      <c r="Q41" s="145"/>
-      <c r="R41" s="145"/>
-      <c r="S41" s="145"/>
-      <c r="T41" s="145"/>
+      <c r="D41" s="146"/>
+      <c r="E41" s="146"/>
+      <c r="F41" s="146"/>
+      <c r="G41" s="146"/>
+      <c r="H41" s="146"/>
+      <c r="I41" s="146"/>
+      <c r="J41" s="146"/>
+      <c r="K41" s="146"/>
+      <c r="L41" s="146"/>
+      <c r="M41" s="146"/>
+      <c r="N41" s="146"/>
+      <c r="O41" s="146"/>
+      <c r="P41" s="146"/>
+      <c r="Q41" s="146"/>
+      <c r="R41" s="146"/>
+      <c r="S41" s="146"/>
+      <c r="T41" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5487,6 +5479,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5525,94 +5522,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="115" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="153"/>
+      <c r="D4" s="154"/>
     </row>
     <row r="5" spans="3:4" s="115" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="154" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="153"/>
+      <c r="D5" s="154"/>
     </row>
     <row r="6" spans="3:4" s="115" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="154" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="153"/>
+      <c r="D6" s="154"/>
     </row>
     <row r="7" spans="3:4" s="115" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="153"/>
+      <c r="D7" s="154"/>
     </row>
     <row r="8" spans="3:4" s="115" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="153" t="s">
+      <c r="C8" s="154" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="153"/>
+      <c r="D8" s="154"/>
     </row>
     <row r="9" spans="3:4" s="115" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="153"/>
+      <c r="D9" s="154"/>
     </row>
     <row r="10" spans="3:4" s="115" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="153" t="s">
+      <c r="C10" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="153"/>
+      <c r="D10" s="154"/>
     </row>
     <row r="11" spans="3:4" s="115" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="153" t="s">
+      <c r="C11" s="154" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="153"/>
+      <c r="D11" s="154"/>
     </row>
     <row r="12" spans="3:4" s="115" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="153" t="s">
+      <c r="C12" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="153"/>
+      <c r="D12" s="154"/>
     </row>
     <row r="13" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="153" t="s">
+      <c r="C13" s="154" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="153"/>
+      <c r="D13" s="154"/>
     </row>
     <row r="14" spans="3:4" s="115" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="153" t="s">
+      <c r="C14" s="154" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="153"/>
+      <c r="D14" s="154"/>
     </row>
     <row r="15" spans="3:4" s="115" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="153" t="s">
+      <c r="C15" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="153"/>
+      <c r="D15" s="154"/>
     </row>
     <row r="16" spans="3:4" s="115" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="153" t="s">
+      <c r="C16" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="153"/>
+      <c r="D16" s="154"/>
     </row>
     <row r="17" spans="3:4" s="115" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="153" t="s">
+      <c r="C17" s="154" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="153"/>
+      <c r="D17" s="154"/>
     </row>
     <row r="18" spans="3:4" s="115" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="153" t="s">
+      <c r="C18" s="154" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="153"/>
+      <c r="D18" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5646,7 +5643,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="P5" sqref="P5:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5717,17 +5714,17 @@
       </c>
     </row>
     <row r="5" spans="1:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="143"/>
-      <c r="D5" s="143"/>
-      <c r="E5" s="143"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="143"/>
-      <c r="H5" s="143"/>
-      <c r="I5" s="143"/>
-      <c r="J5" s="143"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="143"/>
-      <c r="M5" s="143"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="144"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="144"/>
+      <c r="L5" s="144"/>
+      <c r="M5" s="144"/>
       <c r="N5" s="75"/>
       <c r="O5" s="136"/>
       <c r="P5" s="136"/>
@@ -5756,21 +5753,21 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="147" t="s">
+      <c r="H7" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
-      <c r="K7" s="148"/>
-      <c r="L7" s="148"/>
-      <c r="M7" s="149"/>
-      <c r="N7" s="147"/>
-      <c r="O7" s="148"/>
-      <c r="P7" s="148"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="148"/>
-      <c r="S7" s="148"/>
-      <c r="T7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="149"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="148"/>
+      <c r="O7" s="149"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="149"/>
+      <c r="R7" s="149"/>
+      <c r="S7" s="149"/>
+      <c r="T7" s="150"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98" t="s">
@@ -5894,21 +5891,21 @@
       </c>
       <c r="D12" s="54"/>
       <c r="E12" s="116"/>
-      <c r="F12" s="154"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
-      <c r="L12" s="154"/>
-      <c r="M12" s="154"/>
-      <c r="N12" s="154"/>
-      <c r="O12" s="154"/>
-      <c r="P12" s="154"/>
-      <c r="Q12" s="154"/>
-      <c r="R12" s="154"/>
-      <c r="S12" s="154"/>
-      <c r="T12" s="154"/>
+      <c r="F12" s="155"/>
+      <c r="G12" s="155"/>
+      <c r="H12" s="155"/>
+      <c r="I12" s="155"/>
+      <c r="J12" s="155"/>
+      <c r="K12" s="155"/>
+      <c r="L12" s="155"/>
+      <c r="M12" s="155"/>
+      <c r="N12" s="155"/>
+      <c r="O12" s="155"/>
+      <c r="P12" s="155"/>
+      <c r="Q12" s="155"/>
+      <c r="R12" s="155"/>
+      <c r="S12" s="155"/>
+      <c r="T12" s="155"/>
     </row>
     <row r="13" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
@@ -5934,21 +5931,21 @@
         <v>36</v>
       </c>
       <c r="D14" s="54"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
-      <c r="L14" s="154"/>
-      <c r="M14" s="154"/>
-      <c r="N14" s="154"/>
-      <c r="O14" s="154"/>
-      <c r="P14" s="154"/>
-      <c r="Q14" s="154"/>
-      <c r="R14" s="154"/>
-      <c r="S14" s="154"/>
-      <c r="T14" s="154"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="155"/>
+      <c r="H14" s="155"/>
+      <c r="I14" s="155"/>
+      <c r="J14" s="155"/>
+      <c r="K14" s="155"/>
+      <c r="L14" s="155"/>
+      <c r="M14" s="155"/>
+      <c r="N14" s="155"/>
+      <c r="O14" s="155"/>
+      <c r="P14" s="155"/>
+      <c r="Q14" s="155"/>
+      <c r="R14" s="155"/>
+      <c r="S14" s="155"/>
+      <c r="T14" s="155"/>
     </row>
     <row r="15" spans="1:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -5975,21 +5972,21 @@
       </c>
       <c r="D16" s="54"/>
       <c r="E16" s="116"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
-      <c r="M16" s="154"/>
-      <c r="N16" s="154"/>
-      <c r="O16" s="154"/>
-      <c r="P16" s="154"/>
-      <c r="Q16" s="154"/>
-      <c r="R16" s="154"/>
-      <c r="S16" s="154"/>
-      <c r="T16" s="154"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
+      <c r="M16" s="155"/>
+      <c r="N16" s="155"/>
+      <c r="O16" s="155"/>
+      <c r="P16" s="155"/>
+      <c r="Q16" s="155"/>
+      <c r="R16" s="155"/>
+      <c r="S16" s="155"/>
+      <c r="T16" s="155"/>
     </row>
     <row r="17" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -6015,21 +6012,21 @@
         <v>48</v>
       </c>
       <c r="D18" s="54"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
-      <c r="J18" s="154"/>
-      <c r="K18" s="154"/>
-      <c r="L18" s="154"/>
-      <c r="M18" s="154"/>
-      <c r="N18" s="154"/>
-      <c r="O18" s="154"/>
-      <c r="P18" s="154"/>
-      <c r="Q18" s="154"/>
-      <c r="R18" s="154"/>
-      <c r="S18" s="154"/>
-      <c r="T18" s="154"/>
+      <c r="F18" s="155"/>
+      <c r="G18" s="155"/>
+      <c r="H18" s="155"/>
+      <c r="I18" s="155"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="155"/>
+      <c r="N18" s="155"/>
+      <c r="O18" s="155"/>
+      <c r="P18" s="155"/>
+      <c r="Q18" s="155"/>
+      <c r="R18" s="155"/>
+      <c r="S18" s="155"/>
+      <c r="T18" s="155"/>
     </row>
     <row r="19" spans="3:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
@@ -6055,24 +6052,29 @@
         <v>49</v>
       </c>
       <c r="D20" s="54"/>
-      <c r="F20" s="145"/>
-      <c r="G20" s="145"/>
-      <c r="H20" s="145"/>
-      <c r="I20" s="145"/>
-      <c r="J20" s="145"/>
-      <c r="K20" s="145"/>
-      <c r="L20" s="145"/>
-      <c r="M20" s="145"/>
-      <c r="N20" s="145"/>
-      <c r="O20" s="145"/>
-      <c r="P20" s="145"/>
-      <c r="Q20" s="145"/>
-      <c r="R20" s="145"/>
-      <c r="S20" s="145"/>
-      <c r="T20" s="145"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="146"/>
+      <c r="J20" s="146"/>
+      <c r="K20" s="146"/>
+      <c r="L20" s="146"/>
+      <c r="M20" s="146"/>
+      <c r="N20" s="146"/>
+      <c r="O20" s="146"/>
+      <c r="P20" s="146"/>
+      <c r="Q20" s="146"/>
+      <c r="R20" s="146"/>
+      <c r="S20" s="146"/>
+      <c r="T20" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F14:T14"/>
     <mergeCell ref="F16:T16"/>
     <mergeCell ref="F18:T18"/>
     <mergeCell ref="F20:T20"/>
@@ -6080,11 +6082,6 @@
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="N7:T7"/>
     <mergeCell ref="F12:T12"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F14:T14"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:T3 C5 C4:N4 T5 C6:T1048576 P4:Q4 S4">
     <cfRule type="expression" dxfId="0" priority="15">
@@ -6128,18 +6125,18 @@
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="135"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
-      <c r="N2" s="149"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="150"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6279,35 +6276,35 @@
       <c r="B10" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="161"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="162"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="155"/>
-      <c r="H10" s="156"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="157"/>
-      <c r="K10" s="155"/>
-      <c r="L10" s="156"/>
-      <c r="M10" s="156"/>
-      <c r="N10" s="157"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="164"/>
+      <c r="G10" s="156"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="158"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="157"/>
+      <c r="M10" s="157"/>
+      <c r="N10" s="158"/>
       <c r="O10" s="141"/>
     </row>
     <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="135"/>
-      <c r="C12" s="147"/>
-      <c r="D12" s="148"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="149"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="149"/>
-      <c r="L12" s="147"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="149"/>
+      <c r="C12" s="148"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="149"/>
+      <c r="F12" s="149"/>
+      <c r="G12" s="150"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="150"/>
+      <c r="L12" s="148"/>
+      <c r="M12" s="149"/>
+      <c r="N12" s="149"/>
+      <c r="O12" s="150"/>
       <c r="P12" s="29"/>
     </row>
     <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6449,36 +6446,36 @@
       <c r="B20" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="158"/>
-      <c r="D20" s="159"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="159"/>
-      <c r="G20" s="160"/>
-      <c r="H20" s="155"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="156"/>
-      <c r="K20" s="157"/>
-      <c r="L20" s="155"/>
-      <c r="M20" s="156"/>
-      <c r="N20" s="156"/>
-      <c r="O20" s="157"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="161"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="157"/>
+      <c r="J20" s="157"/>
+      <c r="K20" s="158"/>
+      <c r="L20" s="156"/>
+      <c r="M20" s="157"/>
+      <c r="N20" s="157"/>
+      <c r="O20" s="158"/>
       <c r="P20" s="137"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="135"/>
-      <c r="C22" s="147"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="148"/>
-      <c r="F22" s="149"/>
-      <c r="G22" s="148"/>
-      <c r="H22" s="148"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="148"/>
-      <c r="K22" s="149"/>
-      <c r="L22" s="147"/>
-      <c r="M22" s="148"/>
-      <c r="N22" s="148"/>
-      <c r="O22" s="149"/>
+      <c r="C22" s="148"/>
+      <c r="D22" s="149"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="149"/>
+      <c r="H22" s="149"/>
+      <c r="I22" s="149"/>
+      <c r="J22" s="149"/>
+      <c r="K22" s="150"/>
+      <c r="L22" s="148"/>
+      <c r="M22" s="149"/>
+      <c r="N22" s="149"/>
+      <c r="O22" s="150"/>
       <c r="P22" s="29"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6620,36 +6617,36 @@
       <c r="B30" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="155"/>
-      <c r="D30" s="156"/>
-      <c r="E30" s="156"/>
-      <c r="F30" s="157"/>
-      <c r="G30" s="155"/>
-      <c r="H30" s="156"/>
-      <c r="I30" s="156"/>
-      <c r="J30" s="156"/>
-      <c r="K30" s="157"/>
-      <c r="L30" s="155"/>
-      <c r="M30" s="156"/>
-      <c r="N30" s="156"/>
-      <c r="O30" s="157"/>
+      <c r="C30" s="156"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="158"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="157"/>
+      <c r="I30" s="157"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="158"/>
+      <c r="L30" s="156"/>
+      <c r="M30" s="157"/>
+      <c r="N30" s="157"/>
+      <c r="O30" s="158"/>
       <c r="P30" s="137"/>
     </row>
     <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="135"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="148"/>
-      <c r="E32" s="148"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="148"/>
-      <c r="H32" s="148"/>
-      <c r="I32" s="148"/>
-      <c r="J32" s="149"/>
-      <c r="K32" s="147"/>
-      <c r="L32" s="148"/>
-      <c r="M32" s="148"/>
-      <c r="N32" s="148"/>
-      <c r="O32" s="149"/>
+      <c r="C32" s="148"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="149"/>
+      <c r="I32" s="149"/>
+      <c r="J32" s="150"/>
+      <c r="K32" s="148"/>
+      <c r="L32" s="149"/>
+      <c r="M32" s="149"/>
+      <c r="N32" s="149"/>
+      <c r="O32" s="150"/>
       <c r="P32" s="29"/>
     </row>
     <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6791,37 +6788,37 @@
       <c r="B40" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="155"/>
-      <c r="D40" s="156"/>
-      <c r="E40" s="156"/>
-      <c r="F40" s="157"/>
-      <c r="G40" s="155"/>
-      <c r="H40" s="156"/>
-      <c r="I40" s="156"/>
-      <c r="J40" s="157"/>
-      <c r="K40" s="155"/>
-      <c r="L40" s="156"/>
-      <c r="M40" s="156"/>
-      <c r="N40" s="156"/>
-      <c r="O40" s="157"/>
+      <c r="C40" s="156"/>
+      <c r="D40" s="157"/>
+      <c r="E40" s="157"/>
+      <c r="F40" s="158"/>
+      <c r="G40" s="156"/>
+      <c r="H40" s="157"/>
+      <c r="I40" s="157"/>
+      <c r="J40" s="158"/>
+      <c r="K40" s="156"/>
+      <c r="L40" s="157"/>
+      <c r="M40" s="157"/>
+      <c r="N40" s="157"/>
+      <c r="O40" s="158"/>
       <c r="P40" s="137"/>
     </row>
     <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="135"/>
-      <c r="C42" s="147"/>
-      <c r="D42" s="148"/>
-      <c r="E42" s="148"/>
-      <c r="F42" s="148"/>
-      <c r="G42" s="149"/>
-      <c r="H42" s="148"/>
-      <c r="I42" s="148"/>
-      <c r="J42" s="148"/>
-      <c r="K42" s="148"/>
-      <c r="L42" s="149"/>
-      <c r="M42" s="147"/>
-      <c r="N42" s="148"/>
-      <c r="O42" s="148"/>
-      <c r="P42" s="149"/>
+      <c r="C42" s="148"/>
+      <c r="D42" s="149"/>
+      <c r="E42" s="149"/>
+      <c r="F42" s="149"/>
+      <c r="G42" s="150"/>
+      <c r="H42" s="149"/>
+      <c r="I42" s="149"/>
+      <c r="J42" s="149"/>
+      <c r="K42" s="149"/>
+      <c r="L42" s="150"/>
+      <c r="M42" s="148"/>
+      <c r="N42" s="149"/>
+      <c r="O42" s="149"/>
+      <c r="P42" s="150"/>
       <c r="Q42" s="29"/>
     </row>
     <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6970,38 +6967,38 @@
       <c r="B50" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="155"/>
-      <c r="D50" s="156"/>
-      <c r="E50" s="156"/>
-      <c r="F50" s="156"/>
-      <c r="G50" s="157"/>
-      <c r="H50" s="155"/>
-      <c r="I50" s="156"/>
-      <c r="J50" s="156"/>
-      <c r="K50" s="156"/>
-      <c r="L50" s="157"/>
-      <c r="M50" s="155"/>
-      <c r="N50" s="156"/>
-      <c r="O50" s="156"/>
-      <c r="P50" s="157"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="157"/>
+      <c r="E50" s="157"/>
+      <c r="F50" s="157"/>
+      <c r="G50" s="158"/>
+      <c r="H50" s="156"/>
+      <c r="I50" s="157"/>
+      <c r="J50" s="157"/>
+      <c r="K50" s="157"/>
+      <c r="L50" s="158"/>
+      <c r="M50" s="156"/>
+      <c r="N50" s="157"/>
+      <c r="O50" s="157"/>
+      <c r="P50" s="158"/>
       <c r="Q50" s="137"/>
     </row>
     <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="135"/>
-      <c r="C52" s="147"/>
-      <c r="D52" s="148"/>
-      <c r="E52" s="148"/>
-      <c r="F52" s="148"/>
-      <c r="G52" s="149"/>
-      <c r="H52" s="148"/>
-      <c r="I52" s="148"/>
-      <c r="J52" s="148"/>
-      <c r="K52" s="149"/>
-      <c r="L52" s="147"/>
-      <c r="M52" s="148"/>
-      <c r="N52" s="148"/>
-      <c r="O52" s="148"/>
-      <c r="P52" s="149"/>
+      <c r="C52" s="148"/>
+      <c r="D52" s="149"/>
+      <c r="E52" s="149"/>
+      <c r="F52" s="149"/>
+      <c r="G52" s="150"/>
+      <c r="H52" s="149"/>
+      <c r="I52" s="149"/>
+      <c r="J52" s="149"/>
+      <c r="K52" s="150"/>
+      <c r="L52" s="148"/>
+      <c r="M52" s="149"/>
+      <c r="N52" s="149"/>
+      <c r="O52" s="149"/>
+      <c r="P52" s="150"/>
       <c r="Q52" s="29"/>
     </row>
     <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7150,38 +7147,38 @@
       <c r="B60" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="155"/>
-      <c r="D60" s="156"/>
-      <c r="E60" s="156"/>
-      <c r="F60" s="156"/>
-      <c r="G60" s="157"/>
-      <c r="H60" s="155"/>
-      <c r="I60" s="156"/>
-      <c r="J60" s="156"/>
-      <c r="K60" s="157"/>
-      <c r="L60" s="155"/>
-      <c r="M60" s="156"/>
-      <c r="N60" s="156"/>
-      <c r="O60" s="156"/>
-      <c r="P60" s="157"/>
+      <c r="C60" s="156"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="157"/>
+      <c r="F60" s="157"/>
+      <c r="G60" s="158"/>
+      <c r="H60" s="156"/>
+      <c r="I60" s="157"/>
+      <c r="J60" s="157"/>
+      <c r="K60" s="158"/>
+      <c r="L60" s="156"/>
+      <c r="M60" s="157"/>
+      <c r="N60" s="157"/>
+      <c r="O60" s="157"/>
+      <c r="P60" s="158"/>
       <c r="Q60" s="137"/>
     </row>
     <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="135"/>
-      <c r="C62" s="147"/>
-      <c r="D62" s="148"/>
-      <c r="E62" s="148"/>
-      <c r="F62" s="149"/>
-      <c r="G62" s="148"/>
-      <c r="H62" s="148"/>
-      <c r="I62" s="148"/>
-      <c r="J62" s="148"/>
-      <c r="K62" s="149"/>
-      <c r="L62" s="147"/>
-      <c r="M62" s="148"/>
-      <c r="N62" s="148"/>
-      <c r="O62" s="148"/>
-      <c r="P62" s="149"/>
+      <c r="C62" s="148"/>
+      <c r="D62" s="149"/>
+      <c r="E62" s="149"/>
+      <c r="F62" s="150"/>
+      <c r="G62" s="149"/>
+      <c r="H62" s="149"/>
+      <c r="I62" s="149"/>
+      <c r="J62" s="149"/>
+      <c r="K62" s="150"/>
+      <c r="L62" s="148"/>
+      <c r="M62" s="149"/>
+      <c r="N62" s="149"/>
+      <c r="O62" s="149"/>
+      <c r="P62" s="150"/>
       <c r="Q62" s="29"/>
     </row>
     <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7330,50 +7327,24 @@
       <c r="B70" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="155"/>
-      <c r="D70" s="156"/>
-      <c r="E70" s="156"/>
-      <c r="F70" s="157"/>
-      <c r="G70" s="155"/>
-      <c r="H70" s="156"/>
-      <c r="I70" s="156"/>
-      <c r="J70" s="156"/>
-      <c r="K70" s="157"/>
-      <c r="L70" s="155"/>
-      <c r="M70" s="156"/>
-      <c r="N70" s="156"/>
-      <c r="O70" s="156"/>
-      <c r="P70" s="157"/>
+      <c r="C70" s="156"/>
+      <c r="D70" s="157"/>
+      <c r="E70" s="157"/>
+      <c r="F70" s="158"/>
+      <c r="G70" s="156"/>
+      <c r="H70" s="157"/>
+      <c r="I70" s="157"/>
+      <c r="J70" s="157"/>
+      <c r="K70" s="158"/>
+      <c r="L70" s="156"/>
+      <c r="M70" s="157"/>
+      <c r="N70" s="157"/>
+      <c r="O70" s="157"/>
+      <c r="P70" s="158"/>
       <c r="Q70" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C70:F70"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="L70:P70"/>
-    <mergeCell ref="L60:P60"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="K40:O40"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="H50:L50"/>
-    <mergeCell ref="M50:P50"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="H52:K52"/>
     <mergeCell ref="L52:P52"/>
@@ -7390,6 +7361,32 @@
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="G22:K22"/>
     <mergeCell ref="L22:O22"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:O40"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="L70:P70"/>
+    <mergeCell ref="L60:P60"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 L30 L70 K10 K40 M50 C20 H20 C10 G10 C30 G30 C40 G40 C50 H50 C60 C70 H60 G70 L60" xr:uid="{1A174315-2F56-4C74-8CF2-D4F4F4F25C91}"/>

</xml_diff>